<commit_message>
updated AXA new benefits
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chila\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF214120-F581-4B6A-ACAF-078463337FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B11C663-3A23-49B3-BF5F-E046F7D284D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41970" yWindow="-16215" windowWidth="29040" windowHeight="15720" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="352">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1077,6 +1077,21 @@
   </si>
   <si>
     <t>INTENSIVE CARE CHARGES</t>
+  </si>
+  <si>
+    <t>E/VAC</t>
+  </si>
+  <si>
+    <t>Combined Wellness Benefit - Vac&amp;Opt</t>
+  </si>
+  <si>
+    <t>PVIN</t>
+  </si>
+  <si>
+    <t>BON1</t>
+  </si>
+  <si>
+    <t>SPVIN</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:O115"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H88" sqref="H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -1675,6 +1690,9 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F5" t="s">
+        <v>349</v>
+      </c>
       <c r="H5" t="s">
         <v>203</v>
       </c>
@@ -2479,6 +2497,12 @@
       <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F35" t="s">
+        <v>351</v>
+      </c>
+      <c r="G35" t="s">
+        <v>174</v>
+      </c>
       <c r="H35" t="s">
         <v>203</v>
       </c>
@@ -3340,29 +3364,15 @@
       </c>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A69" s="3"/>
       <c r="B69" s="3" t="s">
         <v>29</v>
       </c>
       <c r="F69" t="s">
-        <v>191</v>
+        <v>350</v>
       </c>
       <c r="G69" t="s">
         <v>149</v>
-      </c>
-      <c r="H69" t="s">
-        <v>204</v>
-      </c>
-      <c r="I69" t="s">
-        <v>274</v>
-      </c>
-      <c r="J69" t="s">
-        <v>207</v>
-      </c>
-      <c r="K69" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -3373,7 +3383,7 @@
         <v>29</v>
       </c>
       <c r="F70" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="G70" t="s">
         <v>149</v>
@@ -3382,7 +3392,7 @@
         <v>204</v>
       </c>
       <c r="I70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J70" t="s">
         <v>207</v>
@@ -3396,19 +3406,10 @@
         <v>24</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D71" t="s">
-        <v>75</v>
-      </c>
-      <c r="E71" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F71" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G71" t="s">
         <v>149</v>
@@ -3417,7 +3418,7 @@
         <v>204</v>
       </c>
       <c r="I71" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J71" t="s">
         <v>207</v>
@@ -3431,22 +3432,28 @@
         <v>24</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D72" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E72" t="s">
         <v>50</v>
       </c>
+      <c r="F72" t="s">
+        <v>199</v>
+      </c>
+      <c r="G72" t="s">
+        <v>149</v>
+      </c>
       <c r="H72" t="s">
         <v>204</v>
       </c>
       <c r="I72" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J72" t="s">
         <v>207</v>
@@ -3460,7 +3467,28 @@
         <v>24</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D73" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" t="s">
+        <v>50</v>
+      </c>
+      <c r="H73" t="s">
+        <v>204</v>
+      </c>
+      <c r="I73" t="s">
+        <v>277</v>
+      </c>
+      <c r="J73" t="s">
+        <v>207</v>
+      </c>
+      <c r="K73" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -3468,37 +3496,7 @@
         <v>24</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D74" t="s">
-        <v>72</v>
-      </c>
-      <c r="E74" t="s">
-        <v>50</v>
-      </c>
-      <c r="F74" t="s">
-        <v>155</v>
-      </c>
-      <c r="G74" t="s">
-        <v>149</v>
-      </c>
-      <c r="H74" t="s">
-        <v>204</v>
-      </c>
-      <c r="I74" t="s">
-        <v>278</v>
-      </c>
-      <c r="J74" t="s">
-        <v>207</v>
-      </c>
-      <c r="K74" t="s">
-        <v>221</v>
-      </c>
-      <c r="L74" t="s">
-        <v>318</v>
+        <v>32</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -3508,8 +3506,17 @@
       <c r="B75" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C75" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D75" t="s">
+        <v>72</v>
+      </c>
+      <c r="E75" t="s">
+        <v>50</v>
+      </c>
       <c r="F75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G75" t="s">
         <v>149</v>
@@ -3518,13 +3525,16 @@
         <v>204</v>
       </c>
       <c r="I75" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J75" t="s">
         <v>207</v>
       </c>
       <c r="K75" t="s">
         <v>221</v>
+      </c>
+      <c r="L75" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -3532,19 +3542,10 @@
         <v>24</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D76" t="s">
-        <v>71</v>
-      </c>
-      <c r="E76" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F76" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G76" t="s">
         <v>149</v>
@@ -3553,16 +3554,13 @@
         <v>204</v>
       </c>
       <c r="I76" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J76" t="s">
         <v>207</v>
       </c>
       <c r="K76" t="s">
         <v>221</v>
-      </c>
-      <c r="L76" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -3572,29 +3570,35 @@
       <c r="B77" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C77" s="6">
-        <v>253</v>
+      <c r="C77" s="6" t="s">
+        <v>120</v>
       </c>
       <c r="D77" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="E77" t="s">
         <v>50</v>
       </c>
       <c r="F77" t="s">
-        <v>223</v>
+        <v>154</v>
+      </c>
+      <c r="G77" t="s">
+        <v>149</v>
       </c>
       <c r="H77" t="s">
         <v>204</v>
       </c>
       <c r="I77" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J77" t="s">
         <v>207</v>
       </c>
       <c r="K77" t="s">
         <v>221</v>
+      </c>
+      <c r="L77" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -3604,8 +3608,17 @@
       <c r="B78" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C78" s="6">
+        <v>253</v>
+      </c>
+      <c r="D78" t="s">
+        <v>91</v>
+      </c>
+      <c r="E78" t="s">
+        <v>50</v>
+      </c>
       <c r="F78" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="G78" t="s">
         <v>149</v>
@@ -3614,7 +3627,7 @@
         <v>204</v>
       </c>
       <c r="I78" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J78" t="s">
         <v>207</v>
@@ -3628,28 +3641,25 @@
         <v>24</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D79" t="s">
-        <v>35</v>
-      </c>
-      <c r="E79" t="s">
-        <v>50</v>
+        <v>34</v>
+      </c>
+      <c r="F79" t="s">
+        <v>198</v>
+      </c>
+      <c r="G79" t="s">
+        <v>149</v>
       </c>
       <c r="H79" t="s">
         <v>204</v>
       </c>
       <c r="I79" t="s">
-        <v>35</v>
+        <v>282</v>
       </c>
       <c r="J79" t="s">
         <v>207</v>
       </c>
       <c r="K79" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -3657,28 +3667,22 @@
         <v>24</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D80" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="E80" t="s">
         <v>50</v>
       </c>
-      <c r="F80" t="s">
-        <v>197</v>
-      </c>
-      <c r="G80" t="s">
-        <v>149</v>
-      </c>
       <c r="H80" t="s">
         <v>204</v>
       </c>
       <c r="I80" t="s">
-        <v>283</v>
+        <v>35</v>
       </c>
       <c r="J80" t="s">
         <v>207</v>
@@ -3694,8 +3698,17 @@
       <c r="B81" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="C81" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D81" t="s">
+        <v>90</v>
+      </c>
+      <c r="E81" t="s">
+        <v>50</v>
+      </c>
       <c r="F81" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="G81" t="s">
         <v>149</v>
@@ -3704,13 +3717,13 @@
         <v>204</v>
       </c>
       <c r="I81" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J81" t="s">
         <v>207</v>
       </c>
       <c r="K81" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -3721,13 +3734,22 @@
         <v>36</v>
       </c>
       <c r="F82" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G82" t="s">
         <v>149</v>
       </c>
       <c r="H82" t="s">
         <v>204</v>
+      </c>
+      <c r="I82" t="s">
+        <v>284</v>
+      </c>
+      <c r="J82" t="s">
+        <v>207</v>
+      </c>
+      <c r="K82" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -3735,28 +3757,16 @@
         <v>24</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C83" s="6">
-        <v>311</v>
-      </c>
-      <c r="D83" t="s">
-        <v>76</v>
-      </c>
-      <c r="E83" t="s">
-        <v>52</v>
-      </c>
-      <c r="I83" t="s">
-        <v>285</v>
-      </c>
-      <c r="J83" t="s">
-        <v>207</v>
-      </c>
-      <c r="K83" t="s">
-        <v>221</v>
-      </c>
-      <c r="L83" t="s">
-        <v>333</v>
+        <v>36</v>
+      </c>
+      <c r="F83" t="s">
+        <v>193</v>
+      </c>
+      <c r="G83" t="s">
+        <v>149</v>
+      </c>
+      <c r="H83" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -3767,13 +3777,22 @@
         <v>37</v>
       </c>
       <c r="C84" s="6">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D84" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="E84" t="s">
         <v>52</v>
+      </c>
+      <c r="I84" t="s">
+        <v>285</v>
+      </c>
+      <c r="J84" t="s">
+        <v>207</v>
+      </c>
+      <c r="K84" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -3781,16 +3800,16 @@
         <v>24</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>308</v>
+        <v>37</v>
+      </c>
+      <c r="C85" s="6">
+        <v>312</v>
       </c>
       <c r="D85" t="s">
-        <v>307</v>
+        <v>136</v>
       </c>
       <c r="E85" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -3798,89 +3817,60 @@
         <v>24</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D86" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E86" t="s">
         <v>50</v>
       </c>
-      <c r="F86" t="s">
+    </row>
+    <row r="87" spans="1:12">
+      <c r="A87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D87" t="s">
+        <v>309</v>
+      </c>
+      <c r="E87" t="s">
+        <v>50</v>
+      </c>
+      <c r="F87" t="s">
         <v>189</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G87" t="s">
         <v>149</v>
       </c>
-      <c r="H86" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C87" s="6">
-        <v>511</v>
-      </c>
-      <c r="D87" t="s">
-        <v>82</v>
-      </c>
-      <c r="E87" t="s">
-        <v>51</v>
-      </c>
-      <c r="F87" t="s">
-        <v>182</v>
-      </c>
-      <c r="G87" t="s">
-        <v>187</v>
-      </c>
       <c r="H87" t="s">
         <v>204</v>
       </c>
-      <c r="I87" t="s">
-        <v>286</v>
-      </c>
-      <c r="J87" t="s">
-        <v>209</v>
-      </c>
-      <c r="K87" t="s">
-        <v>220</v>
-      </c>
-      <c r="L87" t="s">
-        <v>316</v>
-      </c>
     </row>
     <row r="88" spans="1:12">
-      <c r="A88" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>39</v>
+      <c r="A88" s="3"/>
+      <c r="B88" s="3" t="s">
+        <v>348</v>
       </c>
       <c r="F88" t="s">
-        <v>180</v>
+        <v>347</v>
       </c>
       <c r="G88" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="H88" t="s">
         <v>204</v>
       </c>
-      <c r="I88" t="s">
-        <v>287</v>
-      </c>
-      <c r="J88" t="s">
-        <v>209</v>
-      </c>
-      <c r="K88" t="s">
-        <v>220</v>
+      <c r="L88" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -3891,16 +3881,16 @@
         <v>39</v>
       </c>
       <c r="C89" s="6">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E89" t="s">
         <v>51</v>
       </c>
       <c r="F89" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="G89" t="s">
         <v>187</v>
@@ -3909,13 +3899,16 @@
         <v>204</v>
       </c>
       <c r="I89" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J89" t="s">
         <v>209</v>
       </c>
       <c r="K89" t="s">
         <v>220</v>
+      </c>
+      <c r="L89" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -3926,7 +3919,7 @@
         <v>39</v>
       </c>
       <c r="F90" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G90" t="s">
         <v>187</v>
@@ -3935,7 +3928,7 @@
         <v>204</v>
       </c>
       <c r="I90" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="J90" t="s">
         <v>209</v>
@@ -3951,8 +3944,17 @@
       <c r="B91" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C91" s="6">
+        <v>513</v>
+      </c>
+      <c r="D91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E91" t="s">
+        <v>51</v>
+      </c>
       <c r="F91" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="G91" t="s">
         <v>187</v>
@@ -3961,13 +3963,13 @@
         <v>204</v>
       </c>
       <c r="I91" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J91" t="s">
         <v>209</v>
       </c>
       <c r="K91" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -3978,13 +3980,16 @@
         <v>39</v>
       </c>
       <c r="F92" t="s">
-        <v>183</v>
+        <v>177</v>
+      </c>
+      <c r="G92" t="s">
+        <v>187</v>
       </c>
       <c r="H92" t="s">
         <v>204</v>
       </c>
       <c r="I92" t="s">
-        <v>39</v>
+        <v>289</v>
       </c>
       <c r="J92" t="s">
         <v>209</v>
@@ -3993,38 +3998,47 @@
         <v>220</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="17" customHeight="1">
+    <row r="93" spans="1:12">
       <c r="A93" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B93" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F93" t="s">
+        <v>38</v>
+      </c>
+      <c r="G93" t="s">
+        <v>187</v>
+      </c>
       <c r="H93" t="s">
         <v>204</v>
       </c>
       <c r="I93" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J93" t="s">
         <v>209</v>
       </c>
       <c r="K93" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" ht="17" customHeight="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
       <c r="A94" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F94" t="s">
+        <v>183</v>
+      </c>
       <c r="H94" t="s">
         <v>204</v>
       </c>
       <c r="I94" t="s">
-        <v>292</v>
+        <v>39</v>
       </c>
       <c r="J94" t="s">
         <v>209</v>
@@ -4044,7 +4058,7 @@
         <v>204</v>
       </c>
       <c r="I95" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="J95" t="s">
         <v>209</v>
@@ -4064,7 +4078,7 @@
         <v>204</v>
       </c>
       <c r="I96" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J96" t="s">
         <v>209</v>
@@ -4080,17 +4094,11 @@
       <c r="B97" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F97" t="s">
-        <v>181</v>
-      </c>
-      <c r="G97" t="s">
-        <v>187</v>
-      </c>
       <c r="H97" t="s">
         <v>204</v>
       </c>
       <c r="I97" t="s">
-        <v>215</v>
+        <v>293</v>
       </c>
       <c r="J97" t="s">
         <v>209</v>
@@ -4106,17 +4114,11 @@
       <c r="B98" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F98" t="s">
-        <v>185</v>
-      </c>
-      <c r="G98" t="s">
-        <v>187</v>
-      </c>
       <c r="H98" t="s">
         <v>204</v>
       </c>
       <c r="I98" t="s">
-        <v>215</v>
+        <v>294</v>
       </c>
       <c r="J98" t="s">
         <v>209</v>
@@ -4132,11 +4134,17 @@
       <c r="B99" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F99" t="s">
+        <v>181</v>
+      </c>
+      <c r="G99" t="s">
+        <v>187</v>
+      </c>
       <c r="H99" t="s">
         <v>204</v>
       </c>
       <c r="I99" t="s">
-        <v>295</v>
+        <v>215</v>
       </c>
       <c r="J99" t="s">
         <v>209</v>
@@ -4145,15 +4153,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" ht="17" customHeight="1">
       <c r="A100" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F100" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="G100" t="s">
         <v>187</v>
@@ -4162,7 +4170,7 @@
         <v>204</v>
       </c>
       <c r="I100" t="s">
-        <v>296</v>
+        <v>215</v>
       </c>
       <c r="J100" t="s">
         <v>209</v>
@@ -4171,18 +4179,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" ht="17" customHeight="1">
       <c r="A101" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H101" t="s">
         <v>204</v>
       </c>
       <c r="I101" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J101" t="s">
         <v>209</v>
@@ -4198,11 +4206,17 @@
       <c r="B102" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="F102" t="s">
+        <v>176</v>
+      </c>
+      <c r="G102" t="s">
+        <v>187</v>
+      </c>
       <c r="H102" t="s">
         <v>204</v>
       </c>
       <c r="I102" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J102" t="s">
         <v>209</v>
@@ -4216,19 +4230,13 @@
         <v>38</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F103" t="s">
-        <v>179</v>
-      </c>
-      <c r="G103" t="s">
-        <v>187</v>
+        <v>40</v>
       </c>
       <c r="H103" t="s">
         <v>204</v>
       </c>
       <c r="I103" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J103" t="s">
         <v>209</v>
@@ -4242,13 +4250,13 @@
         <v>38</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H104" t="s">
         <v>204</v>
       </c>
       <c r="I104" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J104" t="s">
         <v>209</v>
@@ -4262,10 +4270,10 @@
         <v>38</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F105" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="G105" t="s">
         <v>187</v>
@@ -4274,7 +4282,7 @@
         <v>204</v>
       </c>
       <c r="I105" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J105" t="s">
         <v>209</v>
@@ -4288,13 +4296,13 @@
         <v>38</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H106" t="s">
         <v>204</v>
       </c>
       <c r="I106" t="s">
-        <v>42</v>
+        <v>300</v>
       </c>
       <c r="J106" t="s">
         <v>209</v>
@@ -4310,11 +4318,17 @@
       <c r="B107" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="F107" t="s">
+        <v>175</v>
+      </c>
+      <c r="G107" t="s">
+        <v>187</v>
+      </c>
       <c r="H107" t="s">
         <v>204</v>
       </c>
       <c r="I107" t="s">
-        <v>214</v>
+        <v>301</v>
       </c>
       <c r="J107" t="s">
         <v>209</v>
@@ -4334,7 +4348,7 @@
         <v>204</v>
       </c>
       <c r="I108" t="s">
-        <v>302</v>
+        <v>42</v>
       </c>
       <c r="J108" t="s">
         <v>209</v>
@@ -4348,19 +4362,13 @@
         <v>38</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F109" t="s">
-        <v>186</v>
-      </c>
-      <c r="G109" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="H109" t="s">
         <v>204</v>
       </c>
       <c r="I109" t="s">
-        <v>303</v>
+        <v>214</v>
       </c>
       <c r="J109" t="s">
         <v>209</v>
@@ -4374,59 +4382,62 @@
         <v>38</v>
       </c>
       <c r="B110" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H110" t="s">
+        <v>204</v>
+      </c>
+      <c r="I110" t="s">
+        <v>302</v>
+      </c>
+      <c r="J110" t="s">
+        <v>209</v>
+      </c>
+      <c r="K110" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="A111" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B111" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F111" t="s">
+        <v>186</v>
+      </c>
+      <c r="G111" t="s">
+        <v>187</v>
+      </c>
+      <c r="H111" t="s">
+        <v>204</v>
+      </c>
+      <c r="I111" t="s">
+        <v>303</v>
+      </c>
+      <c r="J111" t="s">
+        <v>209</v>
+      </c>
+      <c r="K111" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="A112" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F112" t="s">
         <v>184</v>
       </c>
-      <c r="G110" t="s">
+      <c r="G112" t="s">
         <v>187</v>
       </c>
-      <c r="H110" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11">
-      <c r="A111" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B111" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E111" t="s">
-        <v>53</v>
-      </c>
-      <c r="H111" t="s">
-        <v>203</v>
-      </c>
-      <c r="I111" t="s">
-        <v>304</v>
-      </c>
-      <c r="J111" t="s">
-        <v>212</v>
-      </c>
-      <c r="K111" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="112" spans="1:11">
-      <c r="A112" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="H112" t="s">
-        <v>203</v>
-      </c>
-      <c r="I112" t="s">
-        <v>211</v>
-      </c>
-      <c r="J112" t="s">
-        <v>212</v>
-      </c>
-      <c r="K112" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -4434,28 +4445,16 @@
         <v>44</v>
       </c>
       <c r="B113" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D113" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E113" t="s">
         <v>53</v>
       </c>
-      <c r="F113" t="s">
-        <v>162</v>
-      </c>
-      <c r="G113" t="s">
-        <v>174</v>
-      </c>
       <c r="H113" t="s">
         <v>203</v>
       </c>
       <c r="I113" t="s">
-        <v>46</v>
+        <v>304</v>
       </c>
       <c r="J113" t="s">
         <v>212</v>
@@ -4469,22 +4468,13 @@
         <v>44</v>
       </c>
       <c r="B114" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D114" t="s">
-        <v>92</v>
-      </c>
-      <c r="E114" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H114" t="s">
         <v>203</v>
       </c>
       <c r="I114" t="s">
-        <v>305</v>
+        <v>211</v>
       </c>
       <c r="J114" t="s">
         <v>212</v>
@@ -4498,27 +4488,91 @@
         <v>44</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D115" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E115" t="s">
         <v>53</v>
       </c>
+      <c r="F115" t="s">
+        <v>162</v>
+      </c>
+      <c r="G115" t="s">
+        <v>174</v>
+      </c>
       <c r="H115" t="s">
         <v>203</v>
       </c>
       <c r="I115" t="s">
-        <v>306</v>
+        <v>46</v>
       </c>
       <c r="J115" t="s">
         <v>212</v>
       </c>
       <c r="K115" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11">
+      <c r="A116" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C116" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D116" t="s">
+        <v>92</v>
+      </c>
+      <c r="E116" t="s">
+        <v>53</v>
+      </c>
+      <c r="H116" t="s">
+        <v>203</v>
+      </c>
+      <c r="I116" t="s">
+        <v>305</v>
+      </c>
+      <c r="J116" t="s">
+        <v>212</v>
+      </c>
+      <c r="K116" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11">
+      <c r="A117" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C117" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D117" t="s">
+        <v>48</v>
+      </c>
+      <c r="E117" t="s">
+        <v>53</v>
+      </c>
+      <c r="H117" t="s">
+        <v>203</v>
+      </c>
+      <c r="I117" t="s">
+        <v>306</v>
+      </c>
+      <c r="J117" t="s">
+        <v>212</v>
+      </c>
+      <c r="K117" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the gum benefit type
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chila\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A117DF67-7AB5-C541-96BD-E1F62B36D9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCC3578-9924-4E54-9E6C-9BB9F587EA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18800" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="41970" yWindow="-16215" windowWidth="29040" windowHeight="15720" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="361">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>NURSE1</t>
+  </si>
+  <si>
+    <t>ORALEX</t>
   </si>
 </sst>
 </file>
@@ -1549,11 +1552,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
   <dimension ref="A1:O124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5" customWidth="1"/>
@@ -2917,7 +2920,9 @@
       </c>
     </row>
     <row r="51" spans="1:12">
-      <c r="A51" s="3"/>
+      <c r="A51" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B51" s="3" t="s">
         <v>25</v>
       </c>
@@ -2935,7 +2940,9 @@
       </c>
     </row>
     <row r="52" spans="1:12">
-      <c r="A52" s="3"/>
+      <c r="A52" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B52" s="3" t="s">
         <v>25</v>
       </c>
@@ -2953,7 +2960,9 @@
       </c>
     </row>
     <row r="53" spans="1:12">
-      <c r="A53" s="3"/>
+      <c r="A53" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B53" s="3" t="s">
         <v>25</v>
       </c>
@@ -3031,7 +3040,9 @@
       </c>
     </row>
     <row r="57" spans="1:12">
-      <c r="A57" s="3"/>
+      <c r="A57" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B57" s="3" t="s">
         <v>25</v>
       </c>
@@ -3193,7 +3204,9 @@
       </c>
     </row>
     <row r="64" spans="1:12">
-      <c r="A64" s="3"/>
+      <c r="A64" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B64" s="3" t="s">
         <v>26</v>
       </c>
@@ -3211,7 +3224,9 @@
       </c>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="3"/>
+      <c r="A65" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B65" s="3" t="s">
         <v>26</v>
       </c>
@@ -3249,7 +3264,9 @@
       </c>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="3"/>
+      <c r="A67" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B67" s="3" t="s">
         <v>26</v>
       </c>
@@ -3520,7 +3537,9 @@
       </c>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="3"/>
+      <c r="A76" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B76" s="3" t="s">
         <v>29</v>
       </c>
@@ -4009,7 +4028,9 @@
       </c>
     </row>
     <row r="95" spans="1:12">
-      <c r="A95" s="3"/>
+      <c r="A95" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="B95" s="3" t="s">
         <v>348</v>
       </c>
@@ -4187,6 +4208,9 @@
       <c r="F101" t="s">
         <v>183</v>
       </c>
+      <c r="G101" t="s">
+        <v>187</v>
+      </c>
       <c r="H101" t="s">
         <v>204</v>
       </c>
@@ -4206,6 +4230,12 @@
       </c>
       <c r="B102" s="4" t="s">
         <v>39</v>
+      </c>
+      <c r="F102" t="s">
+        <v>360</v>
+      </c>
+      <c r="G102" t="s">
+        <v>187</v>
       </c>
       <c r="H102" t="s">
         <v>204</v>

</xml_diff>

<commit_message>
update the AXA benefit with logwin's case
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chila\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCC3578-9924-4E54-9E6C-9BB9F587EA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005F8051-5E6C-B648-B046-AA1217B51CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41970" yWindow="-16215" windowWidth="29040" windowHeight="15720" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="367">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1119,6 +1119,24 @@
   </si>
   <si>
     <t>ORALEX</t>
+  </si>
+  <si>
+    <t>H/A/T</t>
+  </si>
+  <si>
+    <t>GHCASH</t>
+  </si>
+  <si>
+    <t>EXTRAC</t>
+  </si>
+  <si>
+    <t>B/A/T</t>
+  </si>
+  <si>
+    <t>FILLIN</t>
+  </si>
+  <si>
+    <t>XL2</t>
   </si>
 </sst>
 </file>
@@ -1550,13 +1568,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:O124"/>
+  <dimension ref="A1:O127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5" customWidth="1"/>
@@ -1720,6 +1738,9 @@
       <c r="F5" t="s">
         <v>349</v>
       </c>
+      <c r="G5" t="s">
+        <v>174</v>
+      </c>
       <c r="H5" t="s">
         <v>203</v>
       </c>
@@ -2687,6 +2708,12 @@
       <c r="B41" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F41" t="s">
+        <v>362</v>
+      </c>
+      <c r="G41" t="s">
+        <v>174</v>
+      </c>
       <c r="H41" t="s">
         <v>203</v>
       </c>
@@ -3549,6 +3576,9 @@
       <c r="G76" t="s">
         <v>149</v>
       </c>
+      <c r="H76" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="3" t="s">
@@ -3607,19 +3637,10 @@
         <v>24</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D79" t="s">
-        <v>75</v>
-      </c>
-      <c r="E79" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F79" t="s">
-        <v>199</v>
+        <v>361</v>
       </c>
       <c r="G79" t="s">
         <v>149</v>
@@ -3627,43 +3648,22 @@
       <c r="H79" t="s">
         <v>204</v>
       </c>
-      <c r="I79" t="s">
-        <v>276</v>
-      </c>
-      <c r="J79" t="s">
-        <v>207</v>
-      </c>
-      <c r="K79" t="s">
-        <v>221</v>
-      </c>
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D80" t="s">
-        <v>93</v>
-      </c>
-      <c r="E80" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="F80" t="s">
+        <v>364</v>
+      </c>
+      <c r="G80" t="s">
+        <v>149</v>
       </c>
       <c r="H80" t="s">
         <v>204</v>
-      </c>
-      <c r="I80" t="s">
-        <v>277</v>
-      </c>
-      <c r="J80" t="s">
-        <v>207</v>
-      </c>
-      <c r="K80" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -3671,7 +3671,34 @@
         <v>24</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D81" t="s">
+        <v>75</v>
+      </c>
+      <c r="E81" t="s">
+        <v>50</v>
+      </c>
+      <c r="F81" t="s">
+        <v>199</v>
+      </c>
+      <c r="G81" t="s">
+        <v>149</v>
+      </c>
+      <c r="H81" t="s">
+        <v>204</v>
+      </c>
+      <c r="I81" t="s">
+        <v>276</v>
+      </c>
+      <c r="J81" t="s">
+        <v>207</v>
+      </c>
+      <c r="K81" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -3679,28 +3706,22 @@
         <v>24</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D82" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="E82" t="s">
         <v>50</v>
       </c>
-      <c r="F82" t="s">
-        <v>155</v>
-      </c>
-      <c r="G82" t="s">
-        <v>149</v>
-      </c>
       <c r="H82" t="s">
         <v>204</v>
       </c>
       <c r="I82" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J82" t="s">
         <v>207</v>
@@ -3708,34 +3729,13 @@
       <c r="K82" t="s">
         <v>221</v>
       </c>
-      <c r="L82" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F83" t="s">
-        <v>156</v>
-      </c>
-      <c r="G83" t="s">
-        <v>149</v>
-      </c>
-      <c r="H83" t="s">
-        <v>204</v>
-      </c>
-      <c r="I83" t="s">
-        <v>279</v>
-      </c>
-      <c r="J83" t="s">
-        <v>207</v>
-      </c>
-      <c r="K83" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -3743,19 +3743,19 @@
         <v>24</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D84" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E84" t="s">
         <v>50</v>
       </c>
       <c r="F84" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G84" t="s">
         <v>149</v>
@@ -3764,7 +3764,7 @@
         <v>204</v>
       </c>
       <c r="I84" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J84" t="s">
         <v>207</v>
@@ -3773,7 +3773,7 @@
         <v>221</v>
       </c>
       <c r="L84" t="s">
-        <v>337</v>
+        <v>318</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -3781,19 +3781,10 @@
         <v>24</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C85" s="6">
-        <v>253</v>
-      </c>
-      <c r="D85" t="s">
-        <v>91</v>
-      </c>
-      <c r="E85" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F85" t="s">
-        <v>223</v>
+        <v>156</v>
       </c>
       <c r="G85" t="s">
         <v>149</v>
@@ -3802,7 +3793,7 @@
         <v>204</v>
       </c>
       <c r="I85" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J85" t="s">
         <v>207</v>
@@ -3816,42 +3807,54 @@
         <v>24</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F86" t="s">
-        <v>198</v>
+        <v>366</v>
       </c>
       <c r="G86" t="s">
         <v>149</v>
       </c>
+      <c r="H86" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D87" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="E87" t="s">
         <v>50</v>
       </c>
+      <c r="F87" t="s">
+        <v>154</v>
+      </c>
+      <c r="G87" t="s">
+        <v>149</v>
+      </c>
       <c r="H87" t="s">
         <v>204</v>
       </c>
       <c r="I87" t="s">
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="J87" t="s">
         <v>207</v>
       </c>
       <c r="K87" t="s">
-        <v>216</v>
+        <v>221</v>
+      </c>
+      <c r="L87" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -3859,19 +3862,19 @@
         <v>24</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>122</v>
+        <v>34</v>
+      </c>
+      <c r="C88" s="6">
+        <v>253</v>
       </c>
       <c r="D88" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E88" t="s">
         <v>50</v>
       </c>
       <c r="F88" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
       <c r="G88" t="s">
         <v>149</v>
@@ -3880,13 +3883,13 @@
         <v>204</v>
       </c>
       <c r="I88" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="J88" t="s">
         <v>207</v>
       </c>
       <c r="K88" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -3894,42 +3897,42 @@
         <v>24</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F89" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="G89" t="s">
         <v>149</v>
       </c>
-      <c r="H89" t="s">
-        <v>204</v>
-      </c>
-      <c r="I89" t="s">
-        <v>284</v>
-      </c>
-      <c r="J89" t="s">
-        <v>207</v>
-      </c>
-      <c r="K89" t="s">
-        <v>221</v>
-      </c>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F90" t="s">
-        <v>193</v>
-      </c>
-      <c r="G90" t="s">
-        <v>149</v>
+        <v>35</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D90" t="s">
+        <v>35</v>
+      </c>
+      <c r="E90" t="s">
+        <v>50</v>
       </c>
       <c r="H90" t="s">
         <v>204</v>
+      </c>
+      <c r="I90" t="s">
+        <v>35</v>
+      </c>
+      <c r="J90" t="s">
+        <v>207</v>
+      </c>
+      <c r="K90" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -3937,25 +3940,34 @@
         <v>24</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C91" s="6">
-        <v>311</v>
+        <v>36</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="D91" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="E91" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="F91" t="s">
+        <v>197</v>
+      </c>
+      <c r="G91" t="s">
+        <v>149</v>
+      </c>
+      <c r="H91" t="s">
+        <v>204</v>
       </c>
       <c r="I91" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J91" t="s">
         <v>207</v>
       </c>
       <c r="K91" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="92" spans="1:12">
@@ -3963,16 +3975,25 @@
         <v>24</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C92" s="6">
-        <v>312</v>
-      </c>
-      <c r="D92" t="s">
-        <v>136</v>
-      </c>
-      <c r="E92" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="F92" t="s">
+        <v>192</v>
+      </c>
+      <c r="G92" t="s">
+        <v>149</v>
+      </c>
+      <c r="H92" t="s">
+        <v>204</v>
+      </c>
+      <c r="I92" t="s">
+        <v>284</v>
+      </c>
+      <c r="J92" t="s">
+        <v>207</v>
+      </c>
+      <c r="K92" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -3980,16 +4001,16 @@
         <v>24</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C93" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D93" t="s">
-        <v>307</v>
-      </c>
-      <c r="E93" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="F93" t="s">
+        <v>193</v>
+      </c>
+      <c r="G93" t="s">
+        <v>149</v>
+      </c>
+      <c r="H93" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -3997,28 +4018,19 @@
         <v>24</v>
       </c>
       <c r="B94" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C94" s="6">
         <v>311</v>
       </c>
-      <c r="C94" s="6" t="s">
-        <v>310</v>
-      </c>
       <c r="D94" t="s">
-        <v>309</v>
+        <v>76</v>
       </c>
       <c r="E94" t="s">
-        <v>50</v>
-      </c>
-      <c r="F94" t="s">
-        <v>189</v>
-      </c>
-      <c r="G94" t="s">
-        <v>149</v>
-      </c>
-      <c r="H94" t="s">
-        <v>204</v>
+        <v>52</v>
       </c>
       <c r="I94" t="s">
-        <v>356</v>
+        <v>285</v>
       </c>
       <c r="J94" t="s">
         <v>207</v>
@@ -4032,129 +4044,108 @@
         <v>24</v>
       </c>
       <c r="B95" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C95" s="6">
+        <v>312</v>
+      </c>
+      <c r="D95" t="s">
+        <v>136</v>
+      </c>
+      <c r="E95" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
+      <c r="A96" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D96" t="s">
+        <v>307</v>
+      </c>
+      <c r="E96" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12">
+      <c r="A97" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D97" t="s">
+        <v>309</v>
+      </c>
+      <c r="E97" t="s">
+        <v>50</v>
+      </c>
+      <c r="F97" t="s">
+        <v>189</v>
+      </c>
+      <c r="G97" t="s">
+        <v>149</v>
+      </c>
+      <c r="H97" t="s">
+        <v>204</v>
+      </c>
+      <c r="I97" t="s">
+        <v>356</v>
+      </c>
+      <c r="J97" t="s">
+        <v>207</v>
+      </c>
+      <c r="K97" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12">
+      <c r="A98" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F98" t="s">
         <v>347</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G98" t="s">
         <v>149</v>
       </c>
-      <c r="H95" t="s">
-        <v>204</v>
-      </c>
-      <c r="L95" t="s">
+      <c r="H98" t="s">
+        <v>204</v>
+      </c>
+      <c r="L98" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="96" spans="1:12">
-      <c r="A96" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C96" s="6">
-        <v>511</v>
-      </c>
-      <c r="D96" t="s">
-        <v>82</v>
-      </c>
-      <c r="E96" t="s">
-        <v>51</v>
-      </c>
-      <c r="F96" t="s">
-        <v>182</v>
-      </c>
-      <c r="G96" t="s">
-        <v>187</v>
-      </c>
-      <c r="H96" t="s">
-        <v>204</v>
-      </c>
-      <c r="I96" t="s">
-        <v>286</v>
-      </c>
-      <c r="J96" t="s">
-        <v>209</v>
-      </c>
-      <c r="K96" t="s">
-        <v>220</v>
-      </c>
-      <c r="L96" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11">
-      <c r="A97" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F97" t="s">
-        <v>180</v>
-      </c>
-      <c r="G97" t="s">
-        <v>187</v>
-      </c>
-      <c r="H97" t="s">
-        <v>204</v>
-      </c>
-      <c r="I97" t="s">
-        <v>287</v>
-      </c>
-      <c r="J97" t="s">
-        <v>209</v>
-      </c>
-      <c r="K97" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11">
-      <c r="A98" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C98" s="6">
-        <v>513</v>
-      </c>
-      <c r="D98" t="s">
-        <v>83</v>
-      </c>
-      <c r="E98" t="s">
-        <v>51</v>
-      </c>
-      <c r="F98" t="s">
-        <v>178</v>
-      </c>
-      <c r="G98" t="s">
-        <v>187</v>
-      </c>
-      <c r="H98" t="s">
-        <v>204</v>
-      </c>
-      <c r="I98" t="s">
-        <v>288</v>
-      </c>
-      <c r="J98" t="s">
-        <v>209</v>
-      </c>
-      <c r="K98" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:12">
       <c r="A99" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C99" s="6">
+        <v>511</v>
+      </c>
+      <c r="D99" t="s">
+        <v>82</v>
+      </c>
+      <c r="E99" t="s">
+        <v>51</v>
+      </c>
       <c r="F99" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G99" t="s">
         <v>187</v>
@@ -4163,7 +4154,7 @@
         <v>204</v>
       </c>
       <c r="I99" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J99" t="s">
         <v>209</v>
@@ -4171,8 +4162,11 @@
       <c r="K99" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="100" spans="1:11">
+      <c r="L99" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12">
       <c r="A100" s="4" t="s">
         <v>38</v>
       </c>
@@ -4180,7 +4174,7 @@
         <v>39</v>
       </c>
       <c r="F100" t="s">
-        <v>38</v>
+        <v>180</v>
       </c>
       <c r="G100" t="s">
         <v>187</v>
@@ -4189,24 +4183,33 @@
         <v>204</v>
       </c>
       <c r="I100" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J100" t="s">
         <v>209</v>
       </c>
       <c r="K100" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12">
       <c r="A101" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B101" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C101" s="6">
+        <v>513</v>
+      </c>
+      <c r="D101" t="s">
+        <v>83</v>
+      </c>
+      <c r="E101" t="s">
+        <v>51</v>
+      </c>
       <c r="F101" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="G101" t="s">
         <v>187</v>
@@ -4215,7 +4218,7 @@
         <v>204</v>
       </c>
       <c r="I101" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
       <c r="J101" t="s">
         <v>209</v>
@@ -4224,7 +4227,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="17" customHeight="1">
+    <row r="102" spans="1:12">
       <c r="A102" s="4" t="s">
         <v>38</v>
       </c>
@@ -4232,7 +4235,7 @@
         <v>39</v>
       </c>
       <c r="F102" t="s">
-        <v>360</v>
+        <v>177</v>
       </c>
       <c r="G102" t="s">
         <v>187</v>
@@ -4241,7 +4244,7 @@
         <v>204</v>
       </c>
       <c r="I102" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J102" t="s">
         <v>209</v>
@@ -4250,38 +4253,50 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="17" customHeight="1">
+    <row r="103" spans="1:12">
       <c r="A103" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B103" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F103" t="s">
+        <v>38</v>
+      </c>
+      <c r="G103" t="s">
+        <v>187</v>
+      </c>
       <c r="H103" t="s">
         <v>204</v>
       </c>
       <c r="I103" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="J103" t="s">
         <v>209</v>
       </c>
       <c r="K103" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="17" customHeight="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12">
       <c r="A104" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B104" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F104" t="s">
+        <v>183</v>
+      </c>
+      <c r="G104" t="s">
+        <v>187</v>
+      </c>
       <c r="H104" t="s">
         <v>204</v>
       </c>
       <c r="I104" t="s">
-        <v>293</v>
+        <v>39</v>
       </c>
       <c r="J104" t="s">
         <v>209</v>
@@ -4290,18 +4305,24 @@
         <v>220</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="17" customHeight="1">
+    <row r="105" spans="1:12" ht="17" customHeight="1">
       <c r="A105" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B105" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F105" t="s">
+        <v>360</v>
+      </c>
+      <c r="G105" t="s">
+        <v>187</v>
+      </c>
       <c r="H105" t="s">
         <v>204</v>
       </c>
       <c r="I105" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J105" t="s">
         <v>209</v>
@@ -4310,24 +4331,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="17" customHeight="1">
+    <row r="106" spans="1:12" ht="17" customHeight="1">
       <c r="A106" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F106" t="s">
-        <v>181</v>
-      </c>
-      <c r="G106" t="s">
-        <v>187</v>
-      </c>
       <c r="H106" t="s">
         <v>204</v>
       </c>
       <c r="I106" t="s">
-        <v>215</v>
+        <v>292</v>
       </c>
       <c r="J106" t="s">
         <v>209</v>
@@ -4336,24 +4351,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="17" customHeight="1">
+    <row r="107" spans="1:12" ht="17" customHeight="1">
       <c r="A107" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B107" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F107" t="s">
-        <v>185</v>
-      </c>
-      <c r="G107" t="s">
-        <v>187</v>
-      </c>
       <c r="H107" t="s">
         <v>204</v>
       </c>
       <c r="I107" t="s">
-        <v>215</v>
+        <v>293</v>
       </c>
       <c r="J107" t="s">
         <v>209</v>
@@ -4362,7 +4371,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="17" customHeight="1">
+    <row r="108" spans="1:12" ht="17" customHeight="1">
       <c r="A108" s="4" t="s">
         <v>38</v>
       </c>
@@ -4373,7 +4382,7 @@
         <v>204</v>
       </c>
       <c r="I108" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J108" t="s">
         <v>209</v>
@@ -4382,15 +4391,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:12" ht="17" customHeight="1">
       <c r="A109" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F109" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G109" t="s">
         <v>187</v>
@@ -4399,7 +4408,7 @@
         <v>204</v>
       </c>
       <c r="I109" t="s">
-        <v>296</v>
+        <v>215</v>
       </c>
       <c r="J109" t="s">
         <v>209</v>
@@ -4408,18 +4417,24 @@
         <v>220</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:12" ht="17" customHeight="1">
       <c r="A110" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="F110" t="s">
+        <v>185</v>
+      </c>
+      <c r="G110" t="s">
+        <v>187</v>
       </c>
       <c r="H110" t="s">
         <v>204</v>
       </c>
       <c r="I110" t="s">
-        <v>297</v>
+        <v>215</v>
       </c>
       <c r="J110" t="s">
         <v>209</v>
@@ -4428,18 +4443,18 @@
         <v>220</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:12" ht="17" customHeight="1">
       <c r="A111" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H111" t="s">
         <v>204</v>
       </c>
       <c r="I111" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="J111" t="s">
         <v>209</v>
@@ -4448,15 +4463,15 @@
         <v>220</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:12">
       <c r="A112" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F112" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G112" t="s">
         <v>187</v>
@@ -4465,7 +4480,7 @@
         <v>204</v>
       </c>
       <c r="I112" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J112" t="s">
         <v>209</v>
@@ -4479,13 +4494,19 @@
         <v>38</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="F113" t="s">
+        <v>365</v>
+      </c>
+      <c r="G113" t="s">
+        <v>187</v>
       </c>
       <c r="H113" t="s">
         <v>204</v>
       </c>
       <c r="I113" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J113" t="s">
         <v>209</v>
@@ -4499,19 +4520,13 @@
         <v>38</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F114" t="s">
-        <v>175</v>
-      </c>
-      <c r="G114" t="s">
-        <v>187</v>
+        <v>40</v>
       </c>
       <c r="H114" t="s">
         <v>204</v>
       </c>
       <c r="I114" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J114" t="s">
         <v>209</v>
@@ -4525,13 +4540,19 @@
         <v>38</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F115" t="s">
+        <v>179</v>
+      </c>
+      <c r="G115" t="s">
+        <v>187</v>
       </c>
       <c r="H115" t="s">
         <v>204</v>
       </c>
       <c r="I115" t="s">
-        <v>42</v>
+        <v>299</v>
       </c>
       <c r="J115" t="s">
         <v>209</v>
@@ -4545,13 +4566,16 @@
         <v>38</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F116" t="s">
+        <v>363</v>
       </c>
       <c r="H116" t="s">
         <v>204</v>
       </c>
       <c r="I116" t="s">
-        <v>214</v>
+        <v>300</v>
       </c>
       <c r="J116" t="s">
         <v>209</v>
@@ -4567,11 +4591,17 @@
       <c r="B117" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="F117" t="s">
+        <v>175</v>
+      </c>
+      <c r="G117" t="s">
+        <v>187</v>
+      </c>
       <c r="H117" t="s">
         <v>204</v>
       </c>
       <c r="I117" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J117" t="s">
         <v>209</v>
@@ -4585,19 +4615,13 @@
         <v>38</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F118" t="s">
-        <v>186</v>
-      </c>
-      <c r="G118" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="H118" t="s">
         <v>204</v>
       </c>
       <c r="I118" t="s">
-        <v>303</v>
+        <v>42</v>
       </c>
       <c r="J118" t="s">
         <v>209</v>
@@ -4611,94 +4635,82 @@
         <v>38</v>
       </c>
       <c r="B119" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H119" t="s">
+        <v>204</v>
+      </c>
+      <c r="I119" t="s">
+        <v>214</v>
+      </c>
+      <c r="J119" t="s">
+        <v>209</v>
+      </c>
+      <c r="K119" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
+      <c r="A120" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H120" t="s">
+        <v>204</v>
+      </c>
+      <c r="I120" t="s">
+        <v>302</v>
+      </c>
+      <c r="J120" t="s">
+        <v>209</v>
+      </c>
+      <c r="K120" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
+      <c r="A121" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F121" t="s">
+        <v>186</v>
+      </c>
+      <c r="G121" t="s">
+        <v>187</v>
+      </c>
+      <c r="H121" t="s">
+        <v>204</v>
+      </c>
+      <c r="I121" t="s">
+        <v>303</v>
+      </c>
+      <c r="J121" t="s">
+        <v>209</v>
+      </c>
+      <c r="K121" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F122" t="s">
         <v>184</v>
       </c>
-      <c r="G119" t="s">
+      <c r="G122" t="s">
         <v>187</v>
       </c>
-      <c r="H119" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11">
-      <c r="A120" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B120" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E120" t="s">
-        <v>53</v>
-      </c>
-      <c r="H120" t="s">
-        <v>203</v>
-      </c>
-      <c r="I120" t="s">
-        <v>304</v>
-      </c>
-      <c r="J120" t="s">
-        <v>212</v>
-      </c>
-      <c r="K120" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11">
-      <c r="A121" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H121" t="s">
-        <v>203</v>
-      </c>
-      <c r="I121" t="s">
-        <v>211</v>
-      </c>
-      <c r="J121" t="s">
-        <v>212</v>
-      </c>
-      <c r="K121" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11">
-      <c r="A122" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D122" t="s">
-        <v>46</v>
-      </c>
-      <c r="E122" t="s">
-        <v>53</v>
-      </c>
-      <c r="F122" t="s">
-        <v>162</v>
-      </c>
-      <c r="G122" t="s">
-        <v>174</v>
-      </c>
       <c r="H122" t="s">
-        <v>203</v>
-      </c>
-      <c r="I122" t="s">
-        <v>46</v>
-      </c>
-      <c r="J122" t="s">
-        <v>212</v>
-      </c>
-      <c r="K122" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
     </row>
     <row r="123" spans="1:11">
@@ -4706,13 +4718,7 @@
         <v>44</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D123" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E123" t="s">
         <v>53</v>
@@ -4721,7 +4727,7 @@
         <v>203</v>
       </c>
       <c r="I123" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J123" t="s">
         <v>212</v>
@@ -4735,27 +4741,111 @@
         <v>44</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D124" t="s">
-        <v>48</v>
-      </c>
-      <c r="E124" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H124" t="s">
         <v>203</v>
       </c>
       <c r="I124" t="s">
-        <v>306</v>
+        <v>211</v>
       </c>
       <c r="J124" t="s">
         <v>212</v>
       </c>
       <c r="K124" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D125" t="s">
+        <v>46</v>
+      </c>
+      <c r="E125" t="s">
+        <v>53</v>
+      </c>
+      <c r="F125" t="s">
+        <v>162</v>
+      </c>
+      <c r="G125" t="s">
+        <v>174</v>
+      </c>
+      <c r="H125" t="s">
+        <v>203</v>
+      </c>
+      <c r="I125" t="s">
+        <v>46</v>
+      </c>
+      <c r="J125" t="s">
+        <v>212</v>
+      </c>
+      <c r="K125" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D126" t="s">
+        <v>92</v>
+      </c>
+      <c r="E126" t="s">
+        <v>53</v>
+      </c>
+      <c r="H126" t="s">
+        <v>203</v>
+      </c>
+      <c r="I126" t="s">
+        <v>305</v>
+      </c>
+      <c r="J126" t="s">
+        <v>212</v>
+      </c>
+      <c r="K126" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D127" t="s">
+        <v>48</v>
+      </c>
+      <c r="E127" t="s">
+        <v>53</v>
+      </c>
+      <c r="H127" t="s">
+        <v>203</v>
+      </c>
+      <c r="I127" t="s">
+        <v>306</v>
+      </c>
+      <c r="J127" t="s">
+        <v>212</v>
+      </c>
+      <c r="K127" t="s">
         <v>217</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the benefit indexing
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005F8051-5E6C-B648-B046-AA1217B51CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB52B4B9-BE17-5F48-BA5E-DDEC2D29EC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="19600" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="371">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -638,9 +660,6 @@
     <t>PSYCHI</t>
   </si>
   <si>
-    <t>Day Centre</t>
-  </si>
-  <si>
     <t>aia_benefit_type</t>
   </si>
   <si>
@@ -1137,6 +1156,21 @@
   </si>
   <si>
     <t>XL2</t>
+  </si>
+  <si>
+    <t>Day Centre - Viral Warts</t>
+  </si>
+  <si>
+    <t>Day Centre - Endoscopy</t>
+  </si>
+  <si>
+    <t>Day Centre - Cancer and Dialysis</t>
+  </si>
+  <si>
+    <t>Pre&amp;Post Hosp Cinic Consultation</t>
+  </si>
+  <si>
+    <t>Pre&amp;Post Hosp Inpatient Consultation</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1255,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1232,6 +1266,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1568,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:O127"/>
+  <dimension ref="A1:R129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -1585,7 +1621,7 @@
     <col min="8" max="8" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>78</v>
       </c>
@@ -1608,22 +1644,22 @@
         <v>148</v>
       </c>
       <c r="H1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I1" t="s">
         <v>201</v>
       </c>
-      <c r="I1" t="s">
-        <v>202</v>
-      </c>
       <c r="J1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="17" customHeight="1">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -1646,22 +1682,22 @@
         <v>174</v>
       </c>
       <c r="H2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I2" t="s">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="17" customHeight="1">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="17" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1675,22 +1711,22 @@
         <v>174</v>
       </c>
       <c r="H3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I3" t="s">
         <v>54</v>
       </c>
       <c r="J3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1713,22 +1749,22 @@
         <v>174</v>
       </c>
       <c r="H4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L4" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -1736,25 +1772,29 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G5" t="s">
         <v>174</v>
       </c>
       <c r="H5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="R5" t="str" cm="1">
+        <f t="array" ref="R5:R60">_xlfn.UNIQUE(B1:B129)</f>
+        <v>gum_benefit</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1777,1176 +1817,1291 @@
         <v>174</v>
       </c>
       <c r="H6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L6" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>329</v>
+      </c>
+      <c r="R6" t="str">
+        <v>Daily Room &amp; Board</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
+      <c r="C7" s="7"/>
       <c r="H7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L7" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>328</v>
+      </c>
+      <c r="R7" t="str">
+        <v>In-hosptial Doctor's Visit</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G8" t="s">
-        <v>174</v>
-      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="L8" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>338</v>
+      </c>
+      <c r="R8" t="str">
+        <v>Miscellaneous Hospital Expense/ Other Hospital Services</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>127</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9" t="s">
-        <v>174</v>
-      </c>
-      <c r="H9" t="s">
-        <v>203</v>
-      </c>
-      <c r="I9" t="s">
-        <v>228</v>
-      </c>
-      <c r="J9" t="s">
-        <v>206</v>
-      </c>
-      <c r="K9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="R9" t="str">
+        <v>Companion Bed</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="H10" t="s">
-        <v>203</v>
-      </c>
-      <c r="I10" t="s">
-        <v>229</v>
-      </c>
-      <c r="J10" t="s">
-        <v>206</v>
-      </c>
-      <c r="K10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>366</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>221</v>
+      </c>
+      <c r="G10" t="s">
+        <v>174</v>
+      </c>
+      <c r="L10" t="s">
+        <v>341</v>
+      </c>
+      <c r="R10" t="str">
+        <v>Day Centre - Viral Warts</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="H11" t="s">
-        <v>203</v>
-      </c>
-      <c r="I11" t="s">
-        <v>230</v>
-      </c>
-      <c r="J11" t="s">
-        <v>206</v>
-      </c>
-      <c r="K11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>367</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R11" t="str">
+        <v>Day Centre - Endoscopy</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="H12" t="s">
-        <v>203</v>
-      </c>
-      <c r="I12" t="s">
-        <v>231</v>
-      </c>
-      <c r="J12" t="s">
-        <v>206</v>
-      </c>
-      <c r="K12" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>368</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" t="s">
+        <v>174</v>
+      </c>
+      <c r="R12" t="str">
+        <v>Day Centre - Cancer and Dialysis</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="H13" t="s">
-        <v>203</v>
-      </c>
-      <c r="I13" t="s">
-        <v>232</v>
-      </c>
-      <c r="J13" t="s">
-        <v>206</v>
-      </c>
-      <c r="K13" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="R13" t="str">
+        <v>Surgeon Fee - Complex</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" t="s">
         <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="G14" t="s">
         <v>174</v>
       </c>
+      <c r="H14" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" t="s">
+        <v>232</v>
+      </c>
+      <c r="J14" t="s">
+        <v>205</v>
+      </c>
+      <c r="K14" t="s">
+        <v>217</v>
+      </c>
       <c r="L14" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12">
+        <v>334</v>
+      </c>
+      <c r="R14" t="str">
+        <v>Surgeon Fee - Major</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>202</v>
+      </c>
+      <c r="I15" t="s">
+        <v>233</v>
+      </c>
+      <c r="J15" t="s">
+        <v>205</v>
+      </c>
+      <c r="K15" t="s">
+        <v>217</v>
+      </c>
+      <c r="R15" t="str">
+        <v>Surgeon Fee - Inter</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="H16" t="s">
+        <v>202</v>
+      </c>
+      <c r="I16" t="s">
+        <v>234</v>
+      </c>
+      <c r="J16" t="s">
+        <v>205</v>
+      </c>
+      <c r="K16" t="s">
+        <v>217</v>
+      </c>
+      <c r="L16" t="s">
+        <v>324</v>
+      </c>
+      <c r="O16" t="s">
+        <v>194</v>
+      </c>
+      <c r="R16" t="str">
+        <v>Surgeon Fee - Minor</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F17" t="s">
-        <v>158</v>
-      </c>
-      <c r="G17" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I17" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="J17" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K17" t="s">
-        <v>218</v>
-      </c>
-      <c r="L17" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="R17" t="str">
+        <v>Anaesthetist's Fees - Complex</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
       </c>
       <c r="H18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I18" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K18" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="L18" t="s">
+        <v>321</v>
+      </c>
+      <c r="R18" t="str">
+        <v>Anaesthetist's Fees - Major</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E19" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I19" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="J19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K19" t="s">
-        <v>218</v>
-      </c>
-      <c r="L19" t="s">
-        <v>325</v>
-      </c>
-      <c r="O19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="R19" t="str">
+        <v>Anaesthetist's Fees - Inter</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" t="s">
-        <v>203</v>
-      </c>
-      <c r="I20" t="s">
-        <v>236</v>
-      </c>
-      <c r="J20" t="s">
-        <v>206</v>
-      </c>
-      <c r="K20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="R20" t="str">
+        <v>Anaesthetist's Fees - Minor</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
         <v>49</v>
       </c>
+      <c r="F21" t="s">
+        <v>159</v>
+      </c>
+      <c r="G21" t="s">
+        <v>174</v>
+      </c>
       <c r="H21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I21" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="J21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L21" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>342</v>
+      </c>
+      <c r="R21" t="str">
+        <v>Operation Theatre Fees - Complex</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
       </c>
       <c r="H22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I22" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="L22" t="s">
+        <v>325</v>
+      </c>
+      <c r="R22" t="str">
+        <v>Operation Theatre Fees - Major</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D23" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="H23" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" t="s">
+        <v>240</v>
+      </c>
+      <c r="J23" t="s">
+        <v>205</v>
+      </c>
+      <c r="K23" t="s">
+        <v>217</v>
+      </c>
+      <c r="L23" t="s">
+        <v>339</v>
+      </c>
+      <c r="R23" t="str">
+        <v>Operation Theatre Fees - Inter</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D24" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s">
         <v>49</v>
       </c>
-      <c r="F24" t="s">
-        <v>159</v>
-      </c>
-      <c r="G24" t="s">
-        <v>174</v>
-      </c>
-      <c r="H24" t="s">
-        <v>203</v>
-      </c>
-      <c r="I24" t="s">
-        <v>239</v>
-      </c>
-      <c r="J24" t="s">
-        <v>206</v>
-      </c>
-      <c r="K24" t="s">
-        <v>218</v>
-      </c>
-      <c r="L24" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="R24" t="str">
+        <v>Operation Theatre Fees - Minor</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E25" t="s">
         <v>49</v>
       </c>
+      <c r="F25" t="s">
+        <v>160</v>
+      </c>
+      <c r="G25" t="s">
+        <v>174</v>
+      </c>
       <c r="H25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I25" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J25" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L25" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15">
+        <v>335</v>
+      </c>
+      <c r="R25" t="str">
+        <v>Specialist's Fee (IP)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I26" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J26" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K26" t="s">
-        <v>218</v>
-      </c>
-      <c r="L26" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="R26" t="str">
+        <v>Intensive Care Unit</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D27" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="H27" t="s">
+        <v>202</v>
+      </c>
+      <c r="I27" t="s">
+        <v>243</v>
+      </c>
+      <c r="J27" t="s">
+        <v>205</v>
+      </c>
+      <c r="K27" t="s">
+        <v>217</v>
+      </c>
+      <c r="L27" t="s">
+        <v>326</v>
+      </c>
+      <c r="R27" t="str">
+        <v>Special Registered Nursing</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" t="s">
-        <v>49</v>
-      </c>
-      <c r="F28" t="s">
-        <v>160</v>
-      </c>
-      <c r="G28" t="s">
-        <v>174</v>
+        <v>13</v>
       </c>
       <c r="H28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I28" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K28" t="s">
-        <v>218</v>
-      </c>
-      <c r="L28" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="R28" t="str">
+        <v>Home Care</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>49</v>
       </c>
       <c r="H29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I29" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="J29" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="L29" t="s">
+        <v>340</v>
+      </c>
+      <c r="R29" t="str">
+        <v>Pre&amp;Post Hosp Cinic Consultation</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D30" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="H30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I30" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K30" t="s">
-        <v>218</v>
-      </c>
-      <c r="L30" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="R30" t="str">
+        <v>Pre&amp;Post Hosp Inpatient Consultation</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" t="s">
+        <v>168</v>
+      </c>
+      <c r="G31" t="s">
+        <v>174</v>
       </c>
       <c r="H31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I31" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="J31" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K31" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15">
+        <v>217</v>
+      </c>
+      <c r="L31" t="s">
+        <v>343</v>
+      </c>
+      <c r="R31" t="str">
+        <v>Daily Cash Benefit (HA's Ward)</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" t="s">
-        <v>49</v>
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>350</v>
+      </c>
+      <c r="G32" t="s">
+        <v>174</v>
       </c>
       <c r="H32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I32" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="J32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K32" t="s">
-        <v>218</v>
-      </c>
-      <c r="L32" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="R32" t="str">
+        <v>Secondary Claim Incentive/ Hospital Income for Coordination</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H33" t="s">
-        <v>203</v>
-      </c>
-      <c r="I33" t="s">
-        <v>247</v>
-      </c>
-      <c r="J33" t="s">
-        <v>206</v>
-      </c>
-      <c r="K33" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12">
+        <v>16</v>
+      </c>
+      <c r="F33" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" t="s">
+        <v>174</v>
+      </c>
+      <c r="L33" t="s">
+        <v>345</v>
+      </c>
+      <c r="R33" t="str">
+        <v xml:space="preserve">Emergency Assistance Service </v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
         <v>49</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>358</v>
       </c>
       <c r="G34" t="s">
         <v>174</v>
       </c>
       <c r="H34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I34" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="J34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K34" t="s">
-        <v>218</v>
-      </c>
-      <c r="L34" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="R34" t="str">
+        <v>Psyciatric treatments</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" t="s">
-        <v>351</v>
-      </c>
-      <c r="G35" t="s">
-        <v>174</v>
-      </c>
-      <c r="H35" t="s">
-        <v>203</v>
-      </c>
-      <c r="I35" t="s">
-        <v>249</v>
-      </c>
-      <c r="J35" t="s">
-        <v>206</v>
-      </c>
-      <c r="K35" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12">
+        <v>18</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="R35" t="str">
+        <v>Top-up/SMM</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
+        <v>369</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="G36" t="s">
         <v>174</v>
       </c>
-      <c r="L36" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="H36" t="s">
+        <v>202</v>
+      </c>
+      <c r="I36" t="s">
+        <v>229</v>
+      </c>
+      <c r="J36" t="s">
+        <v>205</v>
+      </c>
+      <c r="K36" t="s">
+        <v>217</v>
+      </c>
+      <c r="R36" t="str">
+        <v>General Consultation (GP)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D37" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" t="s">
-        <v>49</v>
-      </c>
-      <c r="F37" t="s">
-        <v>359</v>
-      </c>
-      <c r="G37" t="s">
-        <v>174</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
       <c r="H37" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I37" t="s">
-        <v>250</v>
+        <v>231</v>
       </c>
       <c r="J37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K37" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="R37" t="str">
+        <v>Specialist Consultation (SP)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:12">
+        <v>370</v>
+      </c>
+      <c r="C38" s="10"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="H38" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" t="s">
+        <v>227</v>
+      </c>
+      <c r="J38" t="s">
+        <v>205</v>
+      </c>
+      <c r="K38" t="s">
+        <v>217</v>
+      </c>
+      <c r="R38" t="str">
+        <v>Physio (PT)</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="6">
-        <v>210</v>
-      </c>
-      <c r="D39" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" t="s">
-        <v>166</v>
-      </c>
-      <c r="G39" t="s">
-        <v>174</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="C39" s="10"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
       <c r="H39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I39" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
       <c r="J39" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K39" t="s">
-        <v>218</v>
-      </c>
-      <c r="L39" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="R39" t="str">
+        <v>Chiro (CT)</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="6">
-        <v>220</v>
-      </c>
-      <c r="D40" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" t="s">
-        <v>49</v>
-      </c>
-      <c r="F40" t="s">
-        <v>171</v>
-      </c>
-      <c r="G40" t="s">
-        <v>174</v>
-      </c>
+        <v>370</v>
+      </c>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
       <c r="H40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I40" t="s">
-        <v>252</v>
+        <v>230</v>
       </c>
       <c r="J40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K40" t="s">
-        <v>218</v>
-      </c>
-      <c r="L40" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="R40" t="str">
+        <v>Chinese Med (CMT)</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C41" s="6">
+        <v>210</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
+        <v>49</v>
+      </c>
       <c r="F41" t="s">
-        <v>362</v>
+        <v>166</v>
       </c>
       <c r="G41" t="s">
         <v>174</v>
       </c>
       <c r="H41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I41" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K41" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12">
+        <v>217</v>
+      </c>
+      <c r="L41" t="s">
+        <v>319</v>
+      </c>
+      <c r="R41" t="str">
+        <v>Psychiatric Treatment (Psychi)</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C42" s="6">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E42" t="s">
         <v>49</v>
       </c>
       <c r="F42" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="G42" t="s">
         <v>174</v>
       </c>
       <c r="H42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I42" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="J42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L42" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12">
+        <v>337</v>
+      </c>
+      <c r="R42" t="str">
+        <v>Psychology counselling (Psycho)</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" t="s">
-        <v>172</v>
+        <v>361</v>
       </c>
       <c r="G43" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="H43" t="s">
+        <v>202</v>
+      </c>
+      <c r="I43" t="s">
+        <v>252</v>
+      </c>
+      <c r="J43" t="s">
+        <v>205</v>
+      </c>
+      <c r="K43" t="s">
+        <v>217</v>
+      </c>
+      <c r="R43" t="str">
+        <v>Overall Max Number of Visits</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12">
+        <v>20</v>
+      </c>
+      <c r="C44" s="6">
+        <v>230</v>
+      </c>
+      <c r="D44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+      <c r="F44" t="s">
+        <v>164</v>
+      </c>
+      <c r="G44" t="s">
+        <v>174</v>
+      </c>
+      <c r="H44" t="s">
+        <v>202</v>
+      </c>
+      <c r="I44" t="s">
+        <v>253</v>
+      </c>
+      <c r="J44" t="s">
+        <v>205</v>
+      </c>
+      <c r="K44" t="s">
+        <v>217</v>
+      </c>
+      <c r="L44" t="s">
+        <v>344</v>
+      </c>
+      <c r="R44" t="str">
+        <v>Diagnostic: X-Ray &amp; Lab Test (DX)</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" t="s">
+        <v>172</v>
+      </c>
+      <c r="G45" t="s">
+        <v>174</v>
+      </c>
+      <c r="R45" t="str">
+        <v>Prescribed Medicine (PM)</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R46" t="str">
+        <v>Vaccination</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>129</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E47" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="A46" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B46" s="2" t="s">
+      <c r="R47" t="str">
+        <v xml:space="preserve">Physical Health Check up </v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>66</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E48" t="s">
         <v>49</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F48" t="s">
         <v>169</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G48" t="s">
         <v>174</v>
       </c>
-      <c r="H46" t="s">
-        <v>203</v>
-      </c>
-      <c r="I46" t="s">
-        <v>255</v>
-      </c>
-      <c r="J46" t="s">
-        <v>210</v>
-      </c>
-      <c r="K46" t="s">
-        <v>219</v>
-      </c>
-      <c r="L46" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="A47" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D47" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F47" t="s">
-        <v>144</v>
-      </c>
-      <c r="G47" t="s">
-        <v>149</v>
-      </c>
-      <c r="H47" t="s">
-        <v>204</v>
-      </c>
-      <c r="I47" t="s">
-        <v>256</v>
-      </c>
-      <c r="J47" t="s">
-        <v>207</v>
-      </c>
-      <c r="K47" t="s">
-        <v>221</v>
-      </c>
-      <c r="L47" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F48" t="s">
-        <v>145</v>
-      </c>
-      <c r="G48" t="s">
-        <v>149</v>
-      </c>
       <c r="H48" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I48" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="J48" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="K48" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
+        <v>218</v>
+      </c>
+      <c r="L48" t="s">
+        <v>331</v>
+      </c>
+      <c r="R48" t="str">
+        <v>Eye Examination</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C49" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" t="s">
+        <v>144</v>
+      </c>
+      <c r="G49" t="s">
+        <v>149</v>
+      </c>
       <c r="H49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I49" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="J49" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K49" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="L49" t="s">
+        <v>314</v>
+      </c>
+      <c r="R49" t="str">
+        <v>Emergency treatment</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F50" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" t="s">
+        <v>149</v>
+      </c>
       <c r="H50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I50" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="J50" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K50" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R50" t="str">
+        <v>Combined Wellness Benefit</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51" s="3" t="s">
         <v>24</v>
       </c>
@@ -2954,19 +3109,22 @@
         <v>25</v>
       </c>
       <c r="H51" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I51" t="s">
-        <v>353</v>
+        <v>257</v>
       </c>
       <c r="J51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K51" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R51" t="str">
+        <v>Combined Wellness Benefit - Vac&amp;Opt</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="3" t="s">
         <v>24</v>
       </c>
@@ -2974,19 +3132,22 @@
         <v>25</v>
       </c>
       <c r="H52" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I52" t="s">
-        <v>354</v>
+        <v>258</v>
       </c>
       <c r="J52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K52" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R52" t="str">
+        <v>Oral Examination</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" s="3" t="s">
         <v>24</v>
       </c>
@@ -2994,19 +3155,22 @@
         <v>25</v>
       </c>
       <c r="H53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I53" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="J53" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K53" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R53" t="str">
+        <v xml:space="preserve">Fillings </v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" s="3" t="s">
         <v>24</v>
       </c>
@@ -3014,19 +3178,22 @@
         <v>25</v>
       </c>
       <c r="H54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I54" t="s">
-        <v>260</v>
+        <v>353</v>
       </c>
       <c r="J54" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K54" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R54" t="str">
+        <v>Simple Extractions</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
       <c r="A55" s="3" t="s">
         <v>24</v>
       </c>
@@ -3034,19 +3201,22 @@
         <v>25</v>
       </c>
       <c r="H55" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I55" t="s">
-        <v>261</v>
+        <v>356</v>
       </c>
       <c r="J55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K55" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R55" t="str">
+        <v>X-Ray</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18">
       <c r="A56" s="3" t="s">
         <v>24</v>
       </c>
@@ -3054,19 +3224,22 @@
         <v>25</v>
       </c>
       <c r="H56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I56" t="s">
-        <v>215</v>
+        <v>259</v>
       </c>
       <c r="J56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K56" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R56" t="str">
+        <v>Due to accident: Dentures, crowns and bridges</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18">
       <c r="A57" s="3" t="s">
         <v>24</v>
       </c>
@@ -3074,103 +3247,109 @@
         <v>25</v>
       </c>
       <c r="H57" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I57" t="s">
-        <v>352</v>
+        <v>260</v>
       </c>
       <c r="J57" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K57" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R57" t="str">
+        <v>Pre&amp;Post Natal</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18">
       <c r="A58" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D58" t="s">
-        <v>69</v>
-      </c>
-      <c r="E58" t="s">
-        <v>50</v>
-      </c>
-      <c r="F58" t="s">
-        <v>146</v>
-      </c>
-      <c r="G58" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="H58" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I58" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="J58" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K58" t="s">
-        <v>221</v>
-      </c>
-      <c r="L58" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R58" t="str">
+        <v>Normal Delivery</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18">
       <c r="A59" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H59" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I59" t="s">
-        <v>262</v>
+        <v>351</v>
       </c>
       <c r="J59" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K59" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="R59" t="str">
+        <v>Caesarean</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18">
       <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C60" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" t="s">
+        <v>69</v>
+      </c>
+      <c r="E60" t="s">
+        <v>50</v>
+      </c>
       <c r="F60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G60" t="s">
         <v>149</v>
       </c>
       <c r="H60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I60" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="J60" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K60" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12">
+        <v>220</v>
+      </c>
+      <c r="L60" t="s">
+        <v>316</v>
+      </c>
+      <c r="R60" t="str">
+        <v>Miscarriage</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18">
       <c r="A61" s="3" t="s">
         <v>24</v>
       </c>
@@ -3178,39 +3357,45 @@
         <v>26</v>
       </c>
       <c r="H61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I61" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K61" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F62" t="s">
+        <v>147</v>
+      </c>
+      <c r="G62" t="s">
+        <v>149</v>
+      </c>
       <c r="H62" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I62" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K62" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18">
       <c r="A63" s="3" t="s">
         <v>24</v>
       </c>
@@ -3218,19 +3403,19 @@
         <v>26</v>
       </c>
       <c r="H63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I63" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J63" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K63" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="A64" s="3" t="s">
         <v>24</v>
       </c>
@@ -3238,16 +3423,16 @@
         <v>26</v>
       </c>
       <c r="H64" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I64" t="s">
-        <v>355</v>
+        <v>264</v>
       </c>
       <c r="J64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -3258,16 +3443,16 @@
         <v>26</v>
       </c>
       <c r="H65" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I65" t="s">
-        <v>358</v>
+        <v>265</v>
       </c>
       <c r="J65" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K65" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -3278,16 +3463,16 @@
         <v>26</v>
       </c>
       <c r="H66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I66" t="s">
-        <v>208</v>
+        <v>354</v>
       </c>
       <c r="J66" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K66" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -3298,16 +3483,16 @@
         <v>26</v>
       </c>
       <c r="H67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I67" t="s">
-        <v>282</v>
+        <v>357</v>
       </c>
       <c r="J67" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K67" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -3315,37 +3500,19 @@
         <v>24</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D68" t="s">
-        <v>70</v>
-      </c>
-      <c r="E68" t="s">
-        <v>50</v>
-      </c>
-      <c r="F68" t="s">
-        <v>152</v>
-      </c>
-      <c r="G68" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="H68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I68" t="s">
-        <v>267</v>
+        <v>207</v>
       </c>
       <c r="J68" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K68" t="s">
-        <v>221</v>
-      </c>
-      <c r="L68" t="s">
-        <v>334</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:12">
@@ -3353,19 +3520,19 @@
         <v>24</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I69" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="J69" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K69" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:12">
@@ -3375,23 +3542,35 @@
       <c r="B70" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C70" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" t="s">
+        <v>70</v>
+      </c>
+      <c r="E70" t="s">
+        <v>50</v>
+      </c>
       <c r="F70" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G70" t="s">
         <v>149</v>
       </c>
       <c r="H70" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I70" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J70" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K70" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="L70" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -3401,23 +3580,17 @@
       <c r="B71" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F71" t="s">
-        <v>190</v>
-      </c>
-      <c r="G71" t="s">
-        <v>149</v>
-      </c>
       <c r="H71" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I71" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J71" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:12">
@@ -3425,37 +3598,25 @@
         <v>24</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D72" t="s">
-        <v>85</v>
-      </c>
-      <c r="E72" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F72" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="G72" t="s">
         <v>149</v>
       </c>
       <c r="H72" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I72" t="s">
-        <v>85</v>
+        <v>268</v>
       </c>
       <c r="J72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K72" t="s">
-        <v>221</v>
-      </c>
-      <c r="L72" t="s">
-        <v>321</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" spans="1:12">
@@ -3463,37 +3624,25 @@
         <v>24</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D73" t="s">
-        <v>73</v>
-      </c>
-      <c r="E73" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F73" t="s">
-        <v>151</v>
+        <v>190</v>
       </c>
       <c r="G73" t="s">
         <v>149</v>
       </c>
       <c r="H73" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I73" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J73" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K73" t="s">
-        <v>221</v>
-      </c>
-      <c r="L73" t="s">
-        <v>314</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:12">
@@ -3501,37 +3650,37 @@
         <v>24</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D74" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E74" t="s">
         <v>50</v>
       </c>
       <c r="F74" t="s">
-        <v>196</v>
+        <v>150</v>
       </c>
       <c r="G74" t="s">
         <v>149</v>
       </c>
       <c r="H74" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I74" t="s">
-        <v>272</v>
+        <v>85</v>
       </c>
       <c r="J74" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K74" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L74" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="75" spans="1:12">
@@ -3541,26 +3690,35 @@
       <c r="B75" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C75" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D75" t="s">
+        <v>73</v>
+      </c>
+      <c r="E75" t="s">
+        <v>50</v>
+      </c>
       <c r="F75" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="G75" t="s">
         <v>149</v>
       </c>
       <c r="H75" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I75" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J75" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K75" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L75" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="76" spans="1:12">
@@ -3570,14 +3728,35 @@
       <c r="B76" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C76" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D76" t="s">
+        <v>74</v>
+      </c>
+      <c r="E76" t="s">
+        <v>50</v>
+      </c>
       <c r="F76" t="s">
-        <v>350</v>
+        <v>196</v>
       </c>
       <c r="G76" t="s">
         <v>149</v>
       </c>
       <c r="H76" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="I76" t="s">
+        <v>271</v>
+      </c>
+      <c r="J76" t="s">
+        <v>206</v>
+      </c>
+      <c r="K76" t="s">
+        <v>220</v>
+      </c>
+      <c r="L76" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="77" spans="1:12">
@@ -3588,22 +3767,25 @@
         <v>29</v>
       </c>
       <c r="F77" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G77" t="s">
         <v>149</v>
       </c>
       <c r="H77" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I77" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J77" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K77" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="L77" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="78" spans="1:12">
@@ -3614,22 +3796,13 @@
         <v>29</v>
       </c>
       <c r="F78" t="s">
-        <v>195</v>
+        <v>349</v>
       </c>
       <c r="G78" t="s">
         <v>149</v>
       </c>
       <c r="H78" t="s">
-        <v>204</v>
-      </c>
-      <c r="I78" t="s">
-        <v>275</v>
-      </c>
-      <c r="J78" t="s">
-        <v>207</v>
-      </c>
-      <c r="K78" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="1:12">
@@ -3640,13 +3813,22 @@
         <v>29</v>
       </c>
       <c r="F79" t="s">
-        <v>361</v>
+        <v>191</v>
       </c>
       <c r="G79" t="s">
         <v>149</v>
       </c>
       <c r="H79" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="I79" t="s">
+        <v>273</v>
+      </c>
+      <c r="J79" t="s">
+        <v>206</v>
+      </c>
+      <c r="K79" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:12">
@@ -3657,13 +3839,22 @@
         <v>29</v>
       </c>
       <c r="F80" t="s">
-        <v>364</v>
+        <v>195</v>
       </c>
       <c r="G80" t="s">
         <v>149</v>
       </c>
       <c r="H80" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="I80" t="s">
+        <v>274</v>
+      </c>
+      <c r="J80" t="s">
+        <v>206</v>
+      </c>
+      <c r="K80" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -3671,34 +3862,16 @@
         <v>24</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D81" t="s">
-        <v>75</v>
-      </c>
-      <c r="E81" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F81" t="s">
-        <v>199</v>
+        <v>360</v>
       </c>
       <c r="G81" t="s">
         <v>149</v>
       </c>
       <c r="H81" t="s">
-        <v>204</v>
-      </c>
-      <c r="I81" t="s">
-        <v>276</v>
-      </c>
-      <c r="J81" t="s">
-        <v>207</v>
-      </c>
-      <c r="K81" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" spans="1:12">
@@ -3706,28 +3879,16 @@
         <v>24</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D82" t="s">
-        <v>93</v>
-      </c>
-      <c r="E82" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="F82" t="s">
+        <v>363</v>
+      </c>
+      <c r="G82" t="s">
+        <v>149</v>
       </c>
       <c r="H82" t="s">
-        <v>204</v>
-      </c>
-      <c r="I82" t="s">
-        <v>277</v>
-      </c>
-      <c r="J82" t="s">
-        <v>207</v>
-      </c>
-      <c r="K82" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="83" spans="1:12">
@@ -3735,7 +3896,34 @@
         <v>24</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D83" t="s">
+        <v>75</v>
+      </c>
+      <c r="E83" t="s">
+        <v>50</v>
+      </c>
+      <c r="F83" t="s">
+        <v>199</v>
+      </c>
+      <c r="G83" t="s">
+        <v>149</v>
+      </c>
+      <c r="H83" t="s">
+        <v>203</v>
+      </c>
+      <c r="I83" t="s">
+        <v>275</v>
+      </c>
+      <c r="J83" t="s">
+        <v>206</v>
+      </c>
+      <c r="K83" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="84" spans="1:12">
@@ -3743,37 +3931,28 @@
         <v>24</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D84" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="E84" t="s">
         <v>50</v>
       </c>
-      <c r="F84" t="s">
-        <v>155</v>
-      </c>
-      <c r="G84" t="s">
-        <v>149</v>
-      </c>
       <c r="H84" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I84" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J84" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K84" t="s">
-        <v>221</v>
-      </c>
-      <c r="L84" t="s">
-        <v>318</v>
+        <v>220</v>
       </c>
     </row>
     <row r="85" spans="1:12">
@@ -3781,25 +3960,7 @@
         <v>24</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F85" t="s">
-        <v>156</v>
-      </c>
-      <c r="G85" t="s">
-        <v>149</v>
-      </c>
-      <c r="H85" t="s">
-        <v>204</v>
-      </c>
-      <c r="I85" t="s">
-        <v>279</v>
-      </c>
-      <c r="J85" t="s">
-        <v>207</v>
-      </c>
-      <c r="K85" t="s">
-        <v>221</v>
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:12">
@@ -3809,14 +3970,35 @@
       <c r="B86" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C86" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D86" t="s">
+        <v>72</v>
+      </c>
+      <c r="E86" t="s">
+        <v>50</v>
+      </c>
       <c r="F86" t="s">
-        <v>366</v>
+        <v>155</v>
       </c>
       <c r="G86" t="s">
         <v>149</v>
       </c>
       <c r="H86" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="I86" t="s">
+        <v>277</v>
+      </c>
+      <c r="J86" t="s">
+        <v>206</v>
+      </c>
+      <c r="K86" t="s">
+        <v>220</v>
+      </c>
+      <c r="L86" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -3824,37 +4006,25 @@
         <v>24</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D87" t="s">
-        <v>71</v>
-      </c>
-      <c r="E87" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F87" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G87" t="s">
         <v>149</v>
       </c>
       <c r="H87" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J87" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K87" t="s">
-        <v>221</v>
-      </c>
-      <c r="L87" t="s">
-        <v>337</v>
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -3862,34 +4032,16 @@
         <v>24</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C88" s="6">
-        <v>253</v>
-      </c>
-      <c r="D88" t="s">
-        <v>91</v>
-      </c>
-      <c r="E88" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F88" t="s">
-        <v>223</v>
+        <v>365</v>
       </c>
       <c r="G88" t="s">
         <v>149</v>
       </c>
       <c r="H88" t="s">
-        <v>204</v>
-      </c>
-      <c r="I88" t="s">
-        <v>281</v>
-      </c>
-      <c r="J88" t="s">
-        <v>207</v>
-      </c>
-      <c r="K88" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -3899,40 +4051,70 @@
       <c r="B89" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C89" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D89" t="s">
+        <v>71</v>
+      </c>
+      <c r="E89" t="s">
+        <v>50</v>
+      </c>
       <c r="F89" t="s">
-        <v>198</v>
+        <v>154</v>
       </c>
       <c r="G89" t="s">
         <v>149</v>
       </c>
+      <c r="H89" t="s">
+        <v>203</v>
+      </c>
+      <c r="I89" t="s">
+        <v>279</v>
+      </c>
+      <c r="J89" t="s">
+        <v>206</v>
+      </c>
+      <c r="K89" t="s">
+        <v>220</v>
+      </c>
+      <c r="L89" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>121</v>
+        <v>34</v>
+      </c>
+      <c r="C90" s="6">
+        <v>253</v>
       </c>
       <c r="D90" t="s">
-        <v>35</v>
+        <v>91</v>
       </c>
       <c r="E90" t="s">
         <v>50</v>
       </c>
+      <c r="F90" t="s">
+        <v>222</v>
+      </c>
+      <c r="G90" t="s">
+        <v>149</v>
+      </c>
       <c r="H90" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I90" t="s">
-        <v>35</v>
+        <v>280</v>
       </c>
       <c r="J90" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K90" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -3940,60 +4122,42 @@
         <v>24</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C91" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D91" t="s">
-        <v>90</v>
-      </c>
-      <c r="E91" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F91" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G91" t="s">
         <v>149</v>
       </c>
-      <c r="H91" t="s">
-        <v>204</v>
-      </c>
-      <c r="I91" t="s">
-        <v>283</v>
-      </c>
-      <c r="J91" t="s">
-        <v>207</v>
-      </c>
-      <c r="K91" t="s">
-        <v>216</v>
-      </c>
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F92" t="s">
-        <v>192</v>
-      </c>
-      <c r="G92" t="s">
-        <v>149</v>
+        <v>35</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D92" t="s">
+        <v>35</v>
+      </c>
+      <c r="E92" t="s">
+        <v>50</v>
       </c>
       <c r="H92" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I92" t="s">
-        <v>284</v>
+        <v>35</v>
       </c>
       <c r="J92" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K92" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
     </row>
     <row r="93" spans="1:12">
@@ -4003,14 +4167,32 @@
       <c r="B93" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="C93" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D93" t="s">
+        <v>90</v>
+      </c>
+      <c r="E93" t="s">
+        <v>50</v>
+      </c>
       <c r="F93" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G93" t="s">
         <v>149</v>
       </c>
       <c r="H93" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="I93" t="s">
+        <v>282</v>
+      </c>
+      <c r="J93" t="s">
+        <v>206</v>
+      </c>
+      <c r="K93" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -4018,25 +4200,25 @@
         <v>24</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C94" s="6">
-        <v>311</v>
-      </c>
-      <c r="D94" t="s">
-        <v>76</v>
-      </c>
-      <c r="E94" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="F94" t="s">
+        <v>192</v>
+      </c>
+      <c r="G94" t="s">
+        <v>149</v>
+      </c>
+      <c r="H94" t="s">
+        <v>203</v>
       </c>
       <c r="I94" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J94" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K94" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="95" spans="1:12">
@@ -4044,16 +4226,16 @@
         <v>24</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C95" s="6">
-        <v>312</v>
-      </c>
-      <c r="D95" t="s">
-        <v>136</v>
-      </c>
-      <c r="E95" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="F95" t="s">
+        <v>193</v>
+      </c>
+      <c r="G95" t="s">
+        <v>149</v>
+      </c>
+      <c r="H95" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:12">
@@ -4061,16 +4243,25 @@
         <v>24</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C96" s="6" t="s">
-        <v>308</v>
+        <v>37</v>
+      </c>
+      <c r="C96" s="6">
+        <v>311</v>
       </c>
       <c r="D96" t="s">
-        <v>307</v>
+        <v>76</v>
       </c>
       <c r="E96" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="I96" t="s">
+        <v>284</v>
+      </c>
+      <c r="J96" t="s">
+        <v>206</v>
+      </c>
+      <c r="K96" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="97" spans="1:12">
@@ -4078,34 +4269,16 @@
         <v>24</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>310</v>
+        <v>37</v>
+      </c>
+      <c r="C97" s="6">
+        <v>312</v>
       </c>
       <c r="D97" t="s">
-        <v>309</v>
+        <v>136</v>
       </c>
       <c r="E97" t="s">
-        <v>50</v>
-      </c>
-      <c r="F97" t="s">
-        <v>189</v>
-      </c>
-      <c r="G97" t="s">
-        <v>149</v>
-      </c>
-      <c r="H97" t="s">
-        <v>204</v>
-      </c>
-      <c r="I97" t="s">
-        <v>356</v>
-      </c>
-      <c r="J97" t="s">
-        <v>207</v>
-      </c>
-      <c r="K97" t="s">
-        <v>221</v>
+        <v>52</v>
       </c>
     </row>
     <row r="98" spans="1:12">
@@ -4113,83 +4286,71 @@
         <v>24</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="F98" t="s">
-        <v>347</v>
-      </c>
-      <c r="G98" t="s">
+        <v>306</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D98" t="s">
+        <v>306</v>
+      </c>
+      <c r="E98" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12">
+      <c r="A99" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D99" t="s">
+        <v>308</v>
+      </c>
+      <c r="E99" t="s">
+        <v>50</v>
+      </c>
+      <c r="F99" t="s">
+        <v>189</v>
+      </c>
+      <c r="G99" t="s">
         <v>149</v>
       </c>
-      <c r="H98" t="s">
-        <v>204</v>
-      </c>
-      <c r="L98" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12">
-      <c r="A99" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C99" s="6">
-        <v>511</v>
-      </c>
-      <c r="D99" t="s">
-        <v>82</v>
-      </c>
-      <c r="E99" t="s">
-        <v>51</v>
-      </c>
-      <c r="F99" t="s">
-        <v>182</v>
-      </c>
-      <c r="G99" t="s">
-        <v>187</v>
-      </c>
       <c r="H99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I99" t="s">
-        <v>286</v>
+        <v>355</v>
       </c>
       <c r="J99" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K99" t="s">
         <v>220</v>
       </c>
-      <c r="L99" t="s">
-        <v>316</v>
-      </c>
     </row>
     <row r="100" spans="1:12">
-      <c r="A100" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>39</v>
+      <c r="A100" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>347</v>
       </c>
       <c r="F100" t="s">
-        <v>180</v>
+        <v>346</v>
       </c>
       <c r="G100" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="H100" t="s">
-        <v>204</v>
-      </c>
-      <c r="I100" t="s">
-        <v>287</v>
-      </c>
-      <c r="J100" t="s">
-        <v>209</v>
-      </c>
-      <c r="K100" t="s">
-        <v>220</v>
+        <v>203</v>
+      </c>
+      <c r="L100" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="101" spans="1:12">
@@ -4200,31 +4361,34 @@
         <v>39</v>
       </c>
       <c r="C101" s="6">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D101" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E101" t="s">
         <v>51</v>
       </c>
       <c r="F101" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="G101" t="s">
         <v>187</v>
       </c>
       <c r="H101" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I101" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="J101" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K101" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="L101" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="102" spans="1:12">
@@ -4235,22 +4399,22 @@
         <v>39</v>
       </c>
       <c r="F102" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G102" t="s">
         <v>187</v>
       </c>
       <c r="H102" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I102" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J102" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K102" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="103" spans="1:12">
@@ -4260,23 +4424,32 @@
       <c r="B103" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C103" s="6">
+        <v>513</v>
+      </c>
+      <c r="D103" t="s">
+        <v>83</v>
+      </c>
+      <c r="E103" t="s">
+        <v>51</v>
+      </c>
       <c r="F103" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="G103" t="s">
         <v>187</v>
       </c>
       <c r="H103" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I103" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J103" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K103" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="104" spans="1:12">
@@ -4287,25 +4460,25 @@
         <v>39</v>
       </c>
       <c r="F104" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="G104" t="s">
         <v>187</v>
       </c>
       <c r="H104" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I104" t="s">
-        <v>39</v>
+        <v>288</v>
       </c>
       <c r="J104" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K104" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="105" spans="1:12" ht="17" customHeight="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12">
       <c r="A105" s="4" t="s">
         <v>38</v>
       </c>
@@ -4313,42 +4486,48 @@
         <v>39</v>
       </c>
       <c r="F105" t="s">
-        <v>360</v>
+        <v>38</v>
       </c>
       <c r="G105" t="s">
         <v>187</v>
       </c>
       <c r="H105" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I105" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J105" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K105" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="106" spans="1:12" ht="17" customHeight="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12">
       <c r="A106" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B106" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F106" t="s">
+        <v>183</v>
+      </c>
+      <c r="G106" t="s">
+        <v>187</v>
+      </c>
       <c r="H106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I106" t="s">
-        <v>292</v>
+        <v>39</v>
       </c>
       <c r="J106" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K106" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="17" customHeight="1">
@@ -4358,17 +4537,23 @@
       <c r="B107" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F107" t="s">
+        <v>359</v>
+      </c>
+      <c r="G107" t="s">
+        <v>187</v>
+      </c>
       <c r="H107" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I107" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J107" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="17" customHeight="1">
@@ -4379,16 +4564,16 @@
         <v>39</v>
       </c>
       <c r="H108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I108" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J108" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K108" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="17" customHeight="1">
@@ -4398,23 +4583,17 @@
       <c r="B109" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F109" t="s">
-        <v>181</v>
-      </c>
-      <c r="G109" t="s">
-        <v>187</v>
-      </c>
       <c r="H109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I109" t="s">
-        <v>215</v>
+        <v>292</v>
       </c>
       <c r="J109" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K109" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="17" customHeight="1">
@@ -4424,23 +4603,17 @@
       <c r="B110" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F110" t="s">
-        <v>185</v>
-      </c>
-      <c r="G110" t="s">
-        <v>187</v>
-      </c>
       <c r="H110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I110" t="s">
-        <v>215</v>
+        <v>293</v>
       </c>
       <c r="J110" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K110" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="17" customHeight="1">
@@ -4450,69 +4623,69 @@
       <c r="B111" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F111" t="s">
+        <v>181</v>
+      </c>
+      <c r="G111" t="s">
+        <v>187</v>
+      </c>
       <c r="H111" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I111" t="s">
-        <v>295</v>
+        <v>214</v>
       </c>
       <c r="J111" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K111" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="112" spans="1:12">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="17" customHeight="1">
       <c r="A112" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F112" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="G112" t="s">
         <v>187</v>
       </c>
       <c r="H112" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I112" t="s">
-        <v>296</v>
+        <v>214</v>
       </c>
       <c r="J112" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K112" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="17" customHeight="1">
       <c r="A113" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F113" t="s">
-        <v>365</v>
-      </c>
-      <c r="G113" t="s">
-        <v>187</v>
+        <v>39</v>
       </c>
       <c r="H113" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I113" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J113" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K113" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="114" spans="1:11">
@@ -4522,17 +4695,23 @@
       <c r="B114" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="F114" t="s">
+        <v>176</v>
+      </c>
+      <c r="G114" t="s">
+        <v>187</v>
+      </c>
       <c r="H114" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I114" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="J114" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K114" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:11">
@@ -4540,25 +4719,25 @@
         <v>38</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F115" t="s">
-        <v>179</v>
+        <v>364</v>
       </c>
       <c r="G115" t="s">
         <v>187</v>
       </c>
       <c r="H115" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I115" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="J115" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K115" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="116" spans="1:11">
@@ -4566,22 +4745,19 @@
         <v>38</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F116" t="s">
-        <v>363</v>
+        <v>40</v>
       </c>
       <c r="H116" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I116" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="J116" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K116" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="117" spans="1:11">
@@ -4589,25 +4765,25 @@
         <v>38</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F117" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="G117" t="s">
         <v>187</v>
       </c>
       <c r="H117" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I117" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="J117" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K117" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:11">
@@ -4615,19 +4791,22 @@
         <v>38</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F118" t="s">
+        <v>362</v>
       </c>
       <c r="H118" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I118" t="s">
-        <v>42</v>
+        <v>299</v>
       </c>
       <c r="J118" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K118" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="119" spans="1:11">
@@ -4637,17 +4816,23 @@
       <c r="B119" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="F119" t="s">
+        <v>175</v>
+      </c>
+      <c r="G119" t="s">
+        <v>187</v>
+      </c>
       <c r="H119" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I119" t="s">
-        <v>214</v>
+        <v>300</v>
       </c>
       <c r="J119" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K119" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" spans="1:11">
@@ -4658,16 +4843,16 @@
         <v>42</v>
       </c>
       <c r="H120" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I120" t="s">
-        <v>302</v>
+        <v>42</v>
       </c>
       <c r="J120" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K120" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:11">
@@ -4675,25 +4860,19 @@
         <v>38</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F121" t="s">
-        <v>186</v>
-      </c>
-      <c r="G121" t="s">
-        <v>187</v>
+        <v>42</v>
       </c>
       <c r="H121" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I121" t="s">
-        <v>303</v>
+        <v>213</v>
       </c>
       <c r="J121" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K121" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" spans="1:11">
@@ -4701,59 +4880,62 @@
         <v>38</v>
       </c>
       <c r="B122" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H122" t="s">
+        <v>203</v>
+      </c>
+      <c r="I122" t="s">
+        <v>301</v>
+      </c>
+      <c r="J122" t="s">
+        <v>208</v>
+      </c>
+      <c r="K122" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="A123" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F122" t="s">
+      <c r="F123" t="s">
+        <v>186</v>
+      </c>
+      <c r="G123" t="s">
+        <v>187</v>
+      </c>
+      <c r="H123" t="s">
+        <v>203</v>
+      </c>
+      <c r="I123" t="s">
+        <v>302</v>
+      </c>
+      <c r="J123" t="s">
+        <v>208</v>
+      </c>
+      <c r="K123" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F124" t="s">
         <v>184</v>
       </c>
-      <c r="G122" t="s">
+      <c r="G124" t="s">
         <v>187</v>
       </c>
-      <c r="H122" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11">
-      <c r="A123" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B123" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E123" t="s">
-        <v>53</v>
-      </c>
-      <c r="H123" t="s">
-        <v>203</v>
-      </c>
-      <c r="I123" t="s">
-        <v>304</v>
-      </c>
-      <c r="J123" t="s">
-        <v>212</v>
-      </c>
-      <c r="K123" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11">
-      <c r="A124" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="H124" t="s">
         <v>203</v>
-      </c>
-      <c r="I124" t="s">
-        <v>211</v>
-      </c>
-      <c r="J124" t="s">
-        <v>212</v>
-      </c>
-      <c r="K124" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="125" spans="1:11">
@@ -4761,34 +4943,22 @@
         <v>44</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="D125" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E125" t="s">
         <v>53</v>
       </c>
-      <c r="F125" t="s">
-        <v>162</v>
-      </c>
-      <c r="G125" t="s">
-        <v>174</v>
-      </c>
       <c r="H125" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I125" t="s">
-        <v>46</v>
+        <v>303</v>
       </c>
       <c r="J125" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K125" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="126" spans="1:11">
@@ -4796,28 +4966,19 @@
         <v>44</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C126" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D126" t="s">
-        <v>92</v>
-      </c>
-      <c r="E126" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H126" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I126" t="s">
-        <v>305</v>
+        <v>210</v>
       </c>
       <c r="J126" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K126" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="1:11">
@@ -4825,28 +4986,92 @@
         <v>44</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D127" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E127" t="s">
         <v>53</v>
       </c>
+      <c r="F127" t="s">
+        <v>162</v>
+      </c>
+      <c r="G127" t="s">
+        <v>174</v>
+      </c>
       <c r="H127" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I127" t="s">
-        <v>306</v>
+        <v>46</v>
       </c>
       <c r="J127" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K127" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D128" t="s">
+        <v>92</v>
+      </c>
+      <c r="E128" t="s">
+        <v>53</v>
+      </c>
+      <c r="H128" t="s">
+        <v>202</v>
+      </c>
+      <c r="I128" t="s">
+        <v>304</v>
+      </c>
+      <c r="J128" t="s">
+        <v>211</v>
+      </c>
+      <c r="K128" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D129" t="s">
+        <v>48</v>
+      </c>
+      <c r="E129" t="s">
+        <v>53</v>
+      </c>
+      <c r="H129" t="s">
+        <v>202</v>
+      </c>
+      <c r="I129" t="s">
+        <v>305</v>
+      </c>
+      <c r="J129" t="s">
+        <v>211</v>
+      </c>
+      <c r="K129" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update and remove duplicates in the index
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chila\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422374E1-2279-4D82-A0F6-C8AAFCB89CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88517E2-FB1F-4B02-8DA0-4F33C0FF0A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20625" yWindow="-16245" windowWidth="14610" windowHeight="15585" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="6225" yWindow="-16245" windowWidth="14610" windowHeight="15585" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1103" uniqueCount="424">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1767,7 +1767,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -3691,9 +3691,6 @@
       <c r="H66" t="s">
         <v>203</v>
       </c>
-      <c r="I66" t="s">
-        <v>248</v>
-      </c>
       <c r="J66" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
update the combine member census logic and bug fix
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chila\Downloads\RawClaimMCR-main\RawClaimMCR-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/RawClaimMCR-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34622ACD-76D0-4C90-A9DF-AB705697C94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78DEE0D9-CF9B-9B41-871F-C249095BE52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="-16245" windowWidth="14610" windowHeight="15585" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="20060" yWindow="-20980" windowWidth="38400" windowHeight="20980" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="517">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1472,15 +1472,6 @@
     <t>HOMECA</t>
   </si>
   <si>
-    <t>Surgeon Fee - Non Classified (AXA)</t>
-  </si>
-  <si>
-    <t>Anaesthetist's Fees - Non Classified (AXA)</t>
-  </si>
-  <si>
-    <t>Operation Theatre Fees - Non Classified (AXA)</t>
-  </si>
-  <si>
     <t>SP Virtual Consult - DoctorNow+MyDoc+UMP</t>
   </si>
   <si>
@@ -1530,6 +1521,72 @@
   </si>
   <si>
     <t>SURAPP</t>
+  </si>
+  <si>
+    <t>chinese-medicine-practitioner</t>
+  </si>
+  <si>
+    <t>general-practitioner</t>
+  </si>
+  <si>
+    <t>hospital-cash</t>
+  </si>
+  <si>
+    <t>room-and-board</t>
+  </si>
+  <si>
+    <t>specialist</t>
+  </si>
+  <si>
+    <t>miscellaneous-charges</t>
+  </si>
+  <si>
+    <t>physiotherapist-chiropractor</t>
+  </si>
+  <si>
+    <t>Physio (PT) or Chiro (CT)</t>
+  </si>
+  <si>
+    <t>diagnostic-imaging-and-laboratory-tests</t>
+  </si>
+  <si>
+    <t>anaesthetists-fee</t>
+  </si>
+  <si>
+    <t>Anaesthetist's Fees - Non Classified (AXA/ Sunlife)</t>
+  </si>
+  <si>
+    <t>Surgeon Fee - Non Classified (AXA/ Sunlife)</t>
+  </si>
+  <si>
+    <t>Operation Theatre Fees - Non Classified (AXA/ Sunlife)</t>
+  </si>
+  <si>
+    <t>day-case-procedure-cash-benefit</t>
+  </si>
+  <si>
+    <t>operating-theatre-charges</t>
+  </si>
+  <si>
+    <t>surgeons-fee</t>
+  </si>
+  <si>
+    <t>routine-health-check-up</t>
+  </si>
+  <si>
+    <t>physicians-visit</t>
+  </si>
+  <si>
+    <t>Post Hosp Cinic Consultation</t>
+  </si>
+  <si>
+    <t>post-confinement-outpatient-care</t>
+  </si>
+  <si>
+    <t>Pre Hosp Cinic Consultation</t>
+  </si>
+  <si>
+    <t>hospital-income-benefit</t>
   </si>
 </sst>
 </file>
@@ -1964,28 +2021,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:O159"/>
+  <dimension ref="A1:O163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="Q44" sqref="Q44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.08203125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="22.83203125" style="6" customWidth="1"/>
     <col min="4" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.83203125" customWidth="1"/>
-    <col min="9" max="9" width="39.58203125" customWidth="1"/>
+    <col min="9" max="9" width="39.5" customWidth="1"/>
     <col min="12" max="12" width="48.1640625" customWidth="1"/>
     <col min="13" max="13" width="25.1640625" customWidth="1"/>
-    <col min="14" max="14" width="44.58203125" customWidth="1"/>
+    <col min="14" max="14" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -2110,6 +2167,9 @@
       <c r="L3" t="s">
         <v>326</v>
       </c>
+      <c r="O3" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
@@ -2183,6 +2243,9 @@
       <c r="K5" t="s">
         <v>216</v>
       </c>
+      <c r="O5" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
@@ -2240,7 +2303,7 @@
       </c>
       <c r="C7" s="7"/>
       <c r="F7" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="G7" t="s">
         <v>174</v>
@@ -2259,6 +2322,9 @@
       </c>
       <c r="L7" t="s">
         <v>327</v>
+      </c>
+      <c r="O7" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2558,7 +2624,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>478</v>
+        <v>506</v>
       </c>
       <c r="F20" t="s">
         <v>158</v>
@@ -2575,19 +2641,10 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" t="s">
-        <v>88</v>
-      </c>
-      <c r="E21" t="s">
-        <v>49</v>
-      </c>
-      <c r="M21" t="s">
-        <v>387</v>
+        <v>506</v>
+      </c>
+      <c r="O21" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2595,34 +2652,19 @@
         <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="E22" t="s">
         <v>49</v>
       </c>
-      <c r="H22" t="s">
-        <v>201</v>
-      </c>
-      <c r="I22" t="s">
-        <v>237</v>
-      </c>
-      <c r="J22" t="s">
-        <v>204</v>
-      </c>
-      <c r="K22" t="s">
-        <v>216</v>
-      </c>
-      <c r="L22" t="s">
-        <v>341</v>
-      </c>
       <c r="M22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2630,13 +2672,13 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="s">
         <v>49</v>
@@ -2645,7 +2687,7 @@
         <v>201</v>
       </c>
       <c r="I23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J23" t="s">
         <v>204</v>
@@ -2654,10 +2696,10 @@
         <v>216</v>
       </c>
       <c r="L23" t="s">
-        <v>324</v>
+        <v>341</v>
       </c>
       <c r="M23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2665,13 +2707,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E24" t="s">
         <v>49</v>
@@ -2680,7 +2722,7 @@
         <v>201</v>
       </c>
       <c r="I24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J24" t="s">
         <v>204</v>
@@ -2689,13 +2731,10 @@
         <v>216</v>
       </c>
       <c r="L24" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="M24" t="s">
-        <v>390</v>
-      </c>
-      <c r="N24" s="10" t="s">
-        <v>431</v>
+        <v>389</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -2703,17 +2742,37 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>479</v>
-      </c>
-      <c r="F25" t="s">
-        <v>159</v>
-      </c>
-      <c r="G25" t="s">
-        <v>174</v>
-      </c>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10" t="s">
-        <v>445</v>
+        <v>10</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" t="s">
+        <v>201</v>
+      </c>
+      <c r="I25" t="s">
+        <v>239</v>
+      </c>
+      <c r="J25" t="s">
+        <v>204</v>
+      </c>
+      <c r="K25" t="s">
+        <v>216</v>
+      </c>
+      <c r="L25" t="s">
+        <v>338</v>
+      </c>
+      <c r="M25" t="s">
+        <v>390</v>
+      </c>
+      <c r="N25" s="10" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="26" spans="1:15">
@@ -2721,16 +2780,17 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" t="s">
-        <v>49</v>
+        <v>505</v>
+      </c>
+      <c r="F26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" t="s">
+        <v>174</v>
+      </c>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -2738,54 +2798,28 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D27" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" t="s">
-        <v>49</v>
-      </c>
-      <c r="H27" t="s">
-        <v>201</v>
-      </c>
-      <c r="I27" t="s">
-        <v>240</v>
-      </c>
-      <c r="J27" t="s">
-        <v>204</v>
-      </c>
-      <c r="K27" t="s">
-        <v>216</v>
-      </c>
-      <c r="L27" t="s">
-        <v>334</v>
-      </c>
-      <c r="M27" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15">
+        <v>505</v>
+      </c>
+      <c r="N27" s="10"/>
+      <c r="O27" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="17" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="s">
-        <v>201</v>
-      </c>
-      <c r="I28" t="s">
-        <v>241</v>
-      </c>
-      <c r="J28" t="s">
-        <v>204</v>
-      </c>
-      <c r="K28" t="s">
-        <v>216</v>
+        <v>11</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2793,13 +2827,13 @@
         <v>23</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
         <v>49</v>
@@ -2808,7 +2842,7 @@
         <v>201</v>
       </c>
       <c r="I29" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J29" t="s">
         <v>204</v>
@@ -2817,10 +2851,10 @@
         <v>216</v>
       </c>
       <c r="L29" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="M29" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2828,13 +2862,13 @@
         <v>23</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
         <v>201</v>
       </c>
       <c r="I30" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J30" t="s">
         <v>204</v>
@@ -2848,13 +2882,13 @@
         <v>23</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E31" t="s">
         <v>49</v>
@@ -2863,7 +2897,7 @@
         <v>201</v>
       </c>
       <c r="I31" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J31" t="s">
         <v>204</v>
@@ -2872,13 +2906,10 @@
         <v>216</v>
       </c>
       <c r="L31" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="M31" t="s">
-        <v>397</v>
-      </c>
-      <c r="N31" s="10" t="s">
-        <v>429</v>
+        <v>395</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2886,13 +2917,13 @@
         <v>23</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H32" t="s">
         <v>201</v>
       </c>
       <c r="I32" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J32" t="s">
         <v>204</v>
@@ -2906,16 +2937,37 @@
         <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="F33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" t="s">
-        <v>174</v>
-      </c>
-      <c r="O33" s="10" t="s">
-        <v>442</v>
+        <v>14</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" t="s">
+        <v>201</v>
+      </c>
+      <c r="I33" t="s">
+        <v>244</v>
+      </c>
+      <c r="J33" t="s">
+        <v>204</v>
+      </c>
+      <c r="K33" t="s">
+        <v>216</v>
+      </c>
+      <c r="L33" t="s">
+        <v>339</v>
+      </c>
+      <c r="M33" t="s">
+        <v>397</v>
+      </c>
+      <c r="N33" s="10" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:15">
@@ -2923,40 +2975,19 @@
         <v>23</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D34" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" t="s">
-        <v>49</v>
-      </c>
-      <c r="F34" t="s">
-        <v>168</v>
-      </c>
-      <c r="G34" t="s">
-        <v>174</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s">
         <v>201</v>
       </c>
       <c r="I34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J34" t="s">
         <v>204</v>
       </c>
       <c r="K34" t="s">
         <v>216</v>
-      </c>
-      <c r="L34" t="s">
-        <v>342</v>
-      </c>
-      <c r="M34" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="35" spans="1:15">
@@ -2964,25 +2995,16 @@
         <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>507</v>
       </c>
       <c r="F35" t="s">
-        <v>349</v>
+        <v>160</v>
       </c>
       <c r="G35" t="s">
         <v>174</v>
       </c>
-      <c r="H35" t="s">
-        <v>201</v>
-      </c>
-      <c r="I35" t="s">
-        <v>247</v>
-      </c>
-      <c r="J35" t="s">
-        <v>204</v>
-      </c>
-      <c r="K35" t="s">
-        <v>216</v>
+      <c r="O35" s="10" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2990,25 +3012,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>467</v>
-      </c>
-      <c r="D36" t="s">
-        <v>466</v>
-      </c>
-      <c r="E36" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" t="s">
-        <v>165</v>
-      </c>
-      <c r="G36" t="s">
-        <v>174</v>
-      </c>
-      <c r="L36" t="s">
-        <v>344</v>
+        <v>507</v>
+      </c>
+      <c r="O36" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -3016,19 +3023,19 @@
         <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="E37" t="s">
         <v>49</v>
       </c>
       <c r="F37" t="s">
-        <v>357</v>
+        <v>168</v>
       </c>
       <c r="G37" t="s">
         <v>174</v>
@@ -3037,13 +3044,19 @@
         <v>201</v>
       </c>
       <c r="I37" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J37" t="s">
         <v>204</v>
       </c>
       <c r="K37" t="s">
         <v>216</v>
+      </c>
+      <c r="L37" t="s">
+        <v>342</v>
+      </c>
+      <c r="M37" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -3051,17 +3064,25 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="7"/>
+        <v>15</v>
+      </c>
       <c r="F38" t="s">
-        <v>477</v>
+        <v>349</v>
       </c>
       <c r="G38" t="s">
         <v>174</v>
       </c>
       <c r="H38" t="s">
         <v>201</v>
+      </c>
+      <c r="I38" t="s">
+        <v>247</v>
+      </c>
+      <c r="J38" t="s">
+        <v>204</v>
+      </c>
+      <c r="K38" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -3069,34 +3090,25 @@
         <v>23</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>130</v>
+        <v>16</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>467</v>
       </c>
       <c r="D39" t="s">
-        <v>131</v>
+        <v>466</v>
       </c>
       <c r="E39" t="s">
         <v>49</v>
       </c>
       <c r="F39" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="G39" t="s">
         <v>174</v>
       </c>
-      <c r="H39" t="s">
-        <v>201</v>
-      </c>
-      <c r="I39" t="s">
-        <v>228</v>
-      </c>
-      <c r="J39" t="s">
-        <v>204</v>
-      </c>
-      <c r="K39" t="s">
-        <v>216</v>
+      <c r="L39" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -3104,14 +3116,28 @@
         <v>23</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C40" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F40" t="s">
+        <v>357</v>
+      </c>
+      <c r="G40" t="s">
+        <v>174</v>
+      </c>
       <c r="H40" t="s">
         <v>201</v>
       </c>
       <c r="I40" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="J40" t="s">
         <v>204</v>
@@ -3125,23 +3151,17 @@
         <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>369</v>
+        <v>18</v>
       </c>
       <c r="C41" s="7"/>
+      <c r="F41" t="s">
+        <v>477</v>
+      </c>
+      <c r="G41" t="s">
+        <v>174</v>
+      </c>
       <c r="H41" t="s">
         <v>201</v>
-      </c>
-      <c r="I41" t="s">
-        <v>226</v>
-      </c>
-      <c r="J41" t="s">
-        <v>204</v>
-      </c>
-      <c r="K41" t="s">
-        <v>216</v>
-      </c>
-      <c r="M41" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -3149,23 +3169,22 @@
         <v>23</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="H42" t="s">
-        <v>201</v>
-      </c>
-      <c r="I42" t="s">
-        <v>227</v>
-      </c>
-      <c r="J42" t="s">
-        <v>204</v>
-      </c>
-      <c r="K42" t="s">
-        <v>216</v>
-      </c>
-      <c r="M42" t="s">
-        <v>400</v>
+        <v>368</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" t="s">
+        <v>173</v>
+      </c>
+      <c r="G42" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -3173,23 +3192,20 @@
         <v>23</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>369</v>
+        <v>515</v>
       </c>
       <c r="C43" s="7"/>
       <c r="H43" t="s">
         <v>201</v>
       </c>
       <c r="I43" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J43" t="s">
         <v>204</v>
       </c>
       <c r="K43" t="s">
         <v>216</v>
-      </c>
-      <c r="M43" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -3197,28 +3213,14 @@
         <v>23</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="6">
-        <v>210</v>
-      </c>
-      <c r="D44" t="s">
-        <v>84</v>
-      </c>
-      <c r="E44" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" t="s">
-        <v>166</v>
-      </c>
-      <c r="G44" t="s">
-        <v>174</v>
-      </c>
+        <v>513</v>
+      </c>
+      <c r="C44" s="7"/>
       <c r="H44" t="s">
         <v>201</v>
       </c>
       <c r="I44" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="J44" t="s">
         <v>204</v>
@@ -3226,14 +3228,8 @@
       <c r="K44" t="s">
         <v>216</v>
       </c>
-      <c r="L44" t="s">
-        <v>318</v>
-      </c>
-      <c r="M44" t="s">
-        <v>391</v>
-      </c>
-      <c r="N44" s="10" t="s">
-        <v>251</v>
+      <c r="O44" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -3241,28 +3237,14 @@
         <v>23</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" s="6">
-        <v>220</v>
-      </c>
-      <c r="D45" t="s">
-        <v>135</v>
-      </c>
-      <c r="E45" t="s">
-        <v>49</v>
-      </c>
-      <c r="F45" t="s">
-        <v>171</v>
-      </c>
-      <c r="G45" t="s">
-        <v>174</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="C45" s="7"/>
       <c r="H45" t="s">
         <v>201</v>
       </c>
       <c r="I45" t="s">
-        <v>250</v>
+        <v>226</v>
       </c>
       <c r="J45" t="s">
         <v>204</v>
@@ -3270,11 +3252,8 @@
       <c r="K45" t="s">
         <v>216</v>
       </c>
-      <c r="L45" t="s">
-        <v>336</v>
-      </c>
       <c r="M45" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -3282,25 +3261,23 @@
         <v>23</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" t="s">
-        <v>360</v>
-      </c>
-      <c r="G46" t="s">
-        <v>174</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="C46" s="7"/>
       <c r="H46" t="s">
         <v>201</v>
       </c>
       <c r="I46" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="J46" t="s">
         <v>204</v>
       </c>
       <c r="K46" t="s">
         <v>216</v>
+      </c>
+      <c r="M46" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -3308,19 +3285,23 @@
         <v>23</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>369</v>
+      </c>
+      <c r="C47" s="7"/>
       <c r="H47" t="s">
         <v>201</v>
       </c>
       <c r="I47" t="s">
-        <v>422</v>
+        <v>229</v>
       </c>
       <c r="J47" t="s">
         <v>204</v>
       </c>
       <c r="K47" t="s">
         <v>216</v>
+      </c>
+      <c r="M47" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -3328,19 +3309,19 @@
         <v>23</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C48" s="6">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="D48" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="E48" t="s">
         <v>49</v>
       </c>
       <c r="F48" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="G48" t="s">
         <v>174</v>
@@ -3349,7 +3330,7 @@
         <v>201</v>
       </c>
       <c r="I48" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J48" t="s">
         <v>204</v>
@@ -3358,10 +3339,16 @@
         <v>216</v>
       </c>
       <c r="L48" t="s">
-        <v>343</v>
+        <v>318</v>
       </c>
       <c r="M48" t="s">
-        <v>393</v>
+        <v>391</v>
+      </c>
+      <c r="N48" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="O48" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="49" spans="1:15">
@@ -3369,13 +3356,40 @@
         <v>23</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="C49" s="6">
+        <v>220</v>
+      </c>
+      <c r="D49" t="s">
+        <v>135</v>
+      </c>
+      <c r="E49" t="s">
+        <v>49</v>
       </c>
       <c r="F49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G49" t="s">
         <v>174</v>
+      </c>
+      <c r="H49" t="s">
+        <v>201</v>
+      </c>
+      <c r="I49" t="s">
+        <v>250</v>
+      </c>
+      <c r="J49" t="s">
+        <v>204</v>
+      </c>
+      <c r="K49" t="s">
+        <v>216</v>
+      </c>
+      <c r="L49" t="s">
+        <v>336</v>
+      </c>
+      <c r="M49" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="50" spans="1:15">
@@ -3383,13 +3397,25 @@
         <v>23</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="L50" t="s">
-        <v>336</v>
-      </c>
-      <c r="M50" t="s">
-        <v>410</v>
+        <v>19</v>
+      </c>
+      <c r="F50" t="s">
+        <v>360</v>
+      </c>
+      <c r="G50" t="s">
+        <v>174</v>
+      </c>
+      <c r="H50" t="s">
+        <v>201</v>
+      </c>
+      <c r="I50" t="s">
+        <v>251</v>
+      </c>
+      <c r="J50" t="s">
+        <v>204</v>
+      </c>
+      <c r="K50" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="51" spans="1:15">
@@ -3397,7 +3423,19 @@
         <v>23</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="H51" t="s">
+        <v>201</v>
+      </c>
+      <c r="I51" t="s">
+        <v>422</v>
+      </c>
+      <c r="J51" t="s">
+        <v>204</v>
+      </c>
+      <c r="K51" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -3405,176 +3443,140 @@
         <v>23</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>128</v>
+        <v>20</v>
+      </c>
+      <c r="C52" s="6">
+        <v>230</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E52" t="s">
         <v>49</v>
       </c>
+      <c r="F52" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" t="s">
+        <v>174</v>
+      </c>
+      <c r="H52" t="s">
+        <v>201</v>
+      </c>
+      <c r="I52" t="s">
+        <v>252</v>
+      </c>
+      <c r="J52" t="s">
+        <v>204</v>
+      </c>
+      <c r="K52" t="s">
+        <v>216</v>
+      </c>
+      <c r="L52" t="s">
+        <v>343</v>
+      </c>
+      <c r="M52" t="s">
+        <v>393</v>
+      </c>
+      <c r="O52" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="53" spans="1:15">
-      <c r="A53" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D53" t="s">
-        <v>66</v>
-      </c>
-      <c r="E53" t="s">
-        <v>49</v>
+      <c r="A53" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F53" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G53" t="s">
         <v>174</v>
       </c>
-      <c r="H53" t="s">
+    </row>
+    <row r="54" spans="1:15">
+      <c r="A54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="L54" t="s">
+        <v>336</v>
+      </c>
+      <c r="M54" t="s">
+        <v>410</v>
+      </c>
+      <c r="O54" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
+      <c r="A55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
+      <c r="A56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D56" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
+      <c r="A57" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57" t="s">
+        <v>49</v>
+      </c>
+      <c r="F57" t="s">
+        <v>169</v>
+      </c>
+      <c r="G57" t="s">
+        <v>174</v>
+      </c>
+      <c r="H57" t="s">
         <v>201</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I57" t="s">
         <v>253</v>
       </c>
-      <c r="J53" t="s">
+      <c r="J57" t="s">
         <v>208</v>
       </c>
-      <c r="K53" t="s">
+      <c r="K57" t="s">
         <v>217</v>
       </c>
-      <c r="L53" t="s">
+      <c r="L57" t="s">
         <v>330</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M57" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15">
-      <c r="A54" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D54" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" t="s">
-        <v>144</v>
-      </c>
-      <c r="G54" t="s">
-        <v>149</v>
-      </c>
-      <c r="H54" t="s">
-        <v>202</v>
-      </c>
-      <c r="I54" t="s">
-        <v>254</v>
-      </c>
-      <c r="J54" t="s">
-        <v>205</v>
-      </c>
-      <c r="K54" t="s">
-        <v>219</v>
-      </c>
-      <c r="L54" t="s">
-        <v>313</v>
-      </c>
-      <c r="M54" t="s">
-        <v>380</v>
-      </c>
-      <c r="N54" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="O54" s="10" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15">
-      <c r="A55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F55" t="s">
-        <v>145</v>
-      </c>
-      <c r="G55" t="s">
-        <v>149</v>
-      </c>
-      <c r="H55" t="s">
-        <v>202</v>
-      </c>
-      <c r="I55" t="s">
-        <v>255</v>
-      </c>
-      <c r="J55" t="s">
-        <v>205</v>
-      </c>
-      <c r="K55" t="s">
-        <v>219</v>
-      </c>
-      <c r="L55" t="s">
-        <v>451</v>
-      </c>
-      <c r="M55" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15">
-      <c r="A56" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H56" t="s">
-        <v>202</v>
-      </c>
-      <c r="I56" t="s">
-        <v>256</v>
-      </c>
-      <c r="J56" t="s">
-        <v>205</v>
-      </c>
-      <c r="K56" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15">
-      <c r="A57" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" t="s">
-        <v>202</v>
-      </c>
-      <c r="I57" t="s">
-        <v>257</v>
-      </c>
-      <c r="J57" t="s">
-        <v>205</v>
-      </c>
-      <c r="K57" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:15">
@@ -3584,11 +3586,26 @@
       <c r="B58" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C58" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D58" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" t="s">
+        <v>144</v>
+      </c>
+      <c r="G58" t="s">
+        <v>149</v>
+      </c>
       <c r="H58" t="s">
         <v>202</v>
       </c>
       <c r="I58" t="s">
-        <v>351</v>
+        <v>254</v>
       </c>
       <c r="J58" t="s">
         <v>205</v>
@@ -3596,6 +3613,18 @@
       <c r="K58" t="s">
         <v>219</v>
       </c>
+      <c r="L58" t="s">
+        <v>313</v>
+      </c>
+      <c r="M58" t="s">
+        <v>380</v>
+      </c>
+      <c r="N58" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="O58" s="10" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59" s="3" t="s">
@@ -3604,11 +3633,17 @@
       <c r="B59" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F59" t="s">
+        <v>145</v>
+      </c>
+      <c r="G59" t="s">
+        <v>149</v>
+      </c>
       <c r="H59" t="s">
         <v>202</v>
       </c>
       <c r="I59" t="s">
-        <v>352</v>
+        <v>255</v>
       </c>
       <c r="J59" t="s">
         <v>205</v>
@@ -3616,6 +3651,15 @@
       <c r="K59" t="s">
         <v>219</v>
       </c>
+      <c r="L59" t="s">
+        <v>451</v>
+      </c>
+      <c r="M59" t="s">
+        <v>385</v>
+      </c>
+      <c r="O59" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="60" spans="1:15">
       <c r="A60" s="3" t="s">
@@ -3628,7 +3672,7 @@
         <v>202</v>
       </c>
       <c r="I60" t="s">
-        <v>355</v>
+        <v>256</v>
       </c>
       <c r="J60" t="s">
         <v>205</v>
@@ -3648,7 +3692,7 @@
         <v>202</v>
       </c>
       <c r="I61" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J61" t="s">
         <v>205</v>
@@ -3668,7 +3712,7 @@
         <v>202</v>
       </c>
       <c r="I62" t="s">
-        <v>259</v>
+        <v>351</v>
       </c>
       <c r="J62" t="s">
         <v>205</v>
@@ -3688,7 +3732,7 @@
         <v>202</v>
       </c>
       <c r="I63" t="s">
-        <v>414</v>
+        <v>352</v>
       </c>
       <c r="J63" t="s">
         <v>205</v>
@@ -3708,7 +3752,7 @@
         <v>202</v>
       </c>
       <c r="I64" t="s">
-        <v>415</v>
+        <v>355</v>
       </c>
       <c r="J64" t="s">
         <v>205</v>
@@ -3728,7 +3772,7 @@
         <v>202</v>
       </c>
       <c r="I65" t="s">
-        <v>417</v>
+        <v>258</v>
       </c>
       <c r="J65" t="s">
         <v>205</v>
@@ -3748,7 +3792,7 @@
         <v>202</v>
       </c>
       <c r="I66" t="s">
-        <v>416</v>
+        <v>259</v>
       </c>
       <c r="J66" t="s">
         <v>205</v>
@@ -3764,8 +3808,11 @@
       <c r="B67" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H67" t="s">
+        <v>202</v>
+      </c>
       <c r="I67" t="s">
-        <v>487</v>
+        <v>414</v>
       </c>
       <c r="J67" t="s">
         <v>205</v>
@@ -3781,8 +3828,11 @@
       <c r="B68" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H68" t="s">
+        <v>202</v>
+      </c>
       <c r="I68" t="s">
-        <v>488</v>
+        <v>415</v>
       </c>
       <c r="J68" t="s">
         <v>205</v>
@@ -3802,7 +3852,7 @@
         <v>202</v>
       </c>
       <c r="I69" t="s">
-        <v>483</v>
+        <v>417</v>
       </c>
       <c r="J69" t="s">
         <v>205</v>
@@ -3822,7 +3872,7 @@
         <v>202</v>
       </c>
       <c r="I70" t="s">
-        <v>350</v>
+        <v>416</v>
       </c>
       <c r="J70" t="s">
         <v>205</v>
@@ -3838,11 +3888,8 @@
       <c r="B71" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H71" t="s">
-        <v>202</v>
-      </c>
       <c r="I71" t="s">
-        <v>258</v>
+        <v>484</v>
       </c>
       <c r="J71" t="s">
         <v>205</v>
@@ -3856,25 +3903,10 @@
         <v>24</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D72" t="s">
-        <v>69</v>
-      </c>
-      <c r="E72" t="s">
-        <v>50</v>
-      </c>
-      <c r="F72" t="s">
-        <v>146</v>
-      </c>
-      <c r="G72" t="s">
-        <v>149</v>
-      </c>
-      <c r="H72" t="s">
-        <v>202</v>
+        <v>25</v>
+      </c>
+      <c r="I72" t="s">
+        <v>485</v>
       </c>
       <c r="J72" t="s">
         <v>205</v>
@@ -3882,31 +3914,19 @@
       <c r="K72" t="s">
         <v>219</v>
       </c>
-      <c r="L72" t="s">
-        <v>315</v>
-      </c>
-      <c r="M72" t="s">
-        <v>247</v>
-      </c>
-      <c r="N72" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="O72" s="10" t="s">
-        <v>443</v>
-      </c>
     </row>
     <row r="73" spans="1:15">
       <c r="A73" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H73" t="s">
         <v>202</v>
       </c>
       <c r="I73" t="s">
-        <v>260</v>
+        <v>480</v>
       </c>
       <c r="J73" t="s">
         <v>205</v>
@@ -3920,19 +3940,13 @@
         <v>24</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F74" t="s">
-        <v>147</v>
-      </c>
-      <c r="G74" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="H74" t="s">
         <v>202</v>
       </c>
       <c r="I74" t="s">
-        <v>261</v>
+        <v>350</v>
       </c>
       <c r="J74" t="s">
         <v>205</v>
@@ -3946,13 +3960,13 @@
         <v>24</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H75" t="s">
         <v>202</v>
       </c>
       <c r="I75" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="J75" t="s">
         <v>205</v>
@@ -3968,11 +3982,23 @@
       <c r="B76" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C76" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D76" t="s">
+        <v>69</v>
+      </c>
+      <c r="E76" t="s">
+        <v>50</v>
+      </c>
+      <c r="F76" t="s">
+        <v>146</v>
+      </c>
+      <c r="G76" t="s">
+        <v>149</v>
+      </c>
       <c r="H76" t="s">
         <v>202</v>
-      </c>
-      <c r="I76" t="s">
-        <v>263</v>
       </c>
       <c r="J76" t="s">
         <v>205</v>
@@ -3980,6 +4006,18 @@
       <c r="K76" t="s">
         <v>219</v>
       </c>
+      <c r="L76" t="s">
+        <v>315</v>
+      </c>
+      <c r="M76" t="s">
+        <v>247</v>
+      </c>
+      <c r="N76" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="O76" s="10" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="77" spans="1:15">
       <c r="A77" s="3" t="s">
@@ -3992,7 +4030,7 @@
         <v>202</v>
       </c>
       <c r="I77" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="J77" t="s">
         <v>205</v>
@@ -4000,6 +4038,9 @@
       <c r="K77" t="s">
         <v>219</v>
       </c>
+      <c r="O77" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="78" spans="1:15">
       <c r="A78" s="3" t="s">
@@ -4008,11 +4049,17 @@
       <c r="B78" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F78" t="s">
+        <v>147</v>
+      </c>
+      <c r="G78" t="s">
+        <v>149</v>
+      </c>
       <c r="H78" t="s">
         <v>202</v>
       </c>
       <c r="I78" t="s">
-        <v>484</v>
+        <v>261</v>
       </c>
       <c r="J78" t="s">
         <v>205</v>
@@ -4032,7 +4079,7 @@
         <v>202</v>
       </c>
       <c r="I79" t="s">
-        <v>353</v>
+        <v>262</v>
       </c>
       <c r="J79" t="s">
         <v>205</v>
@@ -4052,7 +4099,7 @@
         <v>202</v>
       </c>
       <c r="I80" t="s">
-        <v>356</v>
+        <v>263</v>
       </c>
       <c r="J80" t="s">
         <v>205</v>
@@ -4072,7 +4119,7 @@
         <v>202</v>
       </c>
       <c r="I81" t="s">
-        <v>418</v>
+        <v>264</v>
       </c>
       <c r="J81" t="s">
         <v>205</v>
@@ -4092,7 +4139,7 @@
         <v>202</v>
       </c>
       <c r="I82" t="s">
-        <v>419</v>
+        <v>481</v>
       </c>
       <c r="J82" t="s">
         <v>205</v>
@@ -4112,7 +4159,7 @@
         <v>202</v>
       </c>
       <c r="I83" t="s">
-        <v>420</v>
+        <v>353</v>
       </c>
       <c r="J83" t="s">
         <v>205</v>
@@ -4132,7 +4179,7 @@
         <v>202</v>
       </c>
       <c r="I84" t="s">
-        <v>482</v>
+        <v>356</v>
       </c>
       <c r="J84" t="s">
         <v>205</v>
@@ -4152,7 +4199,7 @@
         <v>202</v>
       </c>
       <c r="I85" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="J85" t="s">
         <v>205</v>
@@ -4168,8 +4215,11 @@
       <c r="B86" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H86" t="s">
+        <v>202</v>
+      </c>
       <c r="I86" t="s">
-        <v>486</v>
+        <v>419</v>
       </c>
       <c r="J86" t="s">
         <v>205</v>
@@ -4185,8 +4235,11 @@
       <c r="B87" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H87" t="s">
+        <v>202</v>
+      </c>
       <c r="I87" t="s">
-        <v>489</v>
+        <v>420</v>
       </c>
       <c r="J87" t="s">
         <v>205</v>
@@ -4202,8 +4255,11 @@
       <c r="B88" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H88" t="s">
+        <v>202</v>
+      </c>
       <c r="I88" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="J88" t="s">
         <v>205</v>
@@ -4223,7 +4279,7 @@
         <v>202</v>
       </c>
       <c r="I89" t="s">
-        <v>206</v>
+        <v>421</v>
       </c>
       <c r="J89" t="s">
         <v>205</v>
@@ -4239,11 +4295,8 @@
       <c r="B90" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H90" t="s">
-        <v>202</v>
-      </c>
       <c r="I90" t="s">
-        <v>280</v>
+        <v>483</v>
       </c>
       <c r="J90" t="s">
         <v>205</v>
@@ -4259,11 +4312,8 @@
       <c r="B91" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H91" t="s">
-        <v>202</v>
-      </c>
       <c r="I91" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="J91" t="s">
         <v>205</v>
@@ -4277,28 +4327,10 @@
         <v>24</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C92" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D92" t="s">
-        <v>70</v>
-      </c>
-      <c r="E92" t="s">
-        <v>50</v>
-      </c>
-      <c r="F92" t="s">
-        <v>152</v>
-      </c>
-      <c r="G92" t="s">
-        <v>149</v>
-      </c>
-      <c r="H92" t="s">
-        <v>202</v>
+        <v>26</v>
       </c>
       <c r="I92" t="s">
-        <v>265</v>
+        <v>487</v>
       </c>
       <c r="J92" t="s">
         <v>205</v>
@@ -4306,31 +4338,19 @@
       <c r="K92" t="s">
         <v>219</v>
       </c>
-      <c r="L92" t="s">
-        <v>332</v>
-      </c>
-      <c r="M92" t="s">
-        <v>267</v>
-      </c>
-      <c r="N92" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="O92" s="10" t="s">
-        <v>444</v>
-      </c>
     </row>
     <row r="93" spans="1:15">
       <c r="A93" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H93" t="s">
         <v>202</v>
       </c>
       <c r="I93" t="s">
-        <v>266</v>
+        <v>206</v>
       </c>
       <c r="J93" t="s">
         <v>205</v>
@@ -4344,19 +4364,13 @@
         <v>24</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F94" t="s">
-        <v>153</v>
-      </c>
-      <c r="G94" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="H94" t="s">
         <v>202</v>
       </c>
       <c r="I94" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="J94" t="s">
         <v>205</v>
@@ -4370,19 +4384,13 @@
         <v>24</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F95" t="s">
-        <v>190</v>
-      </c>
-      <c r="G95" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="H95" t="s">
         <v>202</v>
       </c>
       <c r="I95" t="s">
-        <v>268</v>
+        <v>478</v>
       </c>
       <c r="J95" t="s">
         <v>205</v>
@@ -4396,19 +4404,19 @@
         <v>24</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D96" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E96" t="s">
         <v>50</v>
       </c>
       <c r="F96" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G96" t="s">
         <v>149</v>
@@ -4417,7 +4425,7 @@
         <v>202</v>
       </c>
       <c r="I96" t="s">
-        <v>85</v>
+        <v>265</v>
       </c>
       <c r="J96" t="s">
         <v>205</v>
@@ -4426,10 +4434,13 @@
         <v>219</v>
       </c>
       <c r="L96" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="M96" t="s">
-        <v>375</v>
+        <v>267</v>
+      </c>
+      <c r="O96" s="10" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="97" spans="1:15">
@@ -4437,10 +4448,19 @@
         <v>24</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L97" t="s">
-        <v>465</v>
+        <v>27</v>
+      </c>
+      <c r="H97" t="s">
+        <v>202</v>
+      </c>
+      <c r="I97" t="s">
+        <v>266</v>
+      </c>
+      <c r="J97" t="s">
+        <v>205</v>
+      </c>
+      <c r="K97" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="98" spans="1:15">
@@ -4448,19 +4468,10 @@
         <v>24</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D98" t="s">
-        <v>73</v>
-      </c>
-      <c r="E98" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F98" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="G98" t="s">
         <v>149</v>
@@ -4469,7 +4480,7 @@
         <v>202</v>
       </c>
       <c r="I98" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J98" t="s">
         <v>205</v>
@@ -4477,37 +4488,16 @@
       <c r="K98" t="s">
         <v>219</v>
       </c>
-      <c r="L98" t="s">
-        <v>312</v>
-      </c>
-      <c r="M98" t="s">
-        <v>372</v>
-      </c>
-      <c r="N98" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="O98" s="10" t="s">
-        <v>437</v>
-      </c>
     </row>
     <row r="99" spans="1:15">
       <c r="A99" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C99" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D99" t="s">
-        <v>74</v>
-      </c>
-      <c r="E99" t="s">
-        <v>50</v>
+        <v>502</v>
       </c>
       <c r="F99" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G99" t="s">
         <v>149</v>
@@ -4516,7 +4506,7 @@
         <v>202</v>
       </c>
       <c r="I99" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J99" t="s">
         <v>205</v>
@@ -4524,11 +4514,11 @@
       <c r="K99" t="s">
         <v>219</v>
       </c>
-      <c r="L99" t="s">
-        <v>321</v>
-      </c>
-      <c r="M99" t="s">
-        <v>373</v>
+      <c r="N99" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="O99" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="100" spans="1:15">
@@ -4536,10 +4526,19 @@
         <v>24</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D100" t="s">
+        <v>85</v>
+      </c>
+      <c r="E100" t="s">
+        <v>50</v>
       </c>
       <c r="F100" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="G100" t="s">
         <v>149</v>
@@ -4548,7 +4547,7 @@
         <v>202</v>
       </c>
       <c r="I100" t="s">
-        <v>271</v>
+        <v>85</v>
       </c>
       <c r="J100" t="s">
         <v>205</v>
@@ -4557,10 +4556,10 @@
         <v>219</v>
       </c>
       <c r="L100" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="M100" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="101" spans="1:15">
@@ -4568,25 +4567,10 @@
         <v>24</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F101" t="s">
-        <v>348</v>
-      </c>
-      <c r="G101" t="s">
-        <v>149</v>
-      </c>
-      <c r="H101" t="s">
-        <v>202</v>
-      </c>
-      <c r="I101" t="s">
-        <v>494</v>
+        <v>28</v>
       </c>
       <c r="L101" t="s">
-        <v>461</v>
-      </c>
-      <c r="M101" t="s">
-        <v>384</v>
+        <v>465</v>
       </c>
     </row>
     <row r="102" spans="1:15">
@@ -4596,8 +4580,17 @@
       <c r="B102" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C102" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D102" t="s">
+        <v>73</v>
+      </c>
+      <c r="E102" t="s">
+        <v>50</v>
+      </c>
       <c r="F102" t="s">
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="G102" t="s">
         <v>149</v>
@@ -4606,7 +4599,7 @@
         <v>202</v>
       </c>
       <c r="I102" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J102" t="s">
         <v>205</v>
@@ -4614,8 +4607,17 @@
       <c r="K102" t="s">
         <v>219</v>
       </c>
+      <c r="L102" t="s">
+        <v>312</v>
+      </c>
       <c r="M102" t="s">
-        <v>411</v>
+        <v>372</v>
+      </c>
+      <c r="N102" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="O102" s="10" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="103" spans="1:15">
@@ -4625,8 +4627,17 @@
       <c r="B103" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C103" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" t="s">
+        <v>74</v>
+      </c>
+      <c r="E103" t="s">
+        <v>50</v>
+      </c>
       <c r="F103" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G103" t="s">
         <v>149</v>
@@ -4635,7 +4646,7 @@
         <v>202</v>
       </c>
       <c r="I103" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J103" t="s">
         <v>205</v>
@@ -4643,6 +4654,15 @@
       <c r="K103" t="s">
         <v>219</v>
       </c>
+      <c r="L103" t="s">
+        <v>321</v>
+      </c>
+      <c r="M103" t="s">
+        <v>373</v>
+      </c>
+      <c r="O103" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="104" spans="1:15">
       <c r="A104" s="3" t="s">
@@ -4652,7 +4672,7 @@
         <v>29</v>
       </c>
       <c r="F104" t="s">
-        <v>359</v>
+        <v>188</v>
       </c>
       <c r="G104" t="s">
         <v>149</v>
@@ -4661,7 +4681,19 @@
         <v>202</v>
       </c>
       <c r="I104" t="s">
-        <v>495</v>
+        <v>271</v>
+      </c>
+      <c r="J104" t="s">
+        <v>205</v>
+      </c>
+      <c r="K104" t="s">
+        <v>219</v>
+      </c>
+      <c r="L104" t="s">
+        <v>322</v>
+      </c>
+      <c r="M104" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="105" spans="1:15">
@@ -4672,7 +4704,7 @@
         <v>29</v>
       </c>
       <c r="F105" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
       <c r="G105" t="s">
         <v>149</v>
@@ -4681,7 +4713,13 @@
         <v>202</v>
       </c>
       <c r="I105" t="s">
-        <v>496</v>
+        <v>491</v>
+      </c>
+      <c r="L105" t="s">
+        <v>461</v>
+      </c>
+      <c r="M105" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="106" spans="1:15">
@@ -4691,11 +4729,26 @@
       <c r="B106" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="F106" t="s">
+        <v>191</v>
+      </c>
+      <c r="G106" t="s">
+        <v>149</v>
+      </c>
       <c r="H106" t="s">
         <v>202</v>
       </c>
       <c r="I106" t="s">
-        <v>74</v>
+        <v>272</v>
+      </c>
+      <c r="J106" t="s">
+        <v>205</v>
+      </c>
+      <c r="K106" t="s">
+        <v>219</v>
+      </c>
+      <c r="M106" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="107" spans="1:15">
@@ -4703,19 +4756,10 @@
         <v>24</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D107" t="s">
-        <v>75</v>
-      </c>
-      <c r="E107" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F107" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G107" t="s">
         <v>149</v>
@@ -4724,7 +4768,7 @@
         <v>202</v>
       </c>
       <c r="I107" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J107" t="s">
         <v>205</v>
@@ -4732,43 +4776,25 @@
       <c r="K107" t="s">
         <v>219</v>
       </c>
-      <c r="M107" t="s">
-        <v>383</v>
-      </c>
-      <c r="N107" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="O107" s="10" t="s">
-        <v>449</v>
-      </c>
     </row>
     <row r="108" spans="1:15">
       <c r="A108" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D108" t="s">
-        <v>93</v>
-      </c>
-      <c r="E108" t="s">
-        <v>50</v>
+        <v>29</v>
+      </c>
+      <c r="F108" t="s">
+        <v>359</v>
+      </c>
+      <c r="G108" t="s">
+        <v>149</v>
       </c>
       <c r="H108" t="s">
         <v>202</v>
       </c>
       <c r="I108" t="s">
-        <v>275</v>
-      </c>
-      <c r="J108" t="s">
-        <v>205</v>
-      </c>
-      <c r="K108" t="s">
-        <v>219</v>
+        <v>492</v>
       </c>
     </row>
     <row r="109" spans="1:15">
@@ -4776,7 +4802,19 @@
         <v>24</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="F109" t="s">
+        <v>362</v>
+      </c>
+      <c r="G109" t="s">
+        <v>149</v>
+      </c>
+      <c r="H109" t="s">
+        <v>202</v>
+      </c>
+      <c r="I109" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="110" spans="1:15">
@@ -4784,46 +4822,13 @@
         <v>24</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C110" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D110" t="s">
-        <v>72</v>
-      </c>
-      <c r="E110" t="s">
-        <v>50</v>
-      </c>
-      <c r="F110" t="s">
-        <v>155</v>
-      </c>
-      <c r="G110" t="s">
-        <v>149</v>
+        <v>29</v>
       </c>
       <c r="H110" t="s">
         <v>202</v>
       </c>
       <c r="I110" t="s">
-        <v>276</v>
-      </c>
-      <c r="J110" t="s">
-        <v>205</v>
-      </c>
-      <c r="K110" t="s">
-        <v>219</v>
-      </c>
-      <c r="L110" t="s">
-        <v>316</v>
-      </c>
-      <c r="M110" t="s">
-        <v>386</v>
-      </c>
-      <c r="N110" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="O110" s="10" t="s">
-        <v>439</v>
+        <v>74</v>
       </c>
     </row>
     <row r="111" spans="1:15">
@@ -4831,10 +4836,19 @@
         <v>24</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C111" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D111" t="s">
+        <v>75</v>
+      </c>
+      <c r="E111" t="s">
+        <v>50</v>
       </c>
       <c r="F111" t="s">
-        <v>156</v>
+        <v>198</v>
       </c>
       <c r="G111" t="s">
         <v>149</v>
@@ -4843,7 +4857,7 @@
         <v>202</v>
       </c>
       <c r="I111" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J111" t="s">
         <v>205</v>
@@ -4851,8 +4865,14 @@
       <c r="K111" t="s">
         <v>219</v>
       </c>
-      <c r="L111" t="s">
-        <v>450</v>
+      <c r="M111" t="s">
+        <v>383</v>
+      </c>
+      <c r="N111" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="O111" s="10" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="112" spans="1:15">
@@ -4860,16 +4880,28 @@
         <v>24</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F112" t="s">
-        <v>364</v>
-      </c>
-      <c r="G112" t="s">
-        <v>149</v>
+        <v>31</v>
+      </c>
+      <c r="C112" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D112" t="s">
+        <v>93</v>
+      </c>
+      <c r="E112" t="s">
+        <v>50</v>
       </c>
       <c r="H112" t="s">
         <v>202</v>
+      </c>
+      <c r="I112" t="s">
+        <v>275</v>
+      </c>
+      <c r="J112" t="s">
+        <v>205</v>
+      </c>
+      <c r="K112" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:15">
@@ -4877,40 +4909,7 @@
         <v>24</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D113" t="s">
-        <v>71</v>
-      </c>
-      <c r="E113" t="s">
-        <v>50</v>
-      </c>
-      <c r="F113" t="s">
-        <v>154</v>
-      </c>
-      <c r="G113" t="s">
-        <v>149</v>
-      </c>
-      <c r="H113" t="s">
-        <v>202</v>
-      </c>
-      <c r="I113" t="s">
-        <v>278</v>
-      </c>
-      <c r="J113" t="s">
-        <v>205</v>
-      </c>
-      <c r="K113" t="s">
-        <v>219</v>
-      </c>
-      <c r="L113" t="s">
-        <v>335</v>
-      </c>
-      <c r="M113" t="s">
-        <v>382</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:15">
@@ -4918,19 +4917,19 @@
         <v>24</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C114" s="6">
-        <v>253</v>
+        <v>33</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D114" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E114" t="s">
         <v>50</v>
       </c>
       <c r="F114" t="s">
-        <v>221</v>
+        <v>155</v>
       </c>
       <c r="G114" t="s">
         <v>149</v>
@@ -4939,7 +4938,7 @@
         <v>202</v>
       </c>
       <c r="I114" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J114" t="s">
         <v>205</v>
@@ -4947,16 +4946,28 @@
       <c r="K114" t="s">
         <v>219</v>
       </c>
+      <c r="L114" t="s">
+        <v>316</v>
+      </c>
+      <c r="M114" t="s">
+        <v>386</v>
+      </c>
+      <c r="N114" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="O114" s="10" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="115" spans="1:15">
       <c r="A115" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F115" t="s">
-        <v>197</v>
+        <v>156</v>
       </c>
       <c r="G115" t="s">
         <v>149</v>
@@ -4965,7 +4976,19 @@
         <v>202</v>
       </c>
       <c r="I115" t="s">
-        <v>485</v>
+        <v>277</v>
+      </c>
+      <c r="J115" t="s">
+        <v>205</v>
+      </c>
+      <c r="K115" t="s">
+        <v>219</v>
+      </c>
+      <c r="L115" t="s">
+        <v>450</v>
+      </c>
+      <c r="O115" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="116" spans="1:15">
@@ -4973,19 +4996,10 @@
         <v>24</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D116" t="s">
-        <v>35</v>
-      </c>
-      <c r="E116" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F116" t="s">
-        <v>476</v>
+        <v>364</v>
       </c>
       <c r="G116" t="s">
         <v>149</v>
@@ -4993,43 +5007,25 @@
       <c r="H116" t="s">
         <v>202</v>
       </c>
-      <c r="I116" t="s">
-        <v>35</v>
-      </c>
-      <c r="J116" t="s">
-        <v>205</v>
-      </c>
-      <c r="K116" t="s">
-        <v>214</v>
-      </c>
-      <c r="L116" t="s">
-        <v>464</v>
-      </c>
-      <c r="M116" t="s">
-        <v>35</v>
-      </c>
-      <c r="O116" s="10" t="s">
-        <v>448</v>
-      </c>
     </row>
     <row r="117" spans="1:15">
       <c r="A117" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D117" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="E117" t="s">
         <v>50</v>
       </c>
       <c r="F117" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
       <c r="G117" t="s">
         <v>149</v>
@@ -5038,19 +5034,19 @@
         <v>202</v>
       </c>
       <c r="I117" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J117" t="s">
         <v>205</v>
       </c>
       <c r="K117" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="L117" t="s">
-        <v>463</v>
+        <v>335</v>
       </c>
       <c r="M117" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="118" spans="1:15">
@@ -5058,10 +5054,19 @@
         <v>24</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="C118" s="6">
+        <v>253</v>
+      </c>
+      <c r="D118" t="s">
+        <v>91</v>
+      </c>
+      <c r="E118" t="s">
+        <v>50</v>
       </c>
       <c r="F118" t="s">
-        <v>192</v>
+        <v>221</v>
       </c>
       <c r="G118" t="s">
         <v>149</v>
@@ -5070,7 +5075,7 @@
         <v>202</v>
       </c>
       <c r="I118" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J118" t="s">
         <v>205</v>
@@ -5084,10 +5089,10 @@
         <v>24</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F119" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G119" t="s">
         <v>149</v>
@@ -5095,37 +5100,52 @@
       <c r="H119" t="s">
         <v>202</v>
       </c>
+      <c r="I119" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="120" spans="1:15">
       <c r="A120" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C120" s="6">
-        <v>311</v>
+        <v>35</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="D120" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E120" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="F120" t="s">
+        <v>476</v>
+      </c>
+      <c r="G120" t="s">
+        <v>149</v>
+      </c>
+      <c r="H120" t="s">
+        <v>202</v>
       </c>
       <c r="I120" t="s">
-        <v>283</v>
+        <v>35</v>
       </c>
       <c r="J120" t="s">
         <v>205</v>
       </c>
       <c r="K120" t="s">
-        <v>219</v>
+        <v>214</v>
+      </c>
+      <c r="L120" t="s">
+        <v>464</v>
       </c>
       <c r="M120" t="s">
-        <v>377</v>
+        <v>35</v>
       </c>
       <c r="O120" s="10" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
     </row>
     <row r="121" spans="1:15">
@@ -5133,16 +5153,43 @@
         <v>24</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C121" s="6">
-        <v>312</v>
+        <v>36</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="D121" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
       <c r="E121" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="F121" t="s">
+        <v>196</v>
+      </c>
+      <c r="G121" t="s">
+        <v>149</v>
+      </c>
+      <c r="H121" t="s">
+        <v>202</v>
+      </c>
+      <c r="I121" t="s">
+        <v>281</v>
+      </c>
+      <c r="J121" t="s">
+        <v>205</v>
+      </c>
+      <c r="K121" t="s">
+        <v>214</v>
+      </c>
+      <c r="L121" t="s">
+        <v>463</v>
+      </c>
+      <c r="M121" t="s">
+        <v>381</v>
+      </c>
+      <c r="O121" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="122" spans="1:15">
@@ -5150,19 +5197,25 @@
         <v>24</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="D122" t="s">
-        <v>305</v>
-      </c>
-      <c r="E122" t="s">
-        <v>50</v>
-      </c>
-      <c r="M122" t="s">
-        <v>376</v>
+        <v>36</v>
+      </c>
+      <c r="F122" t="s">
+        <v>192</v>
+      </c>
+      <c r="G122" t="s">
+        <v>149</v>
+      </c>
+      <c r="H122" t="s">
+        <v>202</v>
+      </c>
+      <c r="I122" t="s">
+        <v>282</v>
+      </c>
+      <c r="J122" t="s">
+        <v>205</v>
+      </c>
+      <c r="K122" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="123" spans="1:15">
@@ -5170,10 +5223,16 @@
         <v>24</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="M123" t="s">
-        <v>379</v>
+        <v>36</v>
+      </c>
+      <c r="F123" t="s">
+        <v>193</v>
+      </c>
+      <c r="G123" t="s">
+        <v>149</v>
+      </c>
+      <c r="H123" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="124" spans="1:15">
@@ -5181,28 +5240,19 @@
         <v>24</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>308</v>
+        <v>37</v>
+      </c>
+      <c r="C124" s="6">
+        <v>311</v>
       </c>
       <c r="D124" t="s">
-        <v>307</v>
+        <v>76</v>
       </c>
       <c r="E124" t="s">
-        <v>50</v>
-      </c>
-      <c r="F124" t="s">
-        <v>189</v>
-      </c>
-      <c r="G124" t="s">
-        <v>149</v>
-      </c>
-      <c r="H124" t="s">
-        <v>202</v>
+        <v>52</v>
       </c>
       <c r="I124" t="s">
-        <v>354</v>
+        <v>283</v>
       </c>
       <c r="J124" t="s">
         <v>205</v>
@@ -5210,25 +5260,28 @@
       <c r="K124" t="s">
         <v>219</v>
       </c>
+      <c r="M124" t="s">
+        <v>377</v>
+      </c>
+      <c r="O124" s="10" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="125" spans="1:15">
       <c r="A125" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="F125" t="s">
-        <v>345</v>
-      </c>
-      <c r="G125" t="s">
-        <v>149</v>
-      </c>
-      <c r="H125" t="s">
-        <v>202</v>
-      </c>
-      <c r="L125" t="s">
-        <v>331</v>
+        <v>37</v>
+      </c>
+      <c r="C125" s="6">
+        <v>312</v>
+      </c>
+      <c r="D125" t="s">
+        <v>136</v>
+      </c>
+      <c r="E125" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="126" spans="1:15">
@@ -5236,28 +5289,19 @@
         <v>24</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="F126" t="s">
-        <v>473</v>
-      </c>
-      <c r="G126" t="s">
-        <v>149</v>
-      </c>
-      <c r="H126" t="s">
-        <v>202</v>
-      </c>
-      <c r="I126" t="s">
-        <v>492</v>
-      </c>
-      <c r="J126" t="s">
-        <v>205</v>
-      </c>
-      <c r="K126" t="s">
-        <v>219</v>
-      </c>
-      <c r="L126" t="s">
-        <v>457</v>
+        <v>305</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D126" t="s">
+        <v>305</v>
+      </c>
+      <c r="E126" t="s">
+        <v>50</v>
+      </c>
+      <c r="M126" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="127" spans="1:15">
@@ -5265,28 +5309,10 @@
         <v>24</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="H127" t="s">
-        <v>202</v>
-      </c>
-      <c r="I127" t="s">
-        <v>284</v>
-      </c>
-      <c r="J127" t="s">
-        <v>205</v>
-      </c>
-      <c r="K127" t="s">
-        <v>219</v>
+        <v>378</v>
       </c>
       <c r="M127" t="s">
-        <v>288</v>
-      </c>
-      <c r="N127" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="O127" s="10" t="s">
-        <v>436</v>
+        <v>379</v>
       </c>
     </row>
     <row r="128" spans="1:15">
@@ -5294,21 +5320,45 @@
         <v>24</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="M128" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="129" spans="1:12">
+        <v>309</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D128" t="s">
+        <v>307</v>
+      </c>
+      <c r="E128" t="s">
+        <v>50</v>
+      </c>
+      <c r="F128" t="s">
+        <v>189</v>
+      </c>
+      <c r="G128" t="s">
+        <v>149</v>
+      </c>
+      <c r="H128" t="s">
+        <v>202</v>
+      </c>
+      <c r="I128" t="s">
+        <v>354</v>
+      </c>
+      <c r="J128" t="s">
+        <v>205</v>
+      </c>
+      <c r="K128" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="129" spans="1:15">
       <c r="A129" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>470</v>
+        <v>346</v>
       </c>
       <c r="F129" t="s">
-        <v>471</v>
+        <v>345</v>
       </c>
       <c r="G129" t="s">
         <v>149</v>
@@ -5316,147 +5366,117 @@
       <c r="H129" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="130" spans="1:12">
-      <c r="A130" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B130" s="4" t="s">
+      <c r="L129" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15">
+      <c r="A130" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="F130" t="s">
+        <v>473</v>
+      </c>
+      <c r="G130" t="s">
+        <v>149</v>
+      </c>
+      <c r="H130" t="s">
+        <v>202</v>
+      </c>
+      <c r="I130" t="s">
+        <v>489</v>
+      </c>
+      <c r="J130" t="s">
+        <v>205</v>
+      </c>
+      <c r="K130" t="s">
+        <v>219</v>
+      </c>
+      <c r="L130" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15">
+      <c r="A131" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="H131" t="s">
+        <v>202</v>
+      </c>
+      <c r="I131" t="s">
+        <v>284</v>
+      </c>
+      <c r="J131" t="s">
+        <v>205</v>
+      </c>
+      <c r="K131" t="s">
+        <v>219</v>
+      </c>
+      <c r="M131" t="s">
+        <v>288</v>
+      </c>
+      <c r="N131" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="O131" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
+      <c r="A132" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="M132" t="s">
         <v>39</v>
       </c>
-      <c r="C130" s="6">
-        <v>511</v>
-      </c>
-      <c r="D130" t="s">
-        <v>82</v>
-      </c>
-      <c r="E130" t="s">
-        <v>51</v>
-      </c>
-      <c r="F130" t="s">
-        <v>182</v>
-      </c>
-      <c r="G130" t="s">
-        <v>187</v>
-      </c>
-      <c r="H130" t="s">
-        <v>202</v>
-      </c>
-      <c r="J130" t="s">
-        <v>207</v>
-      </c>
-      <c r="K130" t="s">
-        <v>218</v>
-      </c>
-      <c r="L130" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="131" spans="1:12">
-      <c r="A131" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B131" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F131" t="s">
-        <v>180</v>
-      </c>
-      <c r="G131" t="s">
-        <v>187</v>
-      </c>
-      <c r="H131" t="s">
-        <v>202</v>
-      </c>
-      <c r="I131" t="s">
-        <v>285</v>
-      </c>
-      <c r="J131" t="s">
-        <v>207</v>
-      </c>
-      <c r="K131" t="s">
-        <v>218</v>
-      </c>
-      <c r="L131" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="132" spans="1:12">
-      <c r="A132" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B132" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C132" s="6">
-        <v>513</v>
-      </c>
-      <c r="D132" t="s">
-        <v>83</v>
-      </c>
-      <c r="E132" t="s">
-        <v>51</v>
-      </c>
-      <c r="F132" t="s">
-        <v>178</v>
-      </c>
-      <c r="G132" t="s">
-        <v>187</v>
-      </c>
-      <c r="H132" t="s">
-        <v>202</v>
-      </c>
-      <c r="I132" t="s">
-        <v>286</v>
-      </c>
-      <c r="J132" t="s">
-        <v>207</v>
-      </c>
-      <c r="K132" t="s">
-        <v>218</v>
-      </c>
-      <c r="L132" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="133" spans="1:12">
-      <c r="A133" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>39</v>
+      <c r="O132" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15">
+      <c r="A133" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>470</v>
       </c>
       <c r="F133" t="s">
-        <v>177</v>
+        <v>471</v>
       </c>
       <c r="G133" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="H133" t="s">
         <v>202</v>
       </c>
-      <c r="I133" t="s">
-        <v>287</v>
-      </c>
-      <c r="J133" t="s">
-        <v>207</v>
-      </c>
-      <c r="K133" t="s">
-        <v>218</v>
-      </c>
-      <c r="L133" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="134" spans="1:12">
+    </row>
+    <row r="134" spans="1:15">
       <c r="A134" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B134" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C134" s="6">
+        <v>511</v>
+      </c>
+      <c r="D134" t="s">
+        <v>82</v>
+      </c>
+      <c r="E134" t="s">
+        <v>51</v>
+      </c>
       <c r="F134" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="G134" t="s">
         <v>187</v>
@@ -5464,20 +5484,17 @@
       <c r="H134" t="s">
         <v>202</v>
       </c>
-      <c r="I134" t="s">
-        <v>288</v>
-      </c>
       <c r="J134" t="s">
         <v>207</v>
       </c>
       <c r="K134" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="L134" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="135" spans="1:12">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15">
       <c r="A135" s="4" t="s">
         <v>38</v>
       </c>
@@ -5485,7 +5502,7 @@
         <v>39</v>
       </c>
       <c r="F135" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G135" t="s">
         <v>187</v>
@@ -5494,7 +5511,7 @@
         <v>202</v>
       </c>
       <c r="I135" t="s">
-        <v>39</v>
+        <v>285</v>
       </c>
       <c r="J135" t="s">
         <v>207</v>
@@ -5503,18 +5520,27 @@
         <v>218</v>
       </c>
       <c r="L135" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="136" spans="1:12" ht="17" customHeight="1">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15">
       <c r="A136" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B136" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="C136" s="6">
+        <v>513</v>
+      </c>
+      <c r="D136" t="s">
+        <v>83</v>
+      </c>
+      <c r="E136" t="s">
+        <v>51</v>
+      </c>
       <c r="F136" t="s">
-        <v>358</v>
+        <v>178</v>
       </c>
       <c r="G136" t="s">
         <v>187</v>
@@ -5523,7 +5549,7 @@
         <v>202</v>
       </c>
       <c r="I136" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J136" t="s">
         <v>207</v>
@@ -5531,8 +5557,11 @@
       <c r="K136" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="137" spans="1:12" ht="17" customHeight="1">
+      <c r="L136" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15">
       <c r="A137" s="4" t="s">
         <v>38</v>
       </c>
@@ -5540,7 +5569,7 @@
         <v>39</v>
       </c>
       <c r="F137" t="s">
-        <v>474</v>
+        <v>177</v>
       </c>
       <c r="G137" t="s">
         <v>187</v>
@@ -5549,7 +5578,7 @@
         <v>202</v>
       </c>
       <c r="I137" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="J137" t="s">
         <v>207</v>
@@ -5557,8 +5586,11 @@
       <c r="K137" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="138" spans="1:12" ht="17" customHeight="1">
+      <c r="L137" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15">
       <c r="A138" s="4" t="s">
         <v>38</v>
       </c>
@@ -5566,7 +5598,7 @@
         <v>39</v>
       </c>
       <c r="F138" t="s">
-        <v>475</v>
+        <v>38</v>
       </c>
       <c r="G138" t="s">
         <v>187</v>
@@ -5575,27 +5607,36 @@
         <v>202</v>
       </c>
       <c r="I138" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="J138" t="s">
         <v>207</v>
       </c>
       <c r="K138" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="139" spans="1:12" ht="17" customHeight="1">
+        <v>214</v>
+      </c>
+      <c r="L138" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15">
       <c r="A139" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B139" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F139" t="s">
+        <v>183</v>
+      </c>
+      <c r="G139" t="s">
+        <v>187</v>
+      </c>
       <c r="H139" t="s">
         <v>202</v>
       </c>
       <c r="I139" t="s">
-        <v>292</v>
+        <v>39</v>
       </c>
       <c r="J139" t="s">
         <v>207</v>
@@ -5603,8 +5644,11 @@
       <c r="K139" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="140" spans="1:12" ht="17" customHeight="1">
+      <c r="L139" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" ht="17" customHeight="1">
       <c r="A140" s="4" t="s">
         <v>38</v>
       </c>
@@ -5612,7 +5656,7 @@
         <v>39</v>
       </c>
       <c r="F140" t="s">
-        <v>181</v>
+        <v>358</v>
       </c>
       <c r="G140" t="s">
         <v>187</v>
@@ -5621,7 +5665,7 @@
         <v>202</v>
       </c>
       <c r="I140" t="s">
-        <v>491</v>
+        <v>289</v>
       </c>
       <c r="J140" t="s">
         <v>207</v>
@@ -5630,7 +5674,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="17" customHeight="1">
+    <row r="141" spans="1:15" ht="17" customHeight="1">
       <c r="A141" s="4" t="s">
         <v>38</v>
       </c>
@@ -5638,7 +5682,7 @@
         <v>39</v>
       </c>
       <c r="F141" t="s">
-        <v>185</v>
+        <v>474</v>
       </c>
       <c r="G141" t="s">
         <v>187</v>
@@ -5647,7 +5691,7 @@
         <v>202</v>
       </c>
       <c r="I141" t="s">
-        <v>213</v>
+        <v>290</v>
       </c>
       <c r="J141" t="s">
         <v>207</v>
@@ -5656,18 +5700,24 @@
         <v>218</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="17" customHeight="1">
+    <row r="142" spans="1:15" ht="17" customHeight="1">
       <c r="A142" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F142" t="s">
+        <v>475</v>
+      </c>
+      <c r="G142" t="s">
+        <v>187</v>
+      </c>
       <c r="H142" t="s">
         <v>202</v>
       </c>
       <c r="I142" t="s">
-        <v>493</v>
+        <v>291</v>
       </c>
       <c r="J142" t="s">
         <v>207</v>
@@ -5676,7 +5726,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="17" customHeight="1">
+    <row r="143" spans="1:15" ht="17" customHeight="1">
       <c r="A143" s="4" t="s">
         <v>38</v>
       </c>
@@ -5687,7 +5737,7 @@
         <v>202</v>
       </c>
       <c r="I143" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J143" t="s">
         <v>207</v>
@@ -5696,15 +5746,15 @@
         <v>218</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:15" ht="17" customHeight="1">
       <c r="A144" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F144" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="G144" t="s">
         <v>187</v>
@@ -5713,7 +5763,7 @@
         <v>202</v>
       </c>
       <c r="I144" t="s">
-        <v>294</v>
+        <v>488</v>
       </c>
       <c r="J144" t="s">
         <v>207</v>
@@ -5721,19 +5771,16 @@
       <c r="K144" t="s">
         <v>218</v>
       </c>
-      <c r="L144" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="145" spans="1:12">
+    </row>
+    <row r="145" spans="1:12" ht="17" customHeight="1">
       <c r="A145" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F145" t="s">
-        <v>363</v>
+        <v>185</v>
       </c>
       <c r="G145" t="s">
         <v>187</v>
@@ -5742,7 +5789,7 @@
         <v>202</v>
       </c>
       <c r="I145" t="s">
-        <v>295</v>
+        <v>213</v>
       </c>
       <c r="J145" t="s">
         <v>207</v>
@@ -5751,18 +5798,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" ht="17" customHeight="1">
       <c r="A146" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H146" t="s">
         <v>202</v>
       </c>
       <c r="I146" t="s">
-        <v>296</v>
+        <v>490</v>
       </c>
       <c r="J146" t="s">
         <v>207</v>
@@ -5771,33 +5818,24 @@
         <v>218</v>
       </c>
     </row>
-    <row r="147" spans="1:12">
+    <row r="147" spans="1:12" ht="17" customHeight="1">
       <c r="A147" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F147" t="s">
-        <v>179</v>
-      </c>
-      <c r="G147" t="s">
-        <v>187</v>
+        <v>39</v>
       </c>
       <c r="H147" t="s">
         <v>202</v>
       </c>
       <c r="I147" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J147" t="s">
         <v>207</v>
       </c>
       <c r="K147" t="s">
         <v>218</v>
-      </c>
-      <c r="L147" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="148" spans="1:12">
@@ -5805,22 +5843,28 @@
         <v>38</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F148" t="s">
-        <v>361</v>
+        <v>176</v>
+      </c>
+      <c r="G148" t="s">
+        <v>187</v>
       </c>
       <c r="H148" t="s">
         <v>202</v>
       </c>
       <c r="I148" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="J148" t="s">
         <v>207</v>
       </c>
       <c r="K148" t="s">
         <v>218</v>
+      </c>
+      <c r="L148" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="149" spans="1:12">
@@ -5828,10 +5872,10 @@
         <v>38</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F149" t="s">
-        <v>175</v>
+        <v>363</v>
       </c>
       <c r="G149" t="s">
         <v>187</v>
@@ -5840,16 +5884,13 @@
         <v>202</v>
       </c>
       <c r="I149" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="J149" t="s">
         <v>207</v>
       </c>
       <c r="K149" t="s">
         <v>218</v>
-      </c>
-      <c r="L149" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="150" spans="1:12">
@@ -5857,19 +5898,13 @@
         <v>38</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F150" t="s">
-        <v>472</v>
-      </c>
-      <c r="G150" t="s">
-        <v>187</v>
+        <v>40</v>
       </c>
       <c r="H150" t="s">
         <v>202</v>
       </c>
       <c r="I150" t="s">
-        <v>42</v>
+        <v>296</v>
       </c>
       <c r="J150" t="s">
         <v>207</v>
@@ -5883,19 +5918,28 @@
         <v>38</v>
       </c>
       <c r="B151" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F151" t="s">
+        <v>179</v>
+      </c>
+      <c r="G151" t="s">
+        <v>187</v>
       </c>
       <c r="H151" t="s">
         <v>202</v>
       </c>
       <c r="I151" t="s">
-        <v>212</v>
+        <v>297</v>
       </c>
       <c r="J151" t="s">
         <v>207</v>
       </c>
       <c r="K151" t="s">
         <v>218</v>
+      </c>
+      <c r="L151" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="152" spans="1:12">
@@ -5903,13 +5947,16 @@
         <v>38</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="F152" t="s">
+        <v>361</v>
       </c>
       <c r="H152" t="s">
         <v>202</v>
       </c>
       <c r="I152" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J152" t="s">
         <v>207</v>
@@ -5923,19 +5970,10 @@
         <v>38</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C153" s="6" t="s">
-        <v>469</v>
-      </c>
-      <c r="D153" t="s">
-        <v>468</v>
-      </c>
-      <c r="E153" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F153" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G153" t="s">
         <v>187</v>
@@ -5944,13 +5982,16 @@
         <v>202</v>
       </c>
       <c r="I153" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J153" t="s">
         <v>207</v>
       </c>
       <c r="K153" t="s">
         <v>218</v>
+      </c>
+      <c r="L153" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="154" spans="1:12">
@@ -5958,10 +5999,10 @@
         <v>38</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F154" t="s">
-        <v>184</v>
+        <v>472</v>
       </c>
       <c r="G154" t="s">
         <v>187</v>
@@ -5969,112 +6010,106 @@
       <c r="H154" t="s">
         <v>202</v>
       </c>
+      <c r="I154" t="s">
+        <v>42</v>
+      </c>
+      <c r="J154" t="s">
+        <v>207</v>
+      </c>
+      <c r="K154" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="155" spans="1:12">
-      <c r="A155" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E155" t="s">
-        <v>53</v>
+      <c r="A155" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="H155" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I155" t="s">
-        <v>302</v>
+        <v>212</v>
       </c>
       <c r="J155" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K155" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="156" spans="1:12">
-      <c r="A156" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>46</v>
+      <c r="A156" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="H156" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I156" t="s">
-        <v>209</v>
+        <v>300</v>
       </c>
       <c r="J156" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K156" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="157" spans="1:12">
-      <c r="A157" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B157" s="5" t="s">
-        <v>46</v>
+      <c r="A157" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="C157" s="6" t="s">
-        <v>123</v>
+        <v>469</v>
       </c>
       <c r="D157" t="s">
-        <v>46</v>
+        <v>468</v>
       </c>
       <c r="E157" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F157" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="G157" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="H157" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I157" t="s">
-        <v>46</v>
+        <v>301</v>
       </c>
       <c r="J157" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K157" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="158" spans="1:12">
-      <c r="A158" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B158" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="D158" t="s">
-        <v>92</v>
-      </c>
-      <c r="E158" t="s">
-        <v>53</v>
+      <c r="A158" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F158" t="s">
+        <v>184</v>
+      </c>
+      <c r="G158" t="s">
+        <v>187</v>
       </c>
       <c r="H158" t="s">
-        <v>201</v>
-      </c>
-      <c r="I158" t="s">
-        <v>303</v>
-      </c>
-      <c r="J158" t="s">
-        <v>210</v>
-      </c>
-      <c r="K158" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="159" spans="1:12">
@@ -6082,13 +6117,7 @@
         <v>44</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C159" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="D159" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E159" t="s">
         <v>53</v>
@@ -6097,12 +6126,125 @@
         <v>201</v>
       </c>
       <c r="I159" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="J159" t="s">
         <v>210</v>
       </c>
       <c r="K159" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
+      <c r="A160" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H160" t="s">
+        <v>201</v>
+      </c>
+      <c r="I160" t="s">
+        <v>209</v>
+      </c>
+      <c r="J160" t="s">
+        <v>210</v>
+      </c>
+      <c r="K160" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="A161" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C161" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D161" t="s">
+        <v>46</v>
+      </c>
+      <c r="E161" t="s">
+        <v>53</v>
+      </c>
+      <c r="F161" t="s">
+        <v>162</v>
+      </c>
+      <c r="G161" t="s">
+        <v>174</v>
+      </c>
+      <c r="H161" t="s">
+        <v>201</v>
+      </c>
+      <c r="I161" t="s">
+        <v>46</v>
+      </c>
+      <c r="J161" t="s">
+        <v>210</v>
+      </c>
+      <c r="K161" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="A162" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B162" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C162" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D162" t="s">
+        <v>92</v>
+      </c>
+      <c r="E162" t="s">
+        <v>53</v>
+      </c>
+      <c r="H162" t="s">
+        <v>201</v>
+      </c>
+      <c r="I162" t="s">
+        <v>303</v>
+      </c>
+      <c r="J162" t="s">
+        <v>210</v>
+      </c>
+      <c r="K162" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="A163" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D163" t="s">
+        <v>48</v>
+      </c>
+      <c r="E163" t="s">
+        <v>53</v>
+      </c>
+      <c r="H163" t="s">
+        <v>201</v>
+      </c>
+      <c r="I163" t="s">
+        <v>304</v>
+      </c>
+      <c r="J163" t="s">
+        <v>210</v>
+      </c>
+      <c r="K163" t="s">
         <v>215</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: enhancing the raw claim formatting functions and the usage report conversion
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/RawClaimMCR-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B716B83-6AC3-BA43-8D00-54C1A4A7F61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4962E7-3DC1-F845-B10F-59E8851B2440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18340" yWindow="-20980" windowWidth="38400" windowHeight="19880" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="-18340" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1318" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="569">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1674,6 +1674,75 @@
   </si>
   <si>
     <t>VAC</t>
+  </si>
+  <si>
+    <t>PRESCRIPTIONS</t>
+  </si>
+  <si>
+    <t>HOSP CASH FOR 2ND PAYER</t>
+  </si>
+  <si>
+    <t>liberty_benefit</t>
+  </si>
+  <si>
+    <t>OSP</t>
+  </si>
+  <si>
+    <t>PMA</t>
+  </si>
+  <si>
+    <t>CBAT</t>
+  </si>
+  <si>
+    <t>Outpatient others (Liberty)</t>
+  </si>
+  <si>
+    <t>OTH</t>
+  </si>
+  <si>
+    <t>LAB</t>
+  </si>
+  <si>
+    <t>EXTR</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>FL</t>
+  </si>
+  <si>
+    <t>Abscesses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dental Medication </t>
+  </si>
+  <si>
+    <t>ABSC</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>RCT</t>
+  </si>
+  <si>
+    <t>ROEX</t>
+  </si>
+  <si>
+    <t>RNB</t>
+  </si>
+  <si>
+    <t>HSM</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>HDC</t>
+  </si>
+  <si>
+    <t>EYE</t>
   </si>
 </sst>
 </file>
@@ -2108,13 +2177,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:P167"/>
+  <dimension ref="A1:Q172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G103" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L126" sqref="L126:L127"/>
+      <selection pane="bottomRight" activeCell="O113" sqref="O113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2132,7 +2201,7 @@
     <col min="14" max="14" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -2181,8 +2250,11 @@
       <c r="P1" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" customHeight="1">
+      <c r="Q1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -2231,8 +2303,11 @@
       <c r="P2" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="17" customHeight="1">
+      <c r="Q2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -2263,11 +2338,8 @@
       <c r="O3" t="s">
         <v>497</v>
       </c>
-      <c r="P3" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2313,8 +2385,14 @@
       <c r="O4" s="10" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="P4" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -2343,7 +2421,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -2392,8 +2470,11 @@
       <c r="P6" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -2426,7 +2507,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -2440,7 +2521,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -2457,7 +2538,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -2492,7 +2573,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -2509,7 +2590,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -2532,7 +2613,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -2549,7 +2630,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2584,7 +2665,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -2604,7 +2685,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -2639,7 +2720,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -2659,7 +2740,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -2698,7 +2779,7 @@
       </c>
       <c r="O18" s="10"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -2718,7 +2799,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -2737,8 +2818,11 @@
       <c r="P20" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
@@ -2749,7 +2833,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -2769,7 +2853,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2804,7 +2888,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2839,7 +2923,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2877,7 +2961,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
@@ -2897,8 +2981,11 @@
       <c r="P26" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="1" t="s">
         <v>23</v>
       </c>
@@ -2910,7 +2997,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="17" customHeight="1">
+    <row r="28" spans="1:17" ht="17" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -2927,7 +3014,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17">
       <c r="A29" s="1" t="s">
         <v>23</v>
       </c>
@@ -2962,7 +3049,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
@@ -2982,7 +3069,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -3017,7 +3104,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17">
       <c r="A32" s="1" t="s">
         <v>23</v>
       </c>
@@ -3037,7 +3124,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="A33" s="1" t="s">
         <v>23</v>
       </c>
@@ -3075,7 +3162,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="A34" s="1" t="s">
         <v>23</v>
       </c>
@@ -3095,7 +3182,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="A35" s="1" t="s">
         <v>23</v>
       </c>
@@ -3114,8 +3201,11 @@
       <c r="P35" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36" s="1" t="s">
         <v>23</v>
       </c>
@@ -3126,7 +3216,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17">
       <c r="A37" s="1" t="s">
         <v>23</v>
       </c>
@@ -3170,7 +3260,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:17">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -3196,7 +3286,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:17">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -3222,7 +3312,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17">
       <c r="A40" s="1" t="s">
         <v>23</v>
       </c>
@@ -3257,7 +3347,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17">
       <c r="A41" s="1" t="s">
         <v>23</v>
       </c>
@@ -3275,7 +3365,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="A42" s="1" t="s">
         <v>23</v>
       </c>
@@ -3298,7 +3388,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:17">
       <c r="A43" s="1" t="s">
         <v>23</v>
       </c>
@@ -3319,7 +3409,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:17">
       <c r="A44" s="1" t="s">
         <v>23</v>
       </c>
@@ -3343,7 +3433,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:17">
       <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
@@ -3367,7 +3457,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:17">
       <c r="A46" s="1" t="s">
         <v>23</v>
       </c>
@@ -3391,7 +3481,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:17">
       <c r="A47" s="1" t="s">
         <v>23</v>
       </c>
@@ -3415,7 +3505,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:17">
       <c r="A48" s="1" t="s">
         <v>23</v>
       </c>
@@ -3462,7 +3552,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:17">
       <c r="A49" s="1" t="s">
         <v>23</v>
       </c>
@@ -3503,7 +3593,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:17">
       <c r="A50" s="1" t="s">
         <v>23</v>
       </c>
@@ -3529,7 +3619,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:17">
       <c r="A51" s="1" t="s">
         <v>23</v>
       </c>
@@ -3549,7 +3639,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:17">
       <c r="A52" s="1" t="s">
         <v>23</v>
       </c>
@@ -3592,8 +3682,11 @@
       <c r="O52" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="P52" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53" s="1" t="s">
         <v>23</v>
       </c>
@@ -3607,7 +3700,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:17">
       <c r="A54" s="1" t="s">
         <v>23</v>
       </c>
@@ -3624,7 +3717,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:17">
       <c r="A55" s="1" t="s">
         <v>23</v>
       </c>
@@ -3632,7 +3725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:17">
       <c r="A56" s="1" t="s">
         <v>23</v>
       </c>
@@ -3649,7 +3742,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:17">
       <c r="A57" s="1" t="s">
         <v>23</v>
       </c>
@@ -3661,7 +3754,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:17">
       <c r="A58" s="2" t="s">
         <v>309</v>
       </c>
@@ -3705,7 +3798,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:17">
       <c r="A59" s="3" t="s">
         <v>24</v>
       </c>
@@ -3754,8 +3847,11 @@
       <c r="P59" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60" s="3" t="s">
         <v>24</v>
       </c>
@@ -3790,7 +3886,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:17">
       <c r="A61" s="3" t="s">
         <v>24</v>
       </c>
@@ -3813,7 +3909,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:17">
       <c r="A62" s="3" t="s">
         <v>24</v>
       </c>
@@ -3833,7 +3929,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:17">
       <c r="A63" s="3" t="s">
         <v>24</v>
       </c>
@@ -3853,7 +3949,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:17">
       <c r="A64" s="3" t="s">
         <v>24</v>
       </c>
@@ -3873,7 +3969,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:17">
       <c r="A65" s="3" t="s">
         <v>24</v>
       </c>
@@ -3893,7 +3989,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:17">
       <c r="A66" s="3" t="s">
         <v>24</v>
       </c>
@@ -3913,7 +4009,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:17">
       <c r="A67" s="3" t="s">
         <v>24</v>
       </c>
@@ -3933,7 +4029,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:17">
       <c r="A68" s="3" t="s">
         <v>24</v>
       </c>
@@ -3953,7 +4049,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:17">
       <c r="A69" s="3" t="s">
         <v>24</v>
       </c>
@@ -3973,7 +4069,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:17">
       <c r="A70" s="3" t="s">
         <v>24</v>
       </c>
@@ -3993,7 +4089,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:17">
       <c r="A71" s="3" t="s">
         <v>24</v>
       </c>
@@ -4013,7 +4109,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:17">
       <c r="A72" s="3" t="s">
         <v>24</v>
       </c>
@@ -4030,7 +4126,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:17">
       <c r="A73" s="3" t="s">
         <v>24</v>
       </c>
@@ -4047,7 +4143,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:17">
       <c r="A74" s="3" t="s">
         <v>24</v>
       </c>
@@ -4067,7 +4163,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:17">
       <c r="A75" s="3" t="s">
         <v>24</v>
       </c>
@@ -4087,7 +4183,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:17">
       <c r="A76" s="3" t="s">
         <v>24</v>
       </c>
@@ -4107,7 +4203,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:17">
       <c r="A77" s="3" t="s">
         <v>24</v>
       </c>
@@ -4153,8 +4249,11 @@
       <c r="P77" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="78" spans="1:16">
+      <c r="Q77" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
       <c r="A78" s="3" t="s">
         <v>24</v>
       </c>
@@ -4177,7 +4276,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:17">
       <c r="A79" s="3" t="s">
         <v>24</v>
       </c>
@@ -4206,7 +4305,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:17">
       <c r="A80" s="3" t="s">
         <v>24</v>
       </c>
@@ -4537,7 +4636,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:17">
       <c r="A97" s="3" t="s">
         <v>24</v>
       </c>
@@ -4584,7 +4683,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:17">
       <c r="A98" s="3" t="s">
         <v>24</v>
       </c>
@@ -4607,7 +4706,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:17">
       <c r="A99" s="3" t="s">
         <v>24</v>
       </c>
@@ -4633,7 +4732,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:17">
       <c r="A100" s="3" t="s">
         <v>24</v>
       </c>
@@ -4665,7 +4764,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:17">
       <c r="A101" s="3" t="s">
         <v>24</v>
       </c>
@@ -4709,7 +4808,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:17">
       <c r="A102" s="3" t="s">
         <v>24</v>
       </c>
@@ -4720,7 +4819,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:17">
       <c r="A103" s="3" t="s">
         <v>24</v>
       </c>
@@ -4769,8 +4868,11 @@
       <c r="P103" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="104" spans="1:16">
+      <c r="Q103" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17">
       <c r="A104" s="3" t="s">
         <v>24</v>
       </c>
@@ -4814,7 +4916,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:17">
       <c r="A105" s="3" t="s">
         <v>24</v>
       </c>
@@ -4849,7 +4951,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:17">
       <c r="A106" s="3" t="s">
         <v>24</v>
       </c>
@@ -4875,7 +4977,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:17">
       <c r="A107" s="3" t="s">
         <v>24</v>
       </c>
@@ -4904,7 +5006,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:17">
       <c r="A108" s="3" t="s">
         <v>24</v>
       </c>
@@ -4930,7 +5032,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:17">
       <c r="A109" s="3" t="s">
         <v>24</v>
       </c>
@@ -4950,7 +5052,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:17">
       <c r="A110" s="3" t="s">
         <v>24</v>
       </c>
@@ -4970,7 +5072,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:17">
       <c r="A111" s="3" t="s">
         <v>24</v>
       </c>
@@ -4984,7 +5086,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:17">
       <c r="A112" s="3" t="s">
         <v>24</v>
       </c>
@@ -5028,102 +5130,73 @@
         <v>448</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:17">
       <c r="A113" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B113" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N113" s="10"/>
+      <c r="O113" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17">
+      <c r="A114" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C113" s="6" t="s">
+      <c r="C114" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D114" t="s">
         <v>92</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E114" t="s">
         <v>49</v>
       </c>
-      <c r="H113" t="s">
-        <v>201</v>
-      </c>
-      <c r="I113" t="s">
+      <c r="H114" t="s">
+        <v>201</v>
+      </c>
+      <c r="I114" t="s">
         <v>274</v>
       </c>
-      <c r="J113" t="s">
+      <c r="J114" t="s">
         <v>204</v>
       </c>
-      <c r="K113" t="s">
+      <c r="K114" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
-      <c r="A114" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B114" s="3" t="s">
+    <row r="115" spans="1:17">
+      <c r="A115" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B115" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
-      <c r="A115" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B115" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D115" t="s">
-        <v>71</v>
-      </c>
-      <c r="E115" t="s">
-        <v>49</v>
-      </c>
-      <c r="F115" t="s">
-        <v>154</v>
-      </c>
-      <c r="G115" t="s">
-        <v>148</v>
-      </c>
-      <c r="H115" t="s">
-        <v>201</v>
-      </c>
-      <c r="I115" t="s">
-        <v>275</v>
-      </c>
-      <c r="J115" t="s">
-        <v>204</v>
-      </c>
-      <c r="K115" t="s">
-        <v>218</v>
-      </c>
-      <c r="L115" t="s">
-        <v>315</v>
-      </c>
-      <c r="M115" t="s">
-        <v>385</v>
-      </c>
-      <c r="N115" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="O115" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="P115" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:17">
       <c r="A116" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B116" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C116" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D116" t="s">
+        <v>71</v>
+      </c>
+      <c r="E116" t="s">
+        <v>49</v>
+      </c>
       <c r="F116" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G116" t="s">
         <v>148</v>
@@ -5132,7 +5205,7 @@
         <v>201</v>
       </c>
       <c r="I116" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J116" t="s">
         <v>204</v>
@@ -5141,13 +5214,25 @@
         <v>218</v>
       </c>
       <c r="L116" t="s">
-        <v>449</v>
-      </c>
-      <c r="O116" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16">
+        <v>315</v>
+      </c>
+      <c r="M116" t="s">
+        <v>385</v>
+      </c>
+      <c r="N116" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="O116" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="P116" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q116" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17">
       <c r="A117" s="3" t="s">
         <v>24</v>
       </c>
@@ -5155,7 +5240,7 @@
         <v>32</v>
       </c>
       <c r="F117" t="s">
-        <v>363</v>
+        <v>155</v>
       </c>
       <c r="G117" t="s">
         <v>148</v>
@@ -5163,28 +5248,31 @@
       <c r="H117" t="s">
         <v>201</v>
       </c>
+      <c r="I117" t="s">
+        <v>276</v>
+      </c>
+      <c r="J117" t="s">
+        <v>204</v>
+      </c>
+      <c r="K117" t="s">
+        <v>218</v>
+      </c>
+      <c r="L117" t="s">
+        <v>449</v>
+      </c>
       <c r="O117" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17">
       <c r="A118" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D118" t="s">
-        <v>70</v>
-      </c>
-      <c r="E118" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F118" t="s">
-        <v>153</v>
+        <v>363</v>
       </c>
       <c r="G118" t="s">
         <v>148</v>
@@ -5192,43 +5280,28 @@
       <c r="H118" t="s">
         <v>201</v>
       </c>
-      <c r="I118" t="s">
-        <v>277</v>
-      </c>
-      <c r="J118" t="s">
-        <v>204</v>
-      </c>
-      <c r="K118" t="s">
-        <v>218</v>
-      </c>
-      <c r="L118" t="s">
-        <v>334</v>
-      </c>
-      <c r="M118" t="s">
-        <v>381</v>
-      </c>
       <c r="O118" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
       <c r="A119" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C119" s="6">
-        <v>253</v>
+      <c r="C119" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D119" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E119" t="s">
         <v>49</v>
       </c>
       <c r="F119" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
       <c r="G119" t="s">
         <v>148</v>
@@ -5237,7 +5310,7 @@
         <v>201</v>
       </c>
       <c r="I119" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J119" t="s">
         <v>204</v>
@@ -5245,16 +5318,40 @@
       <c r="K119" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="120" spans="1:16">
+      <c r="L119" t="s">
+        <v>334</v>
+      </c>
+      <c r="M119" t="s">
+        <v>381</v>
+      </c>
+      <c r="O119" t="s">
+        <v>543</v>
+      </c>
+      <c r="P119" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17">
       <c r="A120" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C120" s="6">
+        <v>253</v>
+      </c>
+      <c r="D120" t="s">
+        <v>90</v>
+      </c>
+      <c r="E120" t="s">
+        <v>49</v>
+      </c>
       <c r="F120" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="G120" t="s">
         <v>148</v>
@@ -5263,27 +5360,24 @@
         <v>201</v>
       </c>
       <c r="I120" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16">
+        <v>278</v>
+      </c>
+      <c r="J120" t="s">
+        <v>204</v>
+      </c>
+      <c r="K120" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17">
       <c r="A121" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C121" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D121" t="s">
-        <v>34</v>
-      </c>
-      <c r="E121" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F121" t="s">
-        <v>475</v>
+        <v>196</v>
       </c>
       <c r="G121" t="s">
         <v>148</v>
@@ -5292,88 +5386,82 @@
         <v>201</v>
       </c>
       <c r="I121" t="s">
-        <v>34</v>
-      </c>
-      <c r="J121" t="s">
-        <v>204</v>
-      </c>
-      <c r="K121" t="s">
-        <v>213</v>
-      </c>
-      <c r="L121" t="s">
-        <v>463</v>
-      </c>
-      <c r="M121" t="s">
-        <v>34</v>
-      </c>
-      <c r="O121" s="10" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17">
       <c r="A122" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B122" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C122" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D122" t="s">
+        <v>34</v>
+      </c>
+      <c r="E122" t="s">
+        <v>49</v>
+      </c>
+      <c r="F122" t="s">
+        <v>475</v>
+      </c>
+      <c r="G122" t="s">
+        <v>148</v>
+      </c>
+      <c r="H122" t="s">
+        <v>201</v>
+      </c>
+      <c r="I122" t="s">
+        <v>34</v>
+      </c>
+      <c r="J122" t="s">
+        <v>204</v>
+      </c>
+      <c r="K122" t="s">
+        <v>213</v>
+      </c>
+      <c r="L122" t="s">
+        <v>463</v>
+      </c>
+      <c r="M122" t="s">
+        <v>34</v>
+      </c>
       <c r="O122" s="10" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17">
+      <c r="A123" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O123" s="10" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
-      <c r="A123" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D123" t="s">
-        <v>89</v>
-      </c>
-      <c r="E123" t="s">
-        <v>49</v>
-      </c>
-      <c r="F123" t="s">
-        <v>195</v>
-      </c>
-      <c r="G123" t="s">
-        <v>148</v>
-      </c>
-      <c r="H123" t="s">
-        <v>201</v>
-      </c>
-      <c r="I123" t="s">
-        <v>280</v>
-      </c>
-      <c r="J123" t="s">
-        <v>204</v>
-      </c>
-      <c r="K123" t="s">
-        <v>213</v>
-      </c>
-      <c r="L123" t="s">
-        <v>462</v>
-      </c>
-      <c r="M123" t="s">
-        <v>380</v>
-      </c>
-      <c r="O123" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:17">
       <c r="A124" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B124" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C124" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D124" t="s">
+        <v>89</v>
+      </c>
+      <c r="E124" t="s">
+        <v>49</v>
+      </c>
       <c r="F124" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G124" t="s">
         <v>148</v>
@@ -5382,19 +5470,25 @@
         <v>201</v>
       </c>
       <c r="I124" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J124" t="s">
         <v>204</v>
       </c>
       <c r="K124" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="L124" t="s">
+        <v>462</v>
+      </c>
+      <c r="M124" t="s">
+        <v>380</v>
       </c>
       <c r="O124" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
       <c r="A125" s="3" t="s">
         <v>24</v>
       </c>
@@ -5402,7 +5496,7 @@
         <v>35</v>
       </c>
       <c r="F125" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G125" t="s">
         <v>148</v>
@@ -5410,43 +5504,37 @@
       <c r="H125" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="126" spans="1:16">
+      <c r="I125" t="s">
+        <v>281</v>
+      </c>
+      <c r="J125" t="s">
+        <v>204</v>
+      </c>
+      <c r="K125" t="s">
+        <v>218</v>
+      </c>
+      <c r="O125" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
       <c r="A126" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C126" s="6">
-        <v>311</v>
-      </c>
-      <c r="D126" t="s">
-        <v>75</v>
-      </c>
-      <c r="E126" t="s">
-        <v>51</v>
-      </c>
-      <c r="I126" t="s">
-        <v>282</v>
-      </c>
-      <c r="J126" t="s">
-        <v>204</v>
-      </c>
-      <c r="K126" t="s">
-        <v>218</v>
-      </c>
-      <c r="M126" t="s">
-        <v>376</v>
-      </c>
-      <c r="O126" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="P126" t="s">
-        <v>528</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16">
+        <v>35</v>
+      </c>
+      <c r="F126" t="s">
+        <v>192</v>
+      </c>
+      <c r="G126" t="s">
+        <v>148</v>
+      </c>
+      <c r="H126" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17">
       <c r="A127" s="3" t="s">
         <v>24</v>
       </c>
@@ -5454,90 +5542,102 @@
         <v>36</v>
       </c>
       <c r="C127" s="6">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D127" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="E127" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="128" spans="1:16">
+      <c r="I127" t="s">
+        <v>282</v>
+      </c>
+      <c r="J127" t="s">
+        <v>204</v>
+      </c>
+      <c r="K127" t="s">
+        <v>218</v>
+      </c>
+      <c r="M127" t="s">
+        <v>376</v>
+      </c>
+      <c r="O127" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="P127" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17">
       <c r="A128" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B128" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C128" s="6">
+        <v>312</v>
+      </c>
+      <c r="D128" t="s">
+        <v>135</v>
+      </c>
+      <c r="E128" t="s">
+        <v>51</v>
+      </c>
+      <c r="O128" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
+      <c r="A129" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B129" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="C128" s="6" t="s">
+      <c r="C129" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D129" t="s">
         <v>304</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E129" t="s">
         <v>49</v>
       </c>
-      <c r="M128" t="s">
+      <c r="M129" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
-      <c r="A129" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B129" s="3" t="s">
+    <row r="130" spans="1:17">
+      <c r="A130" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B130" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="M129" t="s">
+      <c r="M130" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
-      <c r="A130" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B130" s="3" t="s">
+    <row r="131" spans="1:17">
+      <c r="A131" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B131" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="C130" s="6" t="s">
+      <c r="C131" s="6" t="s">
         <v>307</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
         <v>306</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E131" t="s">
         <v>49</v>
       </c>
-      <c r="F130" t="s">
+      <c r="F131" t="s">
         <v>188</v>
-      </c>
-      <c r="G130" t="s">
-        <v>148</v>
-      </c>
-      <c r="H130" t="s">
-        <v>201</v>
-      </c>
-      <c r="I130" t="s">
-        <v>353</v>
-      </c>
-      <c r="J130" t="s">
-        <v>204</v>
-      </c>
-      <c r="K130" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="131" spans="1:16">
-      <c r="A131" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B131" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="F131" t="s">
-        <v>344</v>
       </c>
       <c r="G131" t="s">
         <v>148</v>
@@ -5545,19 +5645,25 @@
       <c r="H131" t="s">
         <v>201</v>
       </c>
-      <c r="L131" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="132" spans="1:16">
+      <c r="I131" t="s">
+        <v>353</v>
+      </c>
+      <c r="J131" t="s">
+        <v>204</v>
+      </c>
+      <c r="K131" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
       <c r="A132" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>455</v>
+        <v>345</v>
       </c>
       <c r="F132" t="s">
-        <v>472</v>
+        <v>344</v>
       </c>
       <c r="G132" t="s">
         <v>148</v>
@@ -5565,31 +5671,28 @@
       <c r="H132" t="s">
         <v>201</v>
       </c>
-      <c r="I132" t="s">
+      <c r="L132" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17">
+      <c r="A133" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F133" t="s">
+        <v>472</v>
+      </c>
+      <c r="G133" t="s">
+        <v>148</v>
+      </c>
+      <c r="H133" t="s">
+        <v>201</v>
+      </c>
+      <c r="I133" t="s">
         <v>488</v>
-      </c>
-      <c r="J132" t="s">
-        <v>204</v>
-      </c>
-      <c r="K132" t="s">
-        <v>218</v>
-      </c>
-      <c r="L132" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="133" spans="1:16">
-      <c r="A133" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="H133" t="s">
-        <v>201</v>
-      </c>
-      <c r="I133" t="s">
-        <v>283</v>
       </c>
       <c r="J133" t="s">
         <v>204</v>
@@ -5597,135 +5700,102 @@
       <c r="K133" t="s">
         <v>218</v>
       </c>
-      <c r="M133" t="s">
-        <v>287</v>
-      </c>
-      <c r="N133" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="O133" s="10" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="134" spans="1:16">
+      <c r="L133" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17">
       <c r="A134" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B134" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="N134" s="10"/>
+      <c r="H134" t="s">
+        <v>201</v>
+      </c>
+      <c r="I134" t="s">
+        <v>283</v>
+      </c>
+      <c r="J134" t="s">
+        <v>204</v>
+      </c>
+      <c r="K134" t="s">
+        <v>218</v>
+      </c>
+      <c r="M134" t="s">
+        <v>287</v>
+      </c>
+      <c r="N134" s="10" t="s">
+        <v>287</v>
+      </c>
       <c r="O134" s="10" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17">
+      <c r="A135" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="N135" s="10"/>
+      <c r="O135" s="10" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
-      <c r="A135" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B135" s="3" t="s">
+    <row r="136" spans="1:17">
+      <c r="A136" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B136" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="M135" t="s">
+      <c r="M136" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
-      <c r="A136" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B136" s="3" t="s">
+    <row r="137" spans="1:17">
+      <c r="A137" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B137" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="F136" t="s">
+      <c r="F137" t="s">
         <v>470</v>
       </c>
-      <c r="G136" t="s">
+      <c r="G137" t="s">
         <v>148</v>
       </c>
-      <c r="H136" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="137" spans="1:16">
-      <c r="A137" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B137" s="3" t="s">
+      <c r="H137" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17">
+      <c r="A138" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B138" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="O137" t="s">
+      <c r="O138" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
-      <c r="A138" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B138" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C138" s="6">
-        <v>511</v>
-      </c>
-      <c r="D138" t="s">
-        <v>81</v>
-      </c>
-      <c r="E138" t="s">
-        <v>50</v>
-      </c>
-      <c r="F138" t="s">
-        <v>181</v>
-      </c>
-      <c r="G138" t="s">
-        <v>186</v>
-      </c>
-      <c r="H138" t="s">
-        <v>201</v>
-      </c>
-      <c r="J138" t="s">
-        <v>206</v>
-      </c>
-      <c r="K138" t="s">
-        <v>217</v>
-      </c>
-      <c r="L138" t="s">
-        <v>313</v>
-      </c>
-      <c r="P138" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="139" spans="1:16">
-      <c r="A139" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F139" t="s">
-        <v>179</v>
-      </c>
-      <c r="G139" t="s">
-        <v>186</v>
-      </c>
-      <c r="H139" t="s">
-        <v>201</v>
-      </c>
-      <c r="I139" t="s">
-        <v>284</v>
-      </c>
-      <c r="J139" t="s">
-        <v>206</v>
-      </c>
-      <c r="K139" t="s">
-        <v>217</v>
-      </c>
-      <c r="L139" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="140" spans="1:16">
+    <row r="139" spans="1:17">
+      <c r="A139" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q139" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17">
       <c r="A140" s="4" t="s">
         <v>37</v>
       </c>
@@ -5733,16 +5803,16 @@
         <v>38</v>
       </c>
       <c r="C140" s="6">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D140" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E140" t="s">
         <v>50</v>
       </c>
       <c r="F140" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G140" t="s">
         <v>186</v>
@@ -5750,9 +5820,6 @@
       <c r="H140" t="s">
         <v>201</v>
       </c>
-      <c r="I140" t="s">
-        <v>285</v>
-      </c>
       <c r="J140" t="s">
         <v>206</v>
       </c>
@@ -5760,10 +5827,16 @@
         <v>217</v>
       </c>
       <c r="L140" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="141" spans="1:16">
+        <v>313</v>
+      </c>
+      <c r="P140" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q140" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17">
       <c r="A141" s="4" t="s">
         <v>37</v>
       </c>
@@ -5771,7 +5844,7 @@
         <v>38</v>
       </c>
       <c r="F141" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G141" t="s">
         <v>186</v>
@@ -5780,7 +5853,7 @@
         <v>201</v>
       </c>
       <c r="I141" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J141" t="s">
         <v>206</v>
@@ -5789,18 +5862,27 @@
         <v>217</v>
       </c>
       <c r="L141" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="142" spans="1:16">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17">
       <c r="A142" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B142" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C142" s="6">
+        <v>513</v>
+      </c>
+      <c r="D142" t="s">
+        <v>82</v>
+      </c>
+      <c r="E142" t="s">
+        <v>50</v>
+      </c>
       <c r="F142" t="s">
-        <v>37</v>
+        <v>177</v>
       </c>
       <c r="G142" t="s">
         <v>186</v>
@@ -5809,19 +5891,19 @@
         <v>201</v>
       </c>
       <c r="I142" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J142" t="s">
         <v>206</v>
       </c>
       <c r="K142" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="L142" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="143" spans="1:16">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17">
       <c r="A143" s="4" t="s">
         <v>37</v>
       </c>
@@ -5829,7 +5911,7 @@
         <v>38</v>
       </c>
       <c r="F143" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G143" t="s">
         <v>186</v>
@@ -5838,7 +5920,7 @@
         <v>201</v>
       </c>
       <c r="I143" t="s">
-        <v>38</v>
+        <v>286</v>
       </c>
       <c r="J143" t="s">
         <v>206</v>
@@ -5847,10 +5929,10 @@
         <v>217</v>
       </c>
       <c r="L143" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="144" spans="1:16" ht="17" customHeight="1">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17">
       <c r="A144" s="4" t="s">
         <v>37</v>
       </c>
@@ -5858,7 +5940,7 @@
         <v>38</v>
       </c>
       <c r="F144" t="s">
-        <v>357</v>
+        <v>37</v>
       </c>
       <c r="G144" t="s">
         <v>186</v>
@@ -5867,16 +5949,19 @@
         <v>201</v>
       </c>
       <c r="I144" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J144" t="s">
         <v>206</v>
       </c>
       <c r="K144" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="145" spans="1:16" ht="17" customHeight="1">
+        <v>213</v>
+      </c>
+      <c r="L144" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17">
       <c r="A145" s="4" t="s">
         <v>37</v>
       </c>
@@ -5884,7 +5969,7 @@
         <v>38</v>
       </c>
       <c r="F145" t="s">
-        <v>473</v>
+        <v>182</v>
       </c>
       <c r="G145" t="s">
         <v>186</v>
@@ -5893,7 +5978,7 @@
         <v>201</v>
       </c>
       <c r="I145" t="s">
-        <v>289</v>
+        <v>38</v>
       </c>
       <c r="J145" t="s">
         <v>206</v>
@@ -5901,8 +5986,11 @@
       <c r="K145" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="146" spans="1:16" ht="17" customHeight="1">
+      <c r="L145" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17" ht="17" customHeight="1">
       <c r="A146" s="4" t="s">
         <v>37</v>
       </c>
@@ -5910,7 +5998,7 @@
         <v>38</v>
       </c>
       <c r="F146" t="s">
-        <v>474</v>
+        <v>357</v>
       </c>
       <c r="G146" t="s">
         <v>186</v>
@@ -5919,7 +6007,7 @@
         <v>201</v>
       </c>
       <c r="I146" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="J146" t="s">
         <v>206</v>
@@ -5928,18 +6016,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="17" customHeight="1">
+    <row r="147" spans="1:17" ht="17" customHeight="1">
       <c r="A147" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F147" t="s">
+        <v>473</v>
+      </c>
+      <c r="G147" t="s">
+        <v>186</v>
+      </c>
       <c r="H147" t="s">
         <v>201</v>
       </c>
       <c r="I147" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J147" t="s">
         <v>206</v>
@@ -5948,7 +6042,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="17" customHeight="1">
+    <row r="148" spans="1:17" ht="17" customHeight="1">
       <c r="A148" s="4" t="s">
         <v>37</v>
       </c>
@@ -5956,7 +6050,7 @@
         <v>38</v>
       </c>
       <c r="F148" t="s">
-        <v>180</v>
+        <v>474</v>
       </c>
       <c r="G148" t="s">
         <v>186</v>
@@ -5965,7 +6059,7 @@
         <v>201</v>
       </c>
       <c r="I148" t="s">
-        <v>487</v>
+        <v>290</v>
       </c>
       <c r="J148" t="s">
         <v>206</v>
@@ -5974,24 +6068,18 @@
         <v>217</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="17" customHeight="1">
+    <row r="149" spans="1:17" ht="17" customHeight="1">
       <c r="A149" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F149" t="s">
-        <v>184</v>
-      </c>
-      <c r="G149" t="s">
-        <v>186</v>
-      </c>
       <c r="H149" t="s">
         <v>201</v>
       </c>
       <c r="I149" t="s">
-        <v>212</v>
+        <v>291</v>
       </c>
       <c r="J149" t="s">
         <v>206</v>
@@ -6000,18 +6088,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="17" customHeight="1">
+    <row r="150" spans="1:17" ht="17" customHeight="1">
       <c r="A150" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F150" t="s">
+        <v>180</v>
+      </c>
+      <c r="G150" t="s">
+        <v>186</v>
+      </c>
       <c r="H150" t="s">
         <v>201</v>
       </c>
       <c r="I150" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="J150" t="s">
         <v>206</v>
@@ -6020,18 +6114,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="17" customHeight="1">
+    <row r="151" spans="1:17" ht="17" customHeight="1">
       <c r="A151" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F151" t="s">
+        <v>184</v>
+      </c>
+      <c r="G151" t="s">
+        <v>186</v>
+      </c>
       <c r="H151" t="s">
         <v>201</v>
       </c>
       <c r="I151" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="J151" t="s">
         <v>206</v>
@@ -6040,24 +6140,18 @@
         <v>217</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:17" ht="17" customHeight="1">
       <c r="A152" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B152" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F152" t="s">
-        <v>175</v>
-      </c>
-      <c r="G152" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
       <c r="H152" t="s">
         <v>201</v>
       </c>
       <c r="I152" t="s">
-        <v>293</v>
+        <v>489</v>
       </c>
       <c r="J152" t="s">
         <v>206</v>
@@ -6065,31 +6159,19 @@
       <c r="K152" t="s">
         <v>217</v>
       </c>
-      <c r="L152" t="s">
-        <v>458</v>
-      </c>
-      <c r="P152" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="153" spans="1:16">
+    </row>
+    <row r="153" spans="1:17" ht="17" customHeight="1">
       <c r="A153" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F153" t="s">
-        <v>362</v>
-      </c>
-      <c r="G153" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
       <c r="H153" t="s">
         <v>201</v>
       </c>
       <c r="I153" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="J153" t="s">
         <v>206</v>
@@ -6098,18 +6180,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:17">
       <c r="A154" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F154" t="s">
+        <v>175</v>
+      </c>
+      <c r="G154" t="s">
+        <v>186</v>
+      </c>
       <c r="H154" t="s">
         <v>201</v>
       </c>
       <c r="I154" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="J154" t="s">
         <v>206</v>
@@ -6117,16 +6205,25 @@
       <c r="K154" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="155" spans="1:16">
+      <c r="L154" t="s">
+        <v>458</v>
+      </c>
+      <c r="P154" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q154" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17">
       <c r="A155" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F155" t="s">
-        <v>178</v>
+        <v>362</v>
       </c>
       <c r="G155" t="s">
         <v>186</v>
@@ -6135,7 +6232,7 @@
         <v>201</v>
       </c>
       <c r="I155" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J155" t="s">
         <v>206</v>
@@ -6143,28 +6240,19 @@
       <c r="K155" t="s">
         <v>217</v>
       </c>
-      <c r="L155" t="s">
-        <v>459</v>
-      </c>
-      <c r="P155" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="156" spans="1:16">
+    </row>
+    <row r="156" spans="1:17">
       <c r="A156" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F156" t="s">
-        <v>360</v>
+        <v>39</v>
       </c>
       <c r="H156" t="s">
         <v>201</v>
       </c>
       <c r="I156" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="J156" t="s">
         <v>206</v>
@@ -6173,15 +6261,15 @@
         <v>217</v>
       </c>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:17">
       <c r="A157" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>533</v>
+        <v>40</v>
       </c>
       <c r="F157" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G157" t="s">
         <v>186</v>
@@ -6190,7 +6278,7 @@
         <v>201</v>
       </c>
       <c r="I157" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="J157" t="s">
         <v>206</v>
@@ -6199,30 +6287,30 @@
         <v>217</v>
       </c>
       <c r="L157" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="P157" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="158" spans="1:16">
+        <v>531</v>
+      </c>
+      <c r="Q157" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17">
       <c r="A158" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>533</v>
+        <v>40</v>
       </c>
       <c r="F158" t="s">
-        <v>471</v>
-      </c>
-      <c r="G158" t="s">
-        <v>186</v>
+        <v>360</v>
       </c>
       <c r="H158" t="s">
         <v>201</v>
       </c>
       <c r="I158" t="s">
-        <v>41</v>
+        <v>297</v>
       </c>
       <c r="J158" t="s">
         <v>206</v>
@@ -6231,18 +6319,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:17">
       <c r="A159" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>533</v>
       </c>
+      <c r="F159" t="s">
+        <v>174</v>
+      </c>
+      <c r="G159" t="s">
+        <v>186</v>
+      </c>
       <c r="H159" t="s">
         <v>201</v>
       </c>
       <c r="I159" t="s">
-        <v>211</v>
+        <v>298</v>
       </c>
       <c r="J159" t="s">
         <v>206</v>
@@ -6250,19 +6344,34 @@
       <c r="K159" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="160" spans="1:16">
+      <c r="L159" t="s">
+        <v>452</v>
+      </c>
+      <c r="P159" t="s">
+        <v>532</v>
+      </c>
+      <c r="Q159" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17">
       <c r="A160" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>533</v>
       </c>
+      <c r="F160" t="s">
+        <v>471</v>
+      </c>
+      <c r="G160" t="s">
+        <v>186</v>
+      </c>
       <c r="H160" t="s">
         <v>201</v>
       </c>
       <c r="I160" t="s">
-        <v>299</v>
+        <v>41</v>
       </c>
       <c r="J160" t="s">
         <v>206</v>
@@ -6271,33 +6380,18 @@
         <v>217</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:17">
       <c r="A161" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C161" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="D161" t="s">
-        <v>467</v>
-      </c>
-      <c r="E161" t="s">
-        <v>50</v>
-      </c>
-      <c r="F161" t="s">
-        <v>185</v>
-      </c>
-      <c r="G161" t="s">
-        <v>186</v>
+        <v>533</v>
       </c>
       <c r="H161" t="s">
         <v>201</v>
       </c>
       <c r="I161" t="s">
-        <v>300</v>
+        <v>211</v>
       </c>
       <c r="J161" t="s">
         <v>206</v>
@@ -6306,156 +6400,244 @@
         <v>217</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:17">
       <c r="A162" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B162" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="H162" t="s">
+        <v>201</v>
+      </c>
+      <c r="I162" t="s">
+        <v>299</v>
+      </c>
+      <c r="J162" t="s">
+        <v>206</v>
+      </c>
+      <c r="K162" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17">
+      <c r="A163" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17">
+      <c r="A164" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17">
+      <c r="A165" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q165" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" ht="17" customHeight="1">
+      <c r="A166" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B166" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F162" t="s">
+      <c r="C166" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="D166" t="s">
+        <v>467</v>
+      </c>
+      <c r="E166" t="s">
+        <v>50</v>
+      </c>
+      <c r="F166" t="s">
+        <v>185</v>
+      </c>
+      <c r="G166" t="s">
+        <v>186</v>
+      </c>
+      <c r="H166" t="s">
+        <v>201</v>
+      </c>
+      <c r="I166" t="s">
+        <v>300</v>
+      </c>
+      <c r="J166" t="s">
+        <v>206</v>
+      </c>
+      <c r="K166" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17">
+      <c r="A167" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F167" t="s">
         <v>183</v>
       </c>
-      <c r="G162" t="s">
+      <c r="G167" t="s">
         <v>186</v>
       </c>
-      <c r="H162" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="163" spans="1:11">
-      <c r="A163" s="5" t="s">
+      <c r="H167" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17">
+      <c r="A168" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B168" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E168" t="s">
         <v>52</v>
       </c>
-      <c r="H163" t="s">
+      <c r="H168" t="s">
         <v>200</v>
       </c>
-      <c r="I163" t="s">
+      <c r="I168" t="s">
         <v>301</v>
       </c>
-      <c r="J163" t="s">
+      <c r="J168" t="s">
         <v>209</v>
       </c>
-      <c r="K163" t="s">
+      <c r="K168" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
-      <c r="A164" s="5" t="s">
+    <row r="169" spans="1:17">
+      <c r="A169" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B169" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H164" t="s">
+      <c r="H169" t="s">
         <v>200</v>
       </c>
-      <c r="I164" t="s">
+      <c r="I169" t="s">
         <v>208</v>
       </c>
-      <c r="J164" t="s">
+      <c r="J169" t="s">
         <v>209</v>
       </c>
-      <c r="K164" t="s">
+      <c r="K169" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
-      <c r="A165" s="5" t="s">
+    <row r="170" spans="1:17">
+      <c r="A170" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B170" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C165" s="6" t="s">
+      <c r="C170" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D165" t="s">
+      <c r="D170" t="s">
         <v>45</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E170" t="s">
         <v>52</v>
       </c>
-      <c r="F165" t="s">
+      <c r="F170" t="s">
         <v>161</v>
       </c>
-      <c r="G165" t="s">
+      <c r="G170" t="s">
         <v>173</v>
       </c>
-      <c r="H165" t="s">
+      <c r="H170" t="s">
         <v>200</v>
       </c>
-      <c r="I165" t="s">
+      <c r="I170" t="s">
         <v>45</v>
       </c>
-      <c r="J165" t="s">
+      <c r="J170" t="s">
         <v>209</v>
       </c>
-      <c r="K165" t="s">
+      <c r="K170" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
-      <c r="A166" s="5" t="s">
+    <row r="171" spans="1:17">
+      <c r="A171" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B171" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C166" s="6" t="s">
+      <c r="C171" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D171" t="s">
         <v>91</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E171" t="s">
         <v>52</v>
       </c>
-      <c r="H166" t="s">
+      <c r="H171" t="s">
         <v>200</v>
       </c>
-      <c r="I166" t="s">
+      <c r="I171" t="s">
         <v>302</v>
       </c>
-      <c r="J166" t="s">
+      <c r="J171" t="s">
         <v>209</v>
       </c>
-      <c r="K166" t="s">
+      <c r="K171" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
-      <c r="A167" s="5" t="s">
+    <row r="172" spans="1:17">
+      <c r="A172" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B172" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C167" s="6" t="s">
+      <c r="C172" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D167" t="s">
+      <c r="D172" t="s">
         <v>47</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E172" t="s">
         <v>52</v>
       </c>
-      <c r="H167" t="s">
+      <c r="H172" t="s">
         <v>200</v>
       </c>
-      <c r="I167" t="s">
+      <c r="I172" t="s">
         <v>303</v>
       </c>
-      <c r="J167" t="s">
+      <c r="J172" t="s">
         <v>209</v>
       </c>
-      <c r="K167" t="s">
+      <c r="K172" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated the li raw claim benefit logic
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/RawClaimMCR-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4962E7-3DC1-F845-B10F-59E8851B2440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A54AC04-F80E-694D-B1D8-47469EAF3386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18340" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="20060" yWindow="-20900" windowWidth="38400" windowHeight="19900" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="576">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1589,15 +1589,6 @@
     <t>SURGEON'S FEE</t>
   </si>
   <si>
-    <t>Surgeon Fee - Non Classified (AXA/ Sunlife/ Manulife)</t>
-  </si>
-  <si>
-    <t>Anaesthetist's Fees - Non Classified (AXA/ Sunlife/ Manulife)</t>
-  </si>
-  <si>
-    <t>Operation Theatre Fees - Non Classified (AXA/ Sunlife/ Manulife)</t>
-  </si>
-  <si>
     <t>ANAESTHETIST'S FEE</t>
   </si>
   <si>
@@ -1743,6 +1734,36 @@
   </si>
   <si>
     <t>EYE</t>
+  </si>
+  <si>
+    <t>CHBSA</t>
+  </si>
+  <si>
+    <t>HSS</t>
+  </si>
+  <si>
+    <t>Inpatient Speical Services (Liberty)</t>
+  </si>
+  <si>
+    <t>PNC</t>
+  </si>
+  <si>
+    <t>VACC-1</t>
+  </si>
+  <si>
+    <t>CHBS</t>
+  </si>
+  <si>
+    <t>HSP</t>
+  </si>
+  <si>
+    <t>Surgeon Fee - Non Classified (AXA/ Sunlife/ Manulife/ Liberty)</t>
+  </si>
+  <si>
+    <t>Anaesthetist's Fees - Non Classified (AXA/ Sunlife/ Manulife/ Liberty)</t>
+  </si>
+  <si>
+    <t>Operation Theatre Fees - Non Classified (AXA/ Sunlife/ Manulife/ Liberty)</t>
   </si>
 </sst>
 </file>
@@ -2177,13 +2198,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:Q172"/>
+  <dimension ref="A1:Q173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J103" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O113" sqref="O113"/>
+      <selection pane="bottomRight" activeCell="Q32" sqref="Q32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2251,7 +2272,7 @@
         <v>513</v>
       </c>
       <c r="Q1" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" customHeight="1">
@@ -2304,7 +2325,7 @@
         <v>156</v>
       </c>
       <c r="Q2" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="17" customHeight="1">
@@ -2389,7 +2410,7 @@
         <v>514</v>
       </c>
       <c r="Q4" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -2471,7 +2492,7 @@
         <v>515</v>
       </c>
       <c r="Q6" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -2804,7 +2825,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>517</v>
+        <v>573</v>
       </c>
       <c r="F20" t="s">
         <v>157</v>
@@ -2819,7 +2840,7 @@
         <v>516</v>
       </c>
       <c r="Q20" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -2827,7 +2848,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>517</v>
+        <v>573</v>
       </c>
       <c r="O21" t="s">
         <v>506</v>
@@ -2966,7 +2987,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>518</v>
+        <v>574</v>
       </c>
       <c r="F26" t="s">
         <v>158</v>
@@ -2979,10 +3000,10 @@
         <v>444</v>
       </c>
       <c r="P26" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="Q26" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -2990,7 +3011,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>518</v>
+        <v>574</v>
       </c>
       <c r="N27" s="10"/>
       <c r="O27" t="s">
@@ -3187,7 +3208,7 @@
         <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>519</v>
+        <v>575</v>
       </c>
       <c r="F35" t="s">
         <v>159</v>
@@ -3199,7 +3220,7 @@
         <v>441</v>
       </c>
       <c r="P35" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="Q35" t="s">
         <v>159</v>
@@ -3210,7 +3231,7 @@
         <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>519</v>
+        <v>575</v>
       </c>
       <c r="O36" t="s">
         <v>505</v>
@@ -3257,7 +3278,10 @@
         <v>401</v>
       </c>
       <c r="P37" t="s">
-        <v>522</v>
+        <v>519</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="38" spans="1:17">
@@ -3683,7 +3707,7 @@
         <v>512</v>
       </c>
       <c r="P52" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="53" spans="1:17">
@@ -3747,108 +3771,70 @@
         <v>23</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C57" s="7"/>
       <c r="O57" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="58" spans="1:17">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="Q58" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="A59" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B59" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C59" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>65</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>48</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>168</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G59" t="s">
         <v>173</v>
       </c>
-      <c r="H58" t="s">
+      <c r="H59" t="s">
         <v>200</v>
       </c>
-      <c r="I58" t="s">
+      <c r="I59" t="s">
         <v>252</v>
       </c>
-      <c r="J58" t="s">
+      <c r="J59" t="s">
         <v>207</v>
       </c>
-      <c r="K58" t="s">
+      <c r="K59" t="s">
         <v>216</v>
       </c>
-      <c r="L58" t="s">
+      <c r="L59" t="s">
         <v>329</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M59" t="s">
         <v>370</v>
       </c>
-      <c r="P58" t="s">
+      <c r="P59" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="59" spans="1:17">
-      <c r="A59" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D59" t="s">
-        <v>67</v>
-      </c>
-      <c r="E59" t="s">
-        <v>49</v>
-      </c>
-      <c r="F59" t="s">
-        <v>143</v>
-      </c>
-      <c r="G59" t="s">
-        <v>148</v>
-      </c>
-      <c r="H59" t="s">
-        <v>201</v>
-      </c>
-      <c r="I59" t="s">
-        <v>253</v>
-      </c>
-      <c r="J59" t="s">
-        <v>204</v>
-      </c>
-      <c r="K59" t="s">
-        <v>218</v>
-      </c>
-      <c r="L59" t="s">
-        <v>312</v>
-      </c>
-      <c r="M59" t="s">
-        <v>379</v>
-      </c>
-      <c r="N59" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="O59" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="P59" t="s">
-        <v>523</v>
-      </c>
       <c r="Q59" t="s">
-        <v>523</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:17">
@@ -3858,8 +3844,17 @@
       <c r="B60" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C60" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E60" t="s">
+        <v>49</v>
+      </c>
       <c r="F60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G60" t="s">
         <v>148</v>
@@ -3868,7 +3863,7 @@
         <v>201</v>
       </c>
       <c r="I60" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J60" t="s">
         <v>204</v>
@@ -3877,13 +3872,22 @@
         <v>218</v>
       </c>
       <c r="L60" t="s">
-        <v>450</v>
+        <v>312</v>
       </c>
       <c r="M60" t="s">
-        <v>384</v>
-      </c>
-      <c r="O60" t="s">
-        <v>495</v>
+        <v>379</v>
+      </c>
+      <c r="N60" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="O60" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="P60" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -3893,11 +3897,17 @@
       <c r="B61" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F61" t="s">
+        <v>144</v>
+      </c>
+      <c r="G61" t="s">
+        <v>148</v>
+      </c>
       <c r="H61" t="s">
         <v>201</v>
       </c>
       <c r="I61" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J61" t="s">
         <v>204</v>
@@ -3905,8 +3915,14 @@
       <c r="K61" t="s">
         <v>218</v>
       </c>
+      <c r="L61" t="s">
+        <v>450</v>
+      </c>
+      <c r="M61" t="s">
+        <v>384</v>
+      </c>
       <c r="O61" t="s">
-        <v>523</v>
+        <v>495</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -3920,7 +3936,7 @@
         <v>201</v>
       </c>
       <c r="I62" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J62" t="s">
         <v>204</v>
@@ -3928,6 +3944,9 @@
       <c r="K62" t="s">
         <v>218</v>
       </c>
+      <c r="O62" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="63" spans="1:17">
       <c r="A63" s="3" t="s">
@@ -3940,7 +3959,7 @@
         <v>201</v>
       </c>
       <c r="I63" t="s">
-        <v>350</v>
+        <v>256</v>
       </c>
       <c r="J63" t="s">
         <v>204</v>
@@ -3960,7 +3979,7 @@
         <v>201</v>
       </c>
       <c r="I64" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J64" t="s">
         <v>204</v>
@@ -3980,7 +3999,7 @@
         <v>201</v>
       </c>
       <c r="I65" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J65" t="s">
         <v>204</v>
@@ -4000,7 +4019,7 @@
         <v>201</v>
       </c>
       <c r="I66" t="s">
-        <v>257</v>
+        <v>354</v>
       </c>
       <c r="J66" t="s">
         <v>204</v>
@@ -4020,7 +4039,7 @@
         <v>201</v>
       </c>
       <c r="I67" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J67" t="s">
         <v>204</v>
@@ -4040,7 +4059,7 @@
         <v>201</v>
       </c>
       <c r="I68" t="s">
-        <v>413</v>
+        <v>258</v>
       </c>
       <c r="J68" t="s">
         <v>204</v>
@@ -4060,7 +4079,7 @@
         <v>201</v>
       </c>
       <c r="I69" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J69" t="s">
         <v>204</v>
@@ -4080,7 +4099,7 @@
         <v>201</v>
       </c>
       <c r="I70" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J70" t="s">
         <v>204</v>
@@ -4100,7 +4119,7 @@
         <v>201</v>
       </c>
       <c r="I71" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="J71" t="s">
         <v>204</v>
@@ -4116,8 +4135,11 @@
       <c r="B72" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H72" t="s">
+        <v>201</v>
+      </c>
       <c r="I72" t="s">
-        <v>483</v>
+        <v>415</v>
       </c>
       <c r="J72" t="s">
         <v>204</v>
@@ -4134,7 +4156,7 @@
         <v>25</v>
       </c>
       <c r="I73" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J73" t="s">
         <v>204</v>
@@ -4150,11 +4172,8 @@
       <c r="B74" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H74" t="s">
-        <v>201</v>
-      </c>
       <c r="I74" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="J74" t="s">
         <v>204</v>
@@ -4174,7 +4193,7 @@
         <v>201</v>
       </c>
       <c r="I75" t="s">
-        <v>349</v>
+        <v>479</v>
       </c>
       <c r="J75" t="s">
         <v>204</v>
@@ -4194,7 +4213,7 @@
         <v>201</v>
       </c>
       <c r="I76" t="s">
-        <v>257</v>
+        <v>349</v>
       </c>
       <c r="J76" t="s">
         <v>204</v>
@@ -4208,25 +4227,13 @@
         <v>24</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D77" t="s">
-        <v>68</v>
-      </c>
-      <c r="E77" t="s">
-        <v>49</v>
-      </c>
-      <c r="F77" t="s">
-        <v>145</v>
-      </c>
-      <c r="G77" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
       <c r="H77" t="s">
         <v>201</v>
+      </c>
+      <c r="I77" t="s">
+        <v>257</v>
       </c>
       <c r="J77" t="s">
         <v>204</v>
@@ -4234,24 +4241,6 @@
       <c r="K77" t="s">
         <v>218</v>
       </c>
-      <c r="L77" t="s">
-        <v>314</v>
-      </c>
-      <c r="M77" t="s">
-        <v>246</v>
-      </c>
-      <c r="N77" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="O77" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="P77" t="s">
-        <v>524</v>
-      </c>
-      <c r="Q77" t="s">
-        <v>549</v>
-      </c>
     </row>
     <row r="78" spans="1:17">
       <c r="A78" s="3" t="s">
@@ -4260,11 +4249,23 @@
       <c r="B78" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C78" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" t="s">
+        <v>68</v>
+      </c>
+      <c r="E78" t="s">
+        <v>49</v>
+      </c>
+      <c r="F78" t="s">
+        <v>145</v>
+      </c>
+      <c r="G78" t="s">
+        <v>148</v>
+      </c>
       <c r="H78" t="s">
         <v>201</v>
-      </c>
-      <c r="I78" t="s">
-        <v>259</v>
       </c>
       <c r="J78" t="s">
         <v>204</v>
@@ -4272,8 +4273,23 @@
       <c r="K78" t="s">
         <v>218</v>
       </c>
-      <c r="O78" t="s">
-        <v>498</v>
+      <c r="L78" t="s">
+        <v>314</v>
+      </c>
+      <c r="M78" t="s">
+        <v>246</v>
+      </c>
+      <c r="N78" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="O78" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="P78" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="79" spans="1:17">
@@ -4283,17 +4299,11 @@
       <c r="B79" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F79" t="s">
-        <v>146</v>
-      </c>
-      <c r="G79" t="s">
-        <v>148</v>
-      </c>
       <c r="H79" t="s">
         <v>201</v>
       </c>
       <c r="I79" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J79" t="s">
         <v>204</v>
@@ -4302,7 +4312,7 @@
         <v>218</v>
       </c>
       <c r="O79" t="s">
-        <v>524</v>
+        <v>498</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4312,11 +4322,17 @@
       <c r="B80" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F80" t="s">
+        <v>146</v>
+      </c>
+      <c r="G80" t="s">
+        <v>148</v>
+      </c>
       <c r="H80" t="s">
         <v>201</v>
       </c>
       <c r="I80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J80" t="s">
         <v>204</v>
@@ -4324,6 +4340,9 @@
       <c r="K80" t="s">
         <v>218</v>
       </c>
+      <c r="O80" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="81" spans="1:11">
       <c r="A81" s="3" t="s">
@@ -4336,7 +4355,7 @@
         <v>201</v>
       </c>
       <c r="I81" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J81" t="s">
         <v>204</v>
@@ -4356,7 +4375,7 @@
         <v>201</v>
       </c>
       <c r="I82" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J82" t="s">
         <v>204</v>
@@ -4376,7 +4395,7 @@
         <v>201</v>
       </c>
       <c r="I83" t="s">
-        <v>480</v>
+        <v>263</v>
       </c>
       <c r="J83" t="s">
         <v>204</v>
@@ -4396,7 +4415,7 @@
         <v>201</v>
       </c>
       <c r="I84" t="s">
-        <v>352</v>
+        <v>480</v>
       </c>
       <c r="J84" t="s">
         <v>204</v>
@@ -4416,7 +4435,7 @@
         <v>201</v>
       </c>
       <c r="I85" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J85" t="s">
         <v>204</v>
@@ -4436,7 +4455,7 @@
         <v>201</v>
       </c>
       <c r="I86" t="s">
-        <v>417</v>
+        <v>355</v>
       </c>
       <c r="J86" t="s">
         <v>204</v>
@@ -4456,7 +4475,7 @@
         <v>201</v>
       </c>
       <c r="I87" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J87" t="s">
         <v>204</v>
@@ -4476,7 +4495,7 @@
         <v>201</v>
       </c>
       <c r="I88" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J88" t="s">
         <v>204</v>
@@ -4496,7 +4515,7 @@
         <v>201</v>
       </c>
       <c r="I89" t="s">
-        <v>478</v>
+        <v>419</v>
       </c>
       <c r="J89" t="s">
         <v>204</v>
@@ -4516,7 +4535,7 @@
         <v>201</v>
       </c>
       <c r="I90" t="s">
-        <v>420</v>
+        <v>478</v>
       </c>
       <c r="J90" t="s">
         <v>204</v>
@@ -4532,8 +4551,11 @@
       <c r="B91" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H91" t="s">
+        <v>201</v>
+      </c>
       <c r="I91" t="s">
-        <v>482</v>
+        <v>420</v>
       </c>
       <c r="J91" t="s">
         <v>204</v>
@@ -4550,7 +4572,7 @@
         <v>26</v>
       </c>
       <c r="I92" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J92" t="s">
         <v>204</v>
@@ -4567,7 +4589,7 @@
         <v>26</v>
       </c>
       <c r="I93" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J93" t="s">
         <v>204</v>
@@ -4583,11 +4605,8 @@
       <c r="B94" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H94" t="s">
-        <v>201</v>
-      </c>
       <c r="I94" t="s">
-        <v>205</v>
+        <v>486</v>
       </c>
       <c r="J94" t="s">
         <v>204</v>
@@ -4607,7 +4626,7 @@
         <v>201</v>
       </c>
       <c r="I95" t="s">
-        <v>279</v>
+        <v>205</v>
       </c>
       <c r="J95" t="s">
         <v>204</v>
@@ -4627,7 +4646,7 @@
         <v>201</v>
       </c>
       <c r="I96" t="s">
-        <v>477</v>
+        <v>279</v>
       </c>
       <c r="J96" t="s">
         <v>204</v>
@@ -4641,28 +4660,13 @@
         <v>24</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C97" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D97" t="s">
-        <v>69</v>
-      </c>
-      <c r="E97" t="s">
-        <v>49</v>
-      </c>
-      <c r="F97" t="s">
-        <v>151</v>
-      </c>
-      <c r="G97" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="H97" t="s">
         <v>201</v>
       </c>
       <c r="I97" t="s">
-        <v>264</v>
+        <v>477</v>
       </c>
       <c r="J97" t="s">
         <v>204</v>
@@ -4670,18 +4674,6 @@
       <c r="K97" t="s">
         <v>218</v>
       </c>
-      <c r="L97" t="s">
-        <v>331</v>
-      </c>
-      <c r="M97" t="s">
-        <v>266</v>
-      </c>
-      <c r="O97" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="P97" t="s">
-        <v>527</v>
-      </c>
     </row>
     <row r="98" spans="1:17">
       <c r="A98" s="3" t="s">
@@ -4690,11 +4682,26 @@
       <c r="B98" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C98" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D98" t="s">
+        <v>69</v>
+      </c>
+      <c r="E98" t="s">
+        <v>49</v>
+      </c>
+      <c r="F98" t="s">
+        <v>151</v>
+      </c>
+      <c r="G98" t="s">
+        <v>148</v>
+      </c>
       <c r="H98" t="s">
         <v>201</v>
       </c>
       <c r="I98" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J98" t="s">
         <v>204</v>
@@ -4702,8 +4709,17 @@
       <c r="K98" t="s">
         <v>218</v>
       </c>
-      <c r="O98" t="s">
-        <v>544</v>
+      <c r="L98" t="s">
+        <v>331</v>
+      </c>
+      <c r="M98" t="s">
+        <v>266</v>
+      </c>
+      <c r="O98" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="P98" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="99" spans="1:17">
@@ -4713,17 +4729,11 @@
       <c r="B99" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F99" t="s">
-        <v>152</v>
-      </c>
-      <c r="G99" t="s">
-        <v>148</v>
-      </c>
       <c r="H99" t="s">
         <v>201</v>
       </c>
       <c r="I99" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J99" t="s">
         <v>204</v>
@@ -4731,16 +4741,19 @@
       <c r="K99" t="s">
         <v>218</v>
       </c>
+      <c r="O99" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="100" spans="1:17">
       <c r="A100" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>501</v>
+        <v>27</v>
       </c>
       <c r="F100" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="G100" t="s">
         <v>148</v>
@@ -4749,7 +4762,7 @@
         <v>201</v>
       </c>
       <c r="I100" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J100" t="s">
         <v>204</v>
@@ -4757,31 +4770,16 @@
       <c r="K100" t="s">
         <v>218</v>
       </c>
-      <c r="N100" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="O100" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="101" spans="1:17">
       <c r="A101" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C101" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D101" t="s">
-        <v>84</v>
-      </c>
-      <c r="E101" t="s">
-        <v>49</v>
+        <v>501</v>
       </c>
       <c r="F101" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="G101" t="s">
         <v>148</v>
@@ -4790,7 +4788,7 @@
         <v>201</v>
       </c>
       <c r="I101" t="s">
-        <v>84</v>
+        <v>267</v>
       </c>
       <c r="J101" t="s">
         <v>204</v>
@@ -4798,14 +4796,14 @@
       <c r="K101" t="s">
         <v>218</v>
       </c>
-      <c r="L101" t="s">
-        <v>318</v>
-      </c>
-      <c r="M101" t="s">
-        <v>374</v>
-      </c>
-      <c r="P101" t="s">
-        <v>526</v>
+      <c r="N101" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="O101" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="102" spans="1:17">
@@ -4815,8 +4813,41 @@
       <c r="B102" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C102" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" t="s">
+        <v>84</v>
+      </c>
+      <c r="E102" t="s">
+        <v>49</v>
+      </c>
+      <c r="F102" t="s">
+        <v>149</v>
+      </c>
+      <c r="G102" t="s">
+        <v>148</v>
+      </c>
+      <c r="H102" t="s">
+        <v>201</v>
+      </c>
+      <c r="I102" t="s">
+        <v>84</v>
+      </c>
+      <c r="J102" t="s">
+        <v>204</v>
+      </c>
+      <c r="K102" t="s">
+        <v>218</v>
+      </c>
       <c r="L102" t="s">
-        <v>464</v>
+        <v>318</v>
+      </c>
+      <c r="M102" t="s">
+        <v>374</v>
+      </c>
+      <c r="P102" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="103" spans="1:17">
@@ -4824,52 +4855,10 @@
         <v>24</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>538</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D103" t="s">
-        <v>72</v>
-      </c>
-      <c r="E103" t="s">
-        <v>49</v>
-      </c>
-      <c r="F103" t="s">
-        <v>150</v>
-      </c>
-      <c r="G103" t="s">
-        <v>148</v>
-      </c>
-      <c r="H103" t="s">
-        <v>201</v>
-      </c>
-      <c r="I103" t="s">
-        <v>268</v>
-      </c>
-      <c r="J103" t="s">
-        <v>204</v>
-      </c>
-      <c r="K103" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
       <c r="L103" t="s">
-        <v>311</v>
-      </c>
-      <c r="M103" t="s">
-        <v>371</v>
-      </c>
-      <c r="N103" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="O103" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="P103" t="s">
-        <v>525</v>
-      </c>
-      <c r="Q103" t="s">
-        <v>551</v>
+        <v>464</v>
       </c>
     </row>
     <row r="104" spans="1:17">
@@ -4877,19 +4866,19 @@
         <v>24</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D104" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E104" t="s">
         <v>49</v>
       </c>
       <c r="F104" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="G104" t="s">
         <v>148</v>
@@ -4898,7 +4887,7 @@
         <v>201</v>
       </c>
       <c r="I104" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J104" t="s">
         <v>204</v>
@@ -4907,13 +4896,22 @@
         <v>218</v>
       </c>
       <c r="L104" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="M104" t="s">
-        <v>372</v>
-      </c>
-      <c r="O104" t="s">
-        <v>494</v>
+        <v>371</v>
+      </c>
+      <c r="N104" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="O104" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="P104" t="s">
+        <v>522</v>
+      </c>
+      <c r="Q104" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="105" spans="1:17">
@@ -4921,10 +4919,19 @@
         <v>24</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D105" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" t="s">
+        <v>49</v>
       </c>
       <c r="F105" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G105" t="s">
         <v>148</v>
@@ -4933,7 +4940,7 @@
         <v>201</v>
       </c>
       <c r="I105" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J105" t="s">
         <v>204</v>
@@ -4942,13 +4949,16 @@
         <v>218</v>
       </c>
       <c r="L105" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M105" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O105" t="s">
-        <v>539</v>
+        <v>494</v>
+      </c>
+      <c r="Q105" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="106" spans="1:17">
@@ -4956,10 +4966,10 @@
         <v>24</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F106" t="s">
-        <v>347</v>
+        <v>187</v>
       </c>
       <c r="G106" t="s">
         <v>148</v>
@@ -4968,13 +4978,25 @@
         <v>201</v>
       </c>
       <c r="I106" t="s">
-        <v>490</v>
+        <v>270</v>
+      </c>
+      <c r="J106" t="s">
+        <v>204</v>
+      </c>
+      <c r="K106" t="s">
+        <v>218</v>
       </c>
       <c r="L106" t="s">
-        <v>460</v>
+        <v>321</v>
       </c>
       <c r="M106" t="s">
-        <v>383</v>
+        <v>373</v>
+      </c>
+      <c r="O106" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q106" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="107" spans="1:17">
@@ -4982,10 +5004,10 @@
         <v>24</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F107" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="G107" t="s">
         <v>148</v>
@@ -4994,16 +5016,13 @@
         <v>201</v>
       </c>
       <c r="I107" t="s">
-        <v>271</v>
-      </c>
-      <c r="J107" t="s">
-        <v>204</v>
-      </c>
-      <c r="K107" t="s">
-        <v>218</v>
+        <v>490</v>
+      </c>
+      <c r="L107" t="s">
+        <v>460</v>
       </c>
       <c r="M107" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
     </row>
     <row r="108" spans="1:17">
@@ -5011,10 +5030,10 @@
         <v>24</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F108" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G108" t="s">
         <v>148</v>
@@ -5023,7 +5042,7 @@
         <v>201</v>
       </c>
       <c r="I108" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J108" t="s">
         <v>204</v>
@@ -5031,16 +5050,19 @@
       <c r="K108" t="s">
         <v>218</v>
       </c>
+      <c r="M108" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="109" spans="1:17">
       <c r="A109" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F109" t="s">
-        <v>358</v>
+        <v>193</v>
       </c>
       <c r="G109" t="s">
         <v>148</v>
@@ -5049,7 +5071,13 @@
         <v>201</v>
       </c>
       <c r="I109" t="s">
-        <v>491</v>
+        <v>272</v>
+      </c>
+      <c r="J109" t="s">
+        <v>204</v>
+      </c>
+      <c r="K109" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="1:17">
@@ -5057,10 +5085,10 @@
         <v>24</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F110" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G110" t="s">
         <v>148</v>
@@ -5069,7 +5097,7 @@
         <v>201</v>
       </c>
       <c r="I110" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="111" spans="1:17">
@@ -5077,13 +5105,19 @@
         <v>24</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
+      </c>
+      <c r="F111" t="s">
+        <v>361</v>
+      </c>
+      <c r="G111" t="s">
+        <v>148</v>
       </c>
       <c r="H111" t="s">
         <v>201</v>
       </c>
       <c r="I111" t="s">
-        <v>73</v>
+        <v>492</v>
       </c>
     </row>
     <row r="112" spans="1:17">
@@ -5091,43 +5125,13 @@
         <v>24</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C112" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D112" t="s">
-        <v>74</v>
-      </c>
-      <c r="E112" t="s">
-        <v>49</v>
-      </c>
-      <c r="F112" t="s">
-        <v>197</v>
-      </c>
-      <c r="G112" t="s">
-        <v>148</v>
+        <v>535</v>
       </c>
       <c r="H112" t="s">
         <v>201</v>
       </c>
       <c r="I112" t="s">
-        <v>273</v>
-      </c>
-      <c r="J112" t="s">
-        <v>204</v>
-      </c>
-      <c r="K112" t="s">
-        <v>218</v>
-      </c>
-      <c r="M112" t="s">
-        <v>382</v>
-      </c>
-      <c r="N112" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="O112" s="10" t="s">
-        <v>448</v>
+        <v>73</v>
       </c>
     </row>
     <row r="113" spans="1:17">
@@ -5137,9 +5141,41 @@
       <c r="B113" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N113" s="10"/>
-      <c r="O113" t="s">
+      <c r="C113" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D113" t="s">
+        <v>74</v>
+      </c>
+      <c r="E113" t="s">
+        <v>49</v>
+      </c>
+      <c r="F113" t="s">
         <v>197</v>
+      </c>
+      <c r="G113" t="s">
+        <v>148</v>
+      </c>
+      <c r="H113" t="s">
+        <v>201</v>
+      </c>
+      <c r="I113" t="s">
+        <v>273</v>
+      </c>
+      <c r="J113" t="s">
+        <v>204</v>
+      </c>
+      <c r="K113" t="s">
+        <v>218</v>
+      </c>
+      <c r="M113" t="s">
+        <v>382</v>
+      </c>
+      <c r="N113" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="O113" s="10" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="114" spans="1:17">
@@ -5147,28 +5183,11 @@
         <v>24</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D114" t="s">
-        <v>92</v>
-      </c>
-      <c r="E114" t="s">
-        <v>49</v>
-      </c>
-      <c r="H114" t="s">
-        <v>201</v>
-      </c>
-      <c r="I114" t="s">
-        <v>274</v>
-      </c>
-      <c r="J114" t="s">
-        <v>204</v>
-      </c>
-      <c r="K114" t="s">
-        <v>218</v>
+        <v>29</v>
+      </c>
+      <c r="N114" s="10"/>
+      <c r="O114" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="115" spans="1:17">
@@ -5176,7 +5195,28 @@
         <v>24</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D115" t="s">
+        <v>92</v>
+      </c>
+      <c r="E115" t="s">
+        <v>49</v>
+      </c>
+      <c r="H115" t="s">
+        <v>201</v>
+      </c>
+      <c r="I115" t="s">
+        <v>274</v>
+      </c>
+      <c r="J115" t="s">
+        <v>204</v>
+      </c>
+      <c r="K115" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -5184,52 +5224,7 @@
         <v>24</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C116" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D116" t="s">
-        <v>71</v>
-      </c>
-      <c r="E116" t="s">
-        <v>49</v>
-      </c>
-      <c r="F116" t="s">
-        <v>154</v>
-      </c>
-      <c r="G116" t="s">
-        <v>148</v>
-      </c>
-      <c r="H116" t="s">
-        <v>201</v>
-      </c>
-      <c r="I116" t="s">
-        <v>275</v>
-      </c>
-      <c r="J116" t="s">
-        <v>204</v>
-      </c>
-      <c r="K116" t="s">
-        <v>218</v>
-      </c>
-      <c r="L116" t="s">
-        <v>315</v>
-      </c>
-      <c r="M116" t="s">
-        <v>385</v>
-      </c>
-      <c r="N116" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="O116" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="P116" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q116" t="s">
-        <v>554</v>
+        <v>31</v>
       </c>
     </row>
     <row r="117" spans="1:17">
@@ -5239,8 +5234,17 @@
       <c r="B117" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C117" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D117" t="s">
+        <v>71</v>
+      </c>
+      <c r="E117" t="s">
+        <v>49</v>
+      </c>
       <c r="F117" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G117" t="s">
         <v>148</v>
@@ -5249,7 +5253,7 @@
         <v>201</v>
       </c>
       <c r="I117" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J117" t="s">
         <v>204</v>
@@ -5258,10 +5262,22 @@
         <v>218</v>
       </c>
       <c r="L117" t="s">
-        <v>449</v>
-      </c>
-      <c r="O117" t="s">
-        <v>502</v>
+        <v>315</v>
+      </c>
+      <c r="M117" t="s">
+        <v>385</v>
+      </c>
+      <c r="N117" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="O117" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="P117" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q117" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="118" spans="1:17">
@@ -5272,7 +5288,7 @@
         <v>32</v>
       </c>
       <c r="F118" t="s">
-        <v>363</v>
+        <v>155</v>
       </c>
       <c r="G118" t="s">
         <v>148</v>
@@ -5280,8 +5296,20 @@
       <c r="H118" t="s">
         <v>201</v>
       </c>
+      <c r="I118" t="s">
+        <v>276</v>
+      </c>
+      <c r="J118" t="s">
+        <v>204</v>
+      </c>
+      <c r="K118" t="s">
+        <v>218</v>
+      </c>
+      <c r="L118" t="s">
+        <v>449</v>
+      </c>
       <c r="O118" t="s">
-        <v>541</v>
+        <v>502</v>
       </c>
     </row>
     <row r="119" spans="1:17">
@@ -5289,19 +5317,10 @@
         <v>24</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D119" t="s">
-        <v>70</v>
-      </c>
-      <c r="E119" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F119" t="s">
-        <v>153</v>
+        <v>363</v>
       </c>
       <c r="G119" t="s">
         <v>148</v>
@@ -5309,29 +5328,8 @@
       <c r="H119" t="s">
         <v>201</v>
       </c>
-      <c r="I119" t="s">
-        <v>277</v>
-      </c>
-      <c r="J119" t="s">
-        <v>204</v>
-      </c>
-      <c r="K119" t="s">
-        <v>218</v>
-      </c>
-      <c r="L119" t="s">
-        <v>334</v>
-      </c>
-      <c r="M119" t="s">
-        <v>381</v>
-      </c>
       <c r="O119" t="s">
-        <v>543</v>
-      </c>
-      <c r="P119" t="s">
-        <v>546</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>550</v>
+        <v>538</v>
       </c>
     </row>
     <row r="120" spans="1:17">
@@ -5341,17 +5339,17 @@
       <c r="B120" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C120" s="6">
-        <v>253</v>
+      <c r="C120" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D120" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E120" t="s">
         <v>49</v>
       </c>
       <c r="F120" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
       <c r="G120" t="s">
         <v>148</v>
@@ -5360,7 +5358,7 @@
         <v>201</v>
       </c>
       <c r="I120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J120" t="s">
         <v>204</v>
@@ -5368,6 +5366,21 @@
       <c r="K120" t="s">
         <v>218</v>
       </c>
+      <c r="L120" t="s">
+        <v>334</v>
+      </c>
+      <c r="M120" t="s">
+        <v>381</v>
+      </c>
+      <c r="O120" t="s">
+        <v>540</v>
+      </c>
+      <c r="P120" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="121" spans="1:17">
       <c r="A121" s="3" t="s">
@@ -5376,8 +5389,17 @@
       <c r="B121" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C121" s="6">
+        <v>253</v>
+      </c>
+      <c r="D121" t="s">
+        <v>90</v>
+      </c>
+      <c r="E121" t="s">
+        <v>49</v>
+      </c>
       <c r="F121" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="G121" t="s">
         <v>148</v>
@@ -5386,7 +5408,13 @@
         <v>201</v>
       </c>
       <c r="I121" t="s">
-        <v>481</v>
+        <v>278</v>
+      </c>
+      <c r="J121" t="s">
+        <v>204</v>
+      </c>
+      <c r="K121" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -5394,19 +5422,10 @@
         <v>24</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D122" t="s">
-        <v>34</v>
-      </c>
-      <c r="E122" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F122" t="s">
-        <v>475</v>
+        <v>196</v>
       </c>
       <c r="G122" t="s">
         <v>148</v>
@@ -5415,22 +5434,7 @@
         <v>201</v>
       </c>
       <c r="I122" t="s">
-        <v>34</v>
-      </c>
-      <c r="J122" t="s">
-        <v>204</v>
-      </c>
-      <c r="K122" t="s">
-        <v>213</v>
-      </c>
-      <c r="L122" t="s">
-        <v>463</v>
-      </c>
-      <c r="M122" t="s">
-        <v>34</v>
-      </c>
-      <c r="O122" s="10" t="s">
-        <v>447</v>
+        <v>481</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -5440,8 +5444,44 @@
       <c r="B123" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C123" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D123" t="s">
+        <v>34</v>
+      </c>
+      <c r="E123" t="s">
+        <v>49</v>
+      </c>
+      <c r="F123" t="s">
+        <v>475</v>
+      </c>
+      <c r="G123" t="s">
+        <v>148</v>
+      </c>
+      <c r="H123" t="s">
+        <v>201</v>
+      </c>
+      <c r="I123" t="s">
+        <v>34</v>
+      </c>
+      <c r="J123" t="s">
+        <v>204</v>
+      </c>
+      <c r="K123" t="s">
+        <v>213</v>
+      </c>
+      <c r="L123" t="s">
+        <v>463</v>
+      </c>
+      <c r="M123" t="s">
+        <v>34</v>
+      </c>
       <c r="O123" s="10" t="s">
-        <v>545</v>
+        <v>447</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="124" spans="1:17">
@@ -5449,43 +5489,10 @@
         <v>24</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C124" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D124" t="s">
-        <v>89</v>
-      </c>
-      <c r="E124" t="s">
-        <v>49</v>
-      </c>
-      <c r="F124" t="s">
-        <v>195</v>
-      </c>
-      <c r="G124" t="s">
-        <v>148</v>
-      </c>
-      <c r="H124" t="s">
-        <v>201</v>
-      </c>
-      <c r="I124" t="s">
-        <v>280</v>
-      </c>
-      <c r="J124" t="s">
-        <v>204</v>
-      </c>
-      <c r="K124" t="s">
-        <v>213</v>
-      </c>
-      <c r="L124" t="s">
-        <v>462</v>
-      </c>
-      <c r="M124" t="s">
-        <v>380</v>
-      </c>
-      <c r="O124" t="s">
-        <v>507</v>
+        <v>34</v>
+      </c>
+      <c r="O124" s="10" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="125" spans="1:17">
@@ -5495,8 +5502,17 @@
       <c r="B125" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C125" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D125" t="s">
+        <v>89</v>
+      </c>
+      <c r="E125" t="s">
+        <v>49</v>
+      </c>
       <c r="F125" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G125" t="s">
         <v>148</v>
@@ -5505,16 +5521,25 @@
         <v>201</v>
       </c>
       <c r="I125" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J125" t="s">
         <v>204</v>
       </c>
       <c r="K125" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="L125" t="s">
+        <v>462</v>
+      </c>
+      <c r="M125" t="s">
+        <v>380</v>
       </c>
       <c r="O125" t="s">
-        <v>542</v>
+        <v>507</v>
+      </c>
+      <c r="Q125" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="126" spans="1:17">
@@ -5525,7 +5550,7 @@
         <v>35</v>
       </c>
       <c r="F126" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G126" t="s">
         <v>148</v>
@@ -5533,40 +5558,34 @@
       <c r="H126" t="s">
         <v>201</v>
       </c>
+      <c r="I126" t="s">
+        <v>281</v>
+      </c>
+      <c r="J126" t="s">
+        <v>204</v>
+      </c>
+      <c r="K126" t="s">
+        <v>218</v>
+      </c>
+      <c r="O126" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="127" spans="1:17">
       <c r="A127" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C127" s="6">
-        <v>311</v>
-      </c>
-      <c r="D127" t="s">
-        <v>75</v>
-      </c>
-      <c r="E127" t="s">
-        <v>51</v>
-      </c>
-      <c r="I127" t="s">
-        <v>282</v>
-      </c>
-      <c r="J127" t="s">
-        <v>204</v>
-      </c>
-      <c r="K127" t="s">
-        <v>218</v>
-      </c>
-      <c r="M127" t="s">
-        <v>376</v>
-      </c>
-      <c r="O127" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="P127" t="s">
-        <v>528</v>
+        <v>35</v>
+      </c>
+      <c r="F127" t="s">
+        <v>192</v>
+      </c>
+      <c r="G127" t="s">
+        <v>148</v>
+      </c>
+      <c r="H127" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="128" spans="1:17">
@@ -5577,16 +5596,31 @@
         <v>36</v>
       </c>
       <c r="C128" s="6">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D128" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="E128" t="s">
         <v>51</v>
       </c>
-      <c r="O128" t="s">
-        <v>568</v>
+      <c r="I128" t="s">
+        <v>282</v>
+      </c>
+      <c r="J128" t="s">
+        <v>204</v>
+      </c>
+      <c r="K128" t="s">
+        <v>218</v>
+      </c>
+      <c r="M128" t="s">
+        <v>376</v>
+      </c>
+      <c r="O128" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="P128" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="129" spans="1:17">
@@ -5594,19 +5628,19 @@
         <v>24</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>305</v>
+        <v>36</v>
+      </c>
+      <c r="C129" s="6">
+        <v>312</v>
       </c>
       <c r="D129" t="s">
-        <v>304</v>
+        <v>135</v>
       </c>
       <c r="E129" t="s">
-        <v>49</v>
-      </c>
-      <c r="M129" t="s">
-        <v>375</v>
+        <v>51</v>
+      </c>
+      <c r="O129" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="130" spans="1:17">
@@ -5614,10 +5648,19 @@
         <v>24</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>377</v>
+        <v>304</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D130" t="s">
+        <v>304</v>
+      </c>
+      <c r="E130" t="s">
+        <v>49</v>
       </c>
       <c r="M130" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="131" spans="1:17">
@@ -5625,34 +5668,10 @@
         <v>24</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D131" t="s">
-        <v>306</v>
-      </c>
-      <c r="E131" t="s">
-        <v>49</v>
-      </c>
-      <c r="F131" t="s">
-        <v>188</v>
-      </c>
-      <c r="G131" t="s">
-        <v>148</v>
-      </c>
-      <c r="H131" t="s">
-        <v>201</v>
-      </c>
-      <c r="I131" t="s">
-        <v>353</v>
-      </c>
-      <c r="J131" t="s">
-        <v>204</v>
-      </c>
-      <c r="K131" t="s">
-        <v>218</v>
+        <v>377</v>
+      </c>
+      <c r="M131" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="132" spans="1:17">
@@ -5660,10 +5679,19 @@
         <v>24</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>345</v>
+        <v>308</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D132" t="s">
+        <v>306</v>
+      </c>
+      <c r="E132" t="s">
+        <v>49</v>
       </c>
       <c r="F132" t="s">
-        <v>344</v>
+        <v>188</v>
       </c>
       <c r="G132" t="s">
         <v>148</v>
@@ -5671,8 +5699,14 @@
       <c r="H132" t="s">
         <v>201</v>
       </c>
-      <c r="L132" t="s">
-        <v>330</v>
+      <c r="I132" t="s">
+        <v>353</v>
+      </c>
+      <c r="J132" t="s">
+        <v>204</v>
+      </c>
+      <c r="K132" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="133" spans="1:17">
@@ -5680,10 +5714,10 @@
         <v>24</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>455</v>
+        <v>345</v>
       </c>
       <c r="F133" t="s">
-        <v>472</v>
+        <v>344</v>
       </c>
       <c r="G133" t="s">
         <v>148</v>
@@ -5691,17 +5725,8 @@
       <c r="H133" t="s">
         <v>201</v>
       </c>
-      <c r="I133" t="s">
-        <v>488</v>
-      </c>
-      <c r="J133" t="s">
-        <v>204</v>
-      </c>
-      <c r="K133" t="s">
-        <v>218</v>
-      </c>
       <c r="L133" t="s">
-        <v>456</v>
+        <v>330</v>
       </c>
     </row>
     <row r="134" spans="1:17">
@@ -5709,13 +5734,19 @@
         <v>24</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>406</v>
+        <v>455</v>
+      </c>
+      <c r="F134" t="s">
+        <v>472</v>
+      </c>
+      <c r="G134" t="s">
+        <v>148</v>
       </c>
       <c r="H134" t="s">
         <v>201</v>
       </c>
       <c r="I134" t="s">
-        <v>283</v>
+        <v>488</v>
       </c>
       <c r="J134" t="s">
         <v>204</v>
@@ -5723,14 +5754,8 @@
       <c r="K134" t="s">
         <v>218</v>
       </c>
-      <c r="M134" t="s">
-        <v>287</v>
-      </c>
-      <c r="N134" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="O134" s="10" t="s">
-        <v>435</v>
+      <c r="L134" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="135" spans="1:17">
@@ -5740,9 +5765,26 @@
       <c r="B135" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="N135" s="10"/>
+      <c r="H135" t="s">
+        <v>201</v>
+      </c>
+      <c r="I135" t="s">
+        <v>283</v>
+      </c>
+      <c r="J135" t="s">
+        <v>204</v>
+      </c>
+      <c r="K135" t="s">
+        <v>218</v>
+      </c>
+      <c r="M135" t="s">
+        <v>287</v>
+      </c>
+      <c r="N135" s="10" t="s">
+        <v>287</v>
+      </c>
       <c r="O135" s="10" t="s">
-        <v>540</v>
+        <v>435</v>
       </c>
     </row>
     <row r="136" spans="1:17">
@@ -5750,10 +5792,11 @@
         <v>24</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="M136" t="s">
-        <v>38</v>
+        <v>406</v>
+      </c>
+      <c r="N136" s="10"/>
+      <c r="O136" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="137" spans="1:17">
@@ -5761,16 +5804,10 @@
         <v>24</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="F137" t="s">
-        <v>470</v>
-      </c>
-      <c r="G137" t="s">
-        <v>148</v>
-      </c>
-      <c r="H137" t="s">
-        <v>201</v>
+        <v>407</v>
+      </c>
+      <c r="M137" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="138" spans="1:17">
@@ -5778,10 +5815,16 @@
         <v>24</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>537</v>
-      </c>
-      <c r="O138" t="s">
-        <v>536</v>
+        <v>469</v>
+      </c>
+      <c r="F138" t="s">
+        <v>470</v>
+      </c>
+      <c r="G138" t="s">
+        <v>148</v>
+      </c>
+      <c r="H138" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:17">
@@ -5789,51 +5832,21 @@
         <v>24</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>552</v>
-      </c>
-      <c r="Q139" t="s">
-        <v>553</v>
+        <v>534</v>
+      </c>
+      <c r="O139" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="140" spans="1:17">
-      <c r="A140" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B140" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C140" s="6">
-        <v>511</v>
-      </c>
-      <c r="D140" t="s">
-        <v>81</v>
-      </c>
-      <c r="E140" t="s">
-        <v>50</v>
-      </c>
-      <c r="F140" t="s">
-        <v>181</v>
-      </c>
-      <c r="G140" t="s">
-        <v>186</v>
-      </c>
-      <c r="H140" t="s">
-        <v>201</v>
-      </c>
-      <c r="J140" t="s">
-        <v>206</v>
-      </c>
-      <c r="K140" t="s">
-        <v>217</v>
-      </c>
-      <c r="L140" t="s">
-        <v>313</v>
-      </c>
-      <c r="P140" t="s">
-        <v>529</v>
+      <c r="A140" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>549</v>
       </c>
       <c r="Q140" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
     </row>
     <row r="141" spans="1:17">
@@ -5843,8 +5856,17 @@
       <c r="B141" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C141" s="6">
+        <v>511</v>
+      </c>
+      <c r="D141" t="s">
+        <v>81</v>
+      </c>
+      <c r="E141" t="s">
+        <v>50</v>
+      </c>
       <c r="F141" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G141" t="s">
         <v>186</v>
@@ -5852,9 +5874,6 @@
       <c r="H141" t="s">
         <v>201</v>
       </c>
-      <c r="I141" t="s">
-        <v>284</v>
-      </c>
       <c r="J141" t="s">
         <v>206</v>
       </c>
@@ -5862,7 +5881,13 @@
         <v>217</v>
       </c>
       <c r="L141" t="s">
-        <v>451</v>
+        <v>313</v>
+      </c>
+      <c r="P141" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q141" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="142" spans="1:17">
@@ -5872,17 +5897,8 @@
       <c r="B142" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C142" s="6">
-        <v>513</v>
-      </c>
-      <c r="D142" t="s">
-        <v>82</v>
-      </c>
-      <c r="E142" t="s">
-        <v>50</v>
-      </c>
       <c r="F142" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G142" t="s">
         <v>186</v>
@@ -5891,7 +5907,7 @@
         <v>201</v>
       </c>
       <c r="I142" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J142" t="s">
         <v>206</v>
@@ -5900,7 +5916,7 @@
         <v>217</v>
       </c>
       <c r="L142" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="143" spans="1:17">
@@ -5910,8 +5926,17 @@
       <c r="B143" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C143" s="6">
+        <v>513</v>
+      </c>
+      <c r="D143" t="s">
+        <v>82</v>
+      </c>
+      <c r="E143" t="s">
+        <v>50</v>
+      </c>
       <c r="F143" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G143" t="s">
         <v>186</v>
@@ -5920,7 +5945,7 @@
         <v>201</v>
       </c>
       <c r="I143" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J143" t="s">
         <v>206</v>
@@ -5929,7 +5954,7 @@
         <v>217</v>
       </c>
       <c r="L143" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="144" spans="1:17">
@@ -5940,7 +5965,7 @@
         <v>38</v>
       </c>
       <c r="F144" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="G144" t="s">
         <v>186</v>
@@ -5949,16 +5974,16 @@
         <v>201</v>
       </c>
       <c r="I144" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J144" t="s">
         <v>206</v>
       </c>
       <c r="K144" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="L144" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="145" spans="1:17">
@@ -5969,7 +5994,7 @@
         <v>38</v>
       </c>
       <c r="F145" t="s">
-        <v>182</v>
+        <v>37</v>
       </c>
       <c r="G145" t="s">
         <v>186</v>
@@ -5978,19 +6003,19 @@
         <v>201</v>
       </c>
       <c r="I145" t="s">
-        <v>38</v>
+        <v>287</v>
       </c>
       <c r="J145" t="s">
         <v>206</v>
       </c>
       <c r="K145" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="L145" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="146" spans="1:17" ht="17" customHeight="1">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17">
       <c r="A146" s="4" t="s">
         <v>37</v>
       </c>
@@ -5998,7 +6023,7 @@
         <v>38</v>
       </c>
       <c r="F146" t="s">
-        <v>357</v>
+        <v>182</v>
       </c>
       <c r="G146" t="s">
         <v>186</v>
@@ -6007,13 +6032,16 @@
         <v>201</v>
       </c>
       <c r="I146" t="s">
-        <v>288</v>
+        <v>38</v>
       </c>
       <c r="J146" t="s">
         <v>206</v>
       </c>
       <c r="K146" t="s">
         <v>217</v>
+      </c>
+      <c r="L146" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="147" spans="1:17" ht="17" customHeight="1">
@@ -6024,7 +6052,7 @@
         <v>38</v>
       </c>
       <c r="F147" t="s">
-        <v>473</v>
+        <v>357</v>
       </c>
       <c r="G147" t="s">
         <v>186</v>
@@ -6033,7 +6061,7 @@
         <v>201</v>
       </c>
       <c r="I147" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J147" t="s">
         <v>206</v>
@@ -6050,7 +6078,7 @@
         <v>38</v>
       </c>
       <c r="F148" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G148" t="s">
         <v>186</v>
@@ -6059,7 +6087,7 @@
         <v>201</v>
       </c>
       <c r="I148" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J148" t="s">
         <v>206</v>
@@ -6075,11 +6103,17 @@
       <c r="B149" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F149" t="s">
+        <v>474</v>
+      </c>
+      <c r="G149" t="s">
+        <v>186</v>
+      </c>
       <c r="H149" t="s">
         <v>201</v>
       </c>
       <c r="I149" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J149" t="s">
         <v>206</v>
@@ -6095,17 +6129,11 @@
       <c r="B150" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F150" t="s">
-        <v>180</v>
-      </c>
-      <c r="G150" t="s">
-        <v>186</v>
-      </c>
       <c r="H150" t="s">
         <v>201</v>
       </c>
       <c r="I150" t="s">
-        <v>487</v>
+        <v>291</v>
       </c>
       <c r="J150" t="s">
         <v>206</v>
@@ -6122,7 +6150,7 @@
         <v>38</v>
       </c>
       <c r="F151" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G151" t="s">
         <v>186</v>
@@ -6131,7 +6159,7 @@
         <v>201</v>
       </c>
       <c r="I151" t="s">
-        <v>212</v>
+        <v>487</v>
       </c>
       <c r="J151" t="s">
         <v>206</v>
@@ -6147,11 +6175,17 @@
       <c r="B152" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F152" t="s">
+        <v>184</v>
+      </c>
+      <c r="G152" t="s">
+        <v>186</v>
+      </c>
       <c r="H152" t="s">
         <v>201</v>
       </c>
       <c r="I152" t="s">
-        <v>489</v>
+        <v>212</v>
       </c>
       <c r="J152" t="s">
         <v>206</v>
@@ -6171,7 +6205,7 @@
         <v>201</v>
       </c>
       <c r="I153" t="s">
-        <v>292</v>
+        <v>489</v>
       </c>
       <c r="J153" t="s">
         <v>206</v>
@@ -6180,39 +6214,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="1:17" ht="17" customHeight="1">
       <c r="A154" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F154" t="s">
-        <v>175</v>
-      </c>
-      <c r="G154" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
       <c r="H154" t="s">
         <v>201</v>
       </c>
       <c r="I154" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J154" t="s">
         <v>206</v>
       </c>
       <c r="K154" t="s">
         <v>217</v>
-      </c>
-      <c r="L154" t="s">
-        <v>458</v>
-      </c>
-      <c r="P154" t="s">
-        <v>530</v>
-      </c>
-      <c r="Q154" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="155" spans="1:17">
@@ -6223,7 +6242,7 @@
         <v>39</v>
       </c>
       <c r="F155" t="s">
-        <v>362</v>
+        <v>175</v>
       </c>
       <c r="G155" t="s">
         <v>186</v>
@@ -6232,13 +6251,22 @@
         <v>201</v>
       </c>
       <c r="I155" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J155" t="s">
         <v>206</v>
       </c>
       <c r="K155" t="s">
         <v>217</v>
+      </c>
+      <c r="L155" t="s">
+        <v>458</v>
+      </c>
+      <c r="P155" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q155" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -6248,11 +6276,17 @@
       <c r="B156" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F156" t="s">
+        <v>362</v>
+      </c>
+      <c r="G156" t="s">
+        <v>186</v>
+      </c>
       <c r="H156" t="s">
         <v>201</v>
       </c>
       <c r="I156" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J156" t="s">
         <v>206</v>
@@ -6266,34 +6300,19 @@
         <v>37</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F157" t="s">
-        <v>178</v>
-      </c>
-      <c r="G157" t="s">
-        <v>186</v>
+        <v>39</v>
       </c>
       <c r="H157" t="s">
         <v>201</v>
       </c>
       <c r="I157" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J157" t="s">
         <v>206</v>
       </c>
       <c r="K157" t="s">
         <v>217</v>
-      </c>
-      <c r="L157" t="s">
-        <v>459</v>
-      </c>
-      <c r="P157" t="s">
-        <v>531</v>
-      </c>
-      <c r="Q157" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="158" spans="1:17">
@@ -6304,19 +6323,31 @@
         <v>40</v>
       </c>
       <c r="F158" t="s">
-        <v>360</v>
+        <v>178</v>
+      </c>
+      <c r="G158" t="s">
+        <v>186</v>
       </c>
       <c r="H158" t="s">
         <v>201</v>
       </c>
       <c r="I158" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J158" t="s">
         <v>206</v>
       </c>
       <c r="K158" t="s">
         <v>217</v>
+      </c>
+      <c r="L158" t="s">
+        <v>459</v>
+      </c>
+      <c r="P158" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="159" spans="1:17">
@@ -6324,34 +6355,22 @@
         <v>37</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>533</v>
+        <v>40</v>
       </c>
       <c r="F159" t="s">
-        <v>174</v>
-      </c>
-      <c r="G159" t="s">
-        <v>186</v>
+        <v>360</v>
       </c>
       <c r="H159" t="s">
         <v>201</v>
       </c>
       <c r="I159" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J159" t="s">
         <v>206</v>
       </c>
       <c r="K159" t="s">
         <v>217</v>
-      </c>
-      <c r="L159" t="s">
-        <v>452</v>
-      </c>
-      <c r="P159" t="s">
-        <v>532</v>
-      </c>
-      <c r="Q159" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="160" spans="1:17">
@@ -6359,10 +6378,10 @@
         <v>37</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F160" t="s">
-        <v>471</v>
+        <v>174</v>
       </c>
       <c r="G160" t="s">
         <v>186</v>
@@ -6371,13 +6390,22 @@
         <v>201</v>
       </c>
       <c r="I160" t="s">
-        <v>41</v>
+        <v>298</v>
       </c>
       <c r="J160" t="s">
         <v>206</v>
       </c>
       <c r="K160" t="s">
         <v>217</v>
+      </c>
+      <c r="L160" t="s">
+        <v>452</v>
+      </c>
+      <c r="P160" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q160" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="161" spans="1:17">
@@ -6385,13 +6413,19 @@
         <v>37</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
+      </c>
+      <c r="F161" t="s">
+        <v>471</v>
+      </c>
+      <c r="G161" t="s">
+        <v>186</v>
       </c>
       <c r="H161" t="s">
         <v>201</v>
       </c>
       <c r="I161" t="s">
-        <v>211</v>
+        <v>41</v>
       </c>
       <c r="J161" t="s">
         <v>206</v>
@@ -6405,13 +6439,13 @@
         <v>37</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="H162" t="s">
         <v>201</v>
       </c>
       <c r="I162" t="s">
-        <v>299</v>
+        <v>211</v>
       </c>
       <c r="J162" t="s">
         <v>206</v>
@@ -6425,10 +6459,19 @@
         <v>37</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>558</v>
-      </c>
-      <c r="Q163" t="s">
-        <v>560</v>
+        <v>530</v>
+      </c>
+      <c r="H163" t="s">
+        <v>201</v>
+      </c>
+      <c r="I163" t="s">
+        <v>299</v>
+      </c>
+      <c r="J163" t="s">
+        <v>206</v>
+      </c>
+      <c r="K163" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="164" spans="1:17">
@@ -6436,10 +6479,10 @@
         <v>37</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="Q164" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="165" spans="1:17">
@@ -6447,56 +6490,41 @@
         <v>37</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>291</v>
+        <v>556</v>
       </c>
       <c r="Q165" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" ht="17" customHeight="1">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17">
       <c r="A166" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="D166" t="s">
-        <v>467</v>
-      </c>
-      <c r="E166" t="s">
-        <v>50</v>
-      </c>
-      <c r="F166" t="s">
-        <v>185</v>
-      </c>
-      <c r="G166" t="s">
-        <v>186</v>
-      </c>
-      <c r="H166" t="s">
-        <v>201</v>
-      </c>
-      <c r="I166" t="s">
-        <v>300</v>
-      </c>
-      <c r="J166" t="s">
-        <v>206</v>
-      </c>
-      <c r="K166" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="167" spans="1:17">
+        <v>291</v>
+      </c>
+      <c r="Q166" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" ht="17" customHeight="1">
       <c r="A167" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="C167" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="D167" t="s">
+        <v>467</v>
+      </c>
+      <c r="E167" t="s">
+        <v>50</v>
+      </c>
       <c r="F167" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G167" t="s">
         <v>186</v>
@@ -6504,28 +6532,31 @@
       <c r="H167" t="s">
         <v>201</v>
       </c>
+      <c r="I167" t="s">
+        <v>300</v>
+      </c>
+      <c r="J167" t="s">
+        <v>206</v>
+      </c>
+      <c r="K167" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="168" spans="1:17">
-      <c r="A168" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E168" t="s">
-        <v>52</v>
+      <c r="A168" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F168" t="s">
+        <v>183</v>
+      </c>
+      <c r="G168" t="s">
+        <v>186</v>
       </c>
       <c r="H168" t="s">
-        <v>200</v>
-      </c>
-      <c r="I168" t="s">
-        <v>301</v>
-      </c>
-      <c r="J168" t="s">
-        <v>209</v>
-      </c>
-      <c r="K168" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="169" spans="1:17">
@@ -6533,13 +6564,16 @@
         <v>43</v>
       </c>
       <c r="B169" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="E169" t="s">
+        <v>52</v>
       </c>
       <c r="H169" t="s">
         <v>200</v>
       </c>
       <c r="I169" t="s">
-        <v>208</v>
+        <v>301</v>
       </c>
       <c r="J169" t="s">
         <v>209</v>
@@ -6555,26 +6589,11 @@
       <c r="B170" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C170" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D170" t="s">
-        <v>45</v>
-      </c>
-      <c r="E170" t="s">
-        <v>52</v>
-      </c>
-      <c r="F170" t="s">
-        <v>161</v>
-      </c>
-      <c r="G170" t="s">
-        <v>173</v>
-      </c>
       <c r="H170" t="s">
         <v>200</v>
       </c>
       <c r="I170" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
       <c r="J170" t="s">
         <v>209</v>
@@ -6588,22 +6607,28 @@
         <v>43</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D171" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="E171" t="s">
         <v>52</v>
       </c>
+      <c r="F171" t="s">
+        <v>161</v>
+      </c>
+      <c r="G171" t="s">
+        <v>173</v>
+      </c>
       <c r="H171" t="s">
         <v>200</v>
       </c>
       <c r="I171" t="s">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="J171" t="s">
         <v>209</v>
@@ -6617,13 +6642,13 @@
         <v>43</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D172" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E172" t="s">
         <v>52</v>
@@ -6632,12 +6657,41 @@
         <v>200</v>
       </c>
       <c r="I172" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J172" t="s">
         <v>209</v>
       </c>
       <c r="K172" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17">
+      <c r="A173" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B173" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D173" t="s">
+        <v>47</v>
+      </c>
+      <c r="E173" t="s">
+        <v>52</v>
+      </c>
+      <c r="H173" t="s">
+        <v>200</v>
+      </c>
+      <c r="I173" t="s">
+        <v>303</v>
+      </c>
+      <c r="J173" t="s">
+        <v>209</v>
+      </c>
+      <c r="K173" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update the benefit index
</commit_message>
<xml_diff>
--- a/benefit_indexing.xlsx
+++ b/benefit_indexing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BryanMak/Documents/RawClaimMCR-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFB90FF-EFA5-FF44-8266-91AF7BECA92B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA91E59A-48ED-304A-8E3F-0B9335CE4956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20060" yWindow="-20900" windowWidth="38400" windowHeight="19900" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
+    <workbookView xWindow="-8160" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{A0161F8B-45E3-674F-BD1A-B040F75BC5F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1370" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="587">
   <si>
     <t>Daily Room &amp; Board</t>
   </si>
@@ -1770,6 +1770,33 @@
   </si>
   <si>
     <t>ACU1</t>
+  </si>
+  <si>
+    <t>Routine Oral Examination</t>
+  </si>
+  <si>
+    <t>Non Claimable Expenses (Bolttech)</t>
+  </si>
+  <si>
+    <t>Routine Physical Exam</t>
+  </si>
+  <si>
+    <t>Extractions</t>
+  </si>
+  <si>
+    <t>Physician's Visit</t>
+  </si>
+  <si>
+    <t>Surgeon's Fee - Complex</t>
+  </si>
+  <si>
+    <t>Operating Theatre - Complex</t>
+  </si>
+  <si>
+    <t>Anaesthetist's Fee - Complex</t>
+  </si>
+  <si>
+    <t>Daily Cash Benefit for 2nd Clm</t>
   </si>
 </sst>
 </file>
@@ -2204,13 +2231,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FDC71E-C596-D04E-840B-E0EAE83F6708}">
-  <dimension ref="A1:Q175"/>
+  <dimension ref="A1:Q176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G113" sqref="G113"/>
+      <selection pane="bottomRight" activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2444,6 +2471,9 @@
       <c r="K5" t="s">
         <v>215</v>
       </c>
+      <c r="N5" s="10" t="s">
+        <v>582</v>
+      </c>
       <c r="O5" t="s">
         <v>508</v>
       </c>
@@ -2656,6 +2686,9 @@
       <c r="E13" t="s">
         <v>48</v>
       </c>
+      <c r="N13" s="10" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="1" t="s">
@@ -2879,6 +2912,9 @@
       <c r="M22" t="s">
         <v>386</v>
       </c>
+      <c r="N22" s="10" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="1" t="s">
@@ -3040,6 +3076,9 @@
       <c r="E28" t="s">
         <v>48</v>
       </c>
+      <c r="N28" s="10" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29" s="1" t="s">
@@ -3709,6 +3748,9 @@
       <c r="M52" t="s">
         <v>392</v>
       </c>
+      <c r="N52" s="10" t="s">
+        <v>586</v>
+      </c>
       <c r="O52" t="s">
         <v>512</v>
       </c>
@@ -3797,103 +3839,59 @@
       </c>
     </row>
     <row r="59" spans="1:17">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C59" s="7"/>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="A60" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B60" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C60" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>65</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E60" t="s">
         <v>48</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F60" t="s">
         <v>168</v>
       </c>
-      <c r="G59" t="s">
+      <c r="G60" t="s">
         <v>173</v>
       </c>
-      <c r="H59" t="s">
+      <c r="H60" t="s">
         <v>200</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I60" t="s">
         <v>252</v>
       </c>
-      <c r="J59" t="s">
+      <c r="J60" t="s">
         <v>207</v>
       </c>
-      <c r="K59" t="s">
+      <c r="K60" t="s">
         <v>216</v>
       </c>
-      <c r="L59" t="s">
+      <c r="L60" t="s">
         <v>329</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M60" t="s">
         <v>370</v>
       </c>
-      <c r="P59" t="s">
+      <c r="P60" t="s">
         <v>168</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="Q60" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17">
-      <c r="A60" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" t="s">
-        <v>67</v>
-      </c>
-      <c r="E60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" t="s">
-        <v>143</v>
-      </c>
-      <c r="G60" t="s">
-        <v>148</v>
-      </c>
-      <c r="H60" t="s">
-        <v>201</v>
-      </c>
-      <c r="I60" t="s">
-        <v>253</v>
-      </c>
-      <c r="J60" t="s">
-        <v>204</v>
-      </c>
-      <c r="K60" t="s">
-        <v>218</v>
-      </c>
-      <c r="L60" t="s">
-        <v>312</v>
-      </c>
-      <c r="M60" t="s">
-        <v>379</v>
-      </c>
-      <c r="N60" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="O60" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="P60" t="s">
-        <v>520</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="61" spans="1:17">
@@ -3903,8 +3901,17 @@
       <c r="B61" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="C61" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" t="s">
+        <v>49</v>
+      </c>
       <c r="F61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G61" t="s">
         <v>148</v>
@@ -3913,7 +3920,7 @@
         <v>201</v>
       </c>
       <c r="I61" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J61" t="s">
         <v>204</v>
@@ -3922,13 +3929,22 @@
         <v>218</v>
       </c>
       <c r="L61" t="s">
-        <v>450</v>
+        <v>312</v>
       </c>
       <c r="M61" t="s">
-        <v>384</v>
-      </c>
-      <c r="O61" t="s">
-        <v>495</v>
+        <v>379</v>
+      </c>
+      <c r="N61" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="O61" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="P61" t="s">
+        <v>520</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="62" spans="1:17">
@@ -3938,11 +3954,17 @@
       <c r="B62" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F62" t="s">
+        <v>144</v>
+      </c>
+      <c r="G62" t="s">
+        <v>148</v>
+      </c>
       <c r="H62" t="s">
         <v>201</v>
       </c>
       <c r="I62" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J62" t="s">
         <v>204</v>
@@ -3950,8 +3972,14 @@
       <c r="K62" t="s">
         <v>218</v>
       </c>
+      <c r="L62" t="s">
+        <v>450</v>
+      </c>
+      <c r="M62" t="s">
+        <v>384</v>
+      </c>
       <c r="O62" t="s">
-        <v>520</v>
+        <v>495</v>
       </c>
     </row>
     <row r="63" spans="1:17">
@@ -3965,7 +3993,7 @@
         <v>201</v>
       </c>
       <c r="I63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J63" t="s">
         <v>204</v>
@@ -3973,6 +4001,9 @@
       <c r="K63" t="s">
         <v>218</v>
       </c>
+      <c r="O63" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="64" spans="1:17">
       <c r="A64" s="3" t="s">
@@ -3985,7 +4016,7 @@
         <v>201</v>
       </c>
       <c r="I64" t="s">
-        <v>350</v>
+        <v>256</v>
       </c>
       <c r="J64" t="s">
         <v>204</v>
@@ -4005,7 +4036,7 @@
         <v>201</v>
       </c>
       <c r="I65" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J65" t="s">
         <v>204</v>
@@ -4025,7 +4056,7 @@
         <v>201</v>
       </c>
       <c r="I66" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="J66" t="s">
         <v>204</v>
@@ -4045,7 +4076,7 @@
         <v>201</v>
       </c>
       <c r="I67" t="s">
-        <v>257</v>
+        <v>354</v>
       </c>
       <c r="J67" t="s">
         <v>204</v>
@@ -4065,7 +4096,7 @@
         <v>201</v>
       </c>
       <c r="I68" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J68" t="s">
         <v>204</v>
@@ -4085,7 +4116,7 @@
         <v>201</v>
       </c>
       <c r="I69" t="s">
-        <v>413</v>
+        <v>258</v>
       </c>
       <c r="J69" t="s">
         <v>204</v>
@@ -4105,7 +4136,7 @@
         <v>201</v>
       </c>
       <c r="I70" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J70" t="s">
         <v>204</v>
@@ -4125,7 +4156,7 @@
         <v>201</v>
       </c>
       <c r="I71" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="J71" t="s">
         <v>204</v>
@@ -4145,7 +4176,7 @@
         <v>201</v>
       </c>
       <c r="I72" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="J72" t="s">
         <v>204</v>
@@ -4161,8 +4192,11 @@
       <c r="B73" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="H73" t="s">
+        <v>201</v>
+      </c>
       <c r="I73" t="s">
-        <v>483</v>
+        <v>415</v>
       </c>
       <c r="J73" t="s">
         <v>204</v>
@@ -4179,7 +4213,7 @@
         <v>25</v>
       </c>
       <c r="I74" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="J74" t="s">
         <v>204</v>
@@ -4195,11 +4229,8 @@
       <c r="B75" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H75" t="s">
-        <v>201</v>
-      </c>
       <c r="I75" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="J75" t="s">
         <v>204</v>
@@ -4219,7 +4250,7 @@
         <v>201</v>
       </c>
       <c r="I76" t="s">
-        <v>349</v>
+        <v>479</v>
       </c>
       <c r="J76" t="s">
         <v>204</v>
@@ -4239,7 +4270,7 @@
         <v>201</v>
       </c>
       <c r="I77" t="s">
-        <v>257</v>
+        <v>349</v>
       </c>
       <c r="J77" t="s">
         <v>204</v>
@@ -4253,25 +4284,13 @@
         <v>24</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D78" t="s">
-        <v>68</v>
-      </c>
-      <c r="E78" t="s">
-        <v>49</v>
-      </c>
-      <c r="F78" t="s">
-        <v>145</v>
-      </c>
-      <c r="G78" t="s">
-        <v>148</v>
+        <v>25</v>
       </c>
       <c r="H78" t="s">
         <v>201</v>
+      </c>
+      <c r="I78" t="s">
+        <v>257</v>
       </c>
       <c r="J78" t="s">
         <v>204</v>
@@ -4279,24 +4298,6 @@
       <c r="K78" t="s">
         <v>218</v>
       </c>
-      <c r="L78" t="s">
-        <v>314</v>
-      </c>
-      <c r="M78" t="s">
-        <v>246</v>
-      </c>
-      <c r="N78" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="O78" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="P78" t="s">
-        <v>521</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>546</v>
-      </c>
     </row>
     <row r="79" spans="1:17">
       <c r="A79" s="3" t="s">
@@ -4305,11 +4306,23 @@
       <c r="B79" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="C79" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D79" t="s">
+        <v>68</v>
+      </c>
+      <c r="E79" t="s">
+        <v>49</v>
+      </c>
+      <c r="F79" t="s">
+        <v>145</v>
+      </c>
+      <c r="G79" t="s">
+        <v>148</v>
+      </c>
       <c r="H79" t="s">
         <v>201</v>
-      </c>
-      <c r="I79" t="s">
-        <v>259</v>
       </c>
       <c r="J79" t="s">
         <v>204</v>
@@ -4317,8 +4330,23 @@
       <c r="K79" t="s">
         <v>218</v>
       </c>
-      <c r="O79" t="s">
-        <v>498</v>
+      <c r="L79" t="s">
+        <v>314</v>
+      </c>
+      <c r="M79" t="s">
+        <v>246</v>
+      </c>
+      <c r="N79" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="O79" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="P79" t="s">
+        <v>521</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="80" spans="1:17">
@@ -4328,17 +4356,11 @@
       <c r="B80" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F80" t="s">
-        <v>146</v>
-      </c>
-      <c r="G80" t="s">
-        <v>148</v>
-      </c>
       <c r="H80" t="s">
         <v>201</v>
       </c>
       <c r="I80" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J80" t="s">
         <v>204</v>
@@ -4347,21 +4369,27 @@
         <v>218</v>
       </c>
       <c r="O80" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F81" t="s">
+        <v>146</v>
+      </c>
+      <c r="G81" t="s">
+        <v>148</v>
+      </c>
       <c r="H81" t="s">
         <v>201</v>
       </c>
       <c r="I81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J81" t="s">
         <v>204</v>
@@ -4369,8 +4397,11 @@
       <c r="K81" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="O81" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" s="3" t="s">
         <v>24</v>
       </c>
@@ -4381,7 +4412,7 @@
         <v>201</v>
       </c>
       <c r="I82" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J82" t="s">
         <v>204</v>
@@ -4390,7 +4421,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:15">
       <c r="A83" s="3" t="s">
         <v>24</v>
       </c>
@@ -4401,7 +4432,7 @@
         <v>201</v>
       </c>
       <c r="I83" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J83" t="s">
         <v>204</v>
@@ -4410,7 +4441,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:15">
       <c r="A84" s="3" t="s">
         <v>24</v>
       </c>
@@ -4421,7 +4452,7 @@
         <v>201</v>
       </c>
       <c r="I84" t="s">
-        <v>480</v>
+        <v>263</v>
       </c>
       <c r="J84" t="s">
         <v>204</v>
@@ -4430,7 +4461,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:15">
       <c r="A85" s="3" t="s">
         <v>24</v>
       </c>
@@ -4441,7 +4472,7 @@
         <v>201</v>
       </c>
       <c r="I85" t="s">
-        <v>352</v>
+        <v>480</v>
       </c>
       <c r="J85" t="s">
         <v>204</v>
@@ -4450,7 +4481,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:15">
       <c r="A86" s="3" t="s">
         <v>24</v>
       </c>
@@ -4461,7 +4492,7 @@
         <v>201</v>
       </c>
       <c r="I86" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="J86" t="s">
         <v>204</v>
@@ -4470,7 +4501,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:15">
       <c r="A87" s="3" t="s">
         <v>24</v>
       </c>
@@ -4481,7 +4512,7 @@
         <v>201</v>
       </c>
       <c r="I87" t="s">
-        <v>417</v>
+        <v>355</v>
       </c>
       <c r="J87" t="s">
         <v>204</v>
@@ -4490,7 +4521,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:15">
       <c r="A88" s="3" t="s">
         <v>24</v>
       </c>
@@ -4501,7 +4532,7 @@
         <v>201</v>
       </c>
       <c r="I88" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="J88" t="s">
         <v>204</v>
@@ -4510,7 +4541,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:15">
       <c r="A89" s="3" t="s">
         <v>24</v>
       </c>
@@ -4521,7 +4552,7 @@
         <v>201</v>
       </c>
       <c r="I89" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J89" t="s">
         <v>204</v>
@@ -4530,7 +4561,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:15">
       <c r="A90" s="3" t="s">
         <v>24</v>
       </c>
@@ -4541,7 +4572,7 @@
         <v>201</v>
       </c>
       <c r="I90" t="s">
-        <v>478</v>
+        <v>419</v>
       </c>
       <c r="J90" t="s">
         <v>204</v>
@@ -4550,7 +4581,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:15">
       <c r="A91" s="3" t="s">
         <v>24</v>
       </c>
@@ -4561,7 +4592,7 @@
         <v>201</v>
       </c>
       <c r="I91" t="s">
-        <v>420</v>
+        <v>478</v>
       </c>
       <c r="J91" t="s">
         <v>204</v>
@@ -4570,15 +4601,18 @@
         <v>218</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:15">
       <c r="A92" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H92" t="s">
+        <v>201</v>
+      </c>
       <c r="I92" t="s">
-        <v>482</v>
+        <v>420</v>
       </c>
       <c r="J92" t="s">
         <v>204</v>
@@ -4587,7 +4621,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:15">
       <c r="A93" s="3" t="s">
         <v>24</v>
       </c>
@@ -4595,7 +4629,7 @@
         <v>26</v>
       </c>
       <c r="I93" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="J93" t="s">
         <v>204</v>
@@ -4604,7 +4638,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:15">
       <c r="A94" s="3" t="s">
         <v>24</v>
       </c>
@@ -4612,7 +4646,7 @@
         <v>26</v>
       </c>
       <c r="I94" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J94" t="s">
         <v>204</v>
@@ -4621,18 +4655,15 @@
         <v>218</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:15">
       <c r="A95" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H95" t="s">
-        <v>201</v>
-      </c>
       <c r="I95" t="s">
-        <v>205</v>
+        <v>486</v>
       </c>
       <c r="J95" t="s">
         <v>204</v>
@@ -4641,7 +4672,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:15">
       <c r="A96" s="3" t="s">
         <v>24</v>
       </c>
@@ -4652,7 +4683,7 @@
         <v>201</v>
       </c>
       <c r="I96" t="s">
-        <v>279</v>
+        <v>205</v>
       </c>
       <c r="J96" t="s">
         <v>204</v>
@@ -4672,7 +4703,7 @@
         <v>201</v>
       </c>
       <c r="I97" t="s">
-        <v>477</v>
+        <v>279</v>
       </c>
       <c r="J97" t="s">
         <v>204</v>
@@ -4686,28 +4717,13 @@
         <v>24</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D98" t="s">
-        <v>69</v>
-      </c>
-      <c r="E98" t="s">
-        <v>49</v>
-      </c>
-      <c r="F98" t="s">
-        <v>151</v>
-      </c>
-      <c r="G98" t="s">
-        <v>148</v>
+        <v>26</v>
       </c>
       <c r="H98" t="s">
         <v>201</v>
       </c>
       <c r="I98" t="s">
-        <v>264</v>
+        <v>477</v>
       </c>
       <c r="J98" t="s">
         <v>204</v>
@@ -4715,18 +4731,6 @@
       <c r="K98" t="s">
         <v>218</v>
       </c>
-      <c r="L98" t="s">
-        <v>331</v>
-      </c>
-      <c r="M98" t="s">
-        <v>266</v>
-      </c>
-      <c r="O98" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="P98" t="s">
-        <v>524</v>
-      </c>
     </row>
     <row r="99" spans="1:17">
       <c r="A99" s="3" t="s">
@@ -4735,11 +4739,26 @@
       <c r="B99" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C99" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D99" t="s">
+        <v>69</v>
+      </c>
+      <c r="E99" t="s">
+        <v>49</v>
+      </c>
+      <c r="F99" t="s">
+        <v>151</v>
+      </c>
+      <c r="G99" t="s">
+        <v>148</v>
+      </c>
       <c r="H99" t="s">
         <v>201</v>
       </c>
       <c r="I99" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J99" t="s">
         <v>204</v>
@@ -4747,8 +4766,17 @@
       <c r="K99" t="s">
         <v>218</v>
       </c>
-      <c r="O99" t="s">
-        <v>541</v>
+      <c r="L99" t="s">
+        <v>331</v>
+      </c>
+      <c r="M99" t="s">
+        <v>266</v>
+      </c>
+      <c r="O99" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="P99" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="100" spans="1:17">
@@ -4758,17 +4786,11 @@
       <c r="B100" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F100" t="s">
-        <v>152</v>
-      </c>
-      <c r="G100" t="s">
-        <v>148</v>
-      </c>
       <c r="H100" t="s">
         <v>201</v>
       </c>
       <c r="I100" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J100" t="s">
         <v>204</v>
@@ -4776,16 +4798,19 @@
       <c r="K100" t="s">
         <v>218</v>
       </c>
+      <c r="O100" t="s">
+        <v>541</v>
+      </c>
     </row>
     <row r="101" spans="1:17">
       <c r="A101" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>501</v>
+        <v>27</v>
       </c>
       <c r="F101" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="G101" t="s">
         <v>148</v>
@@ -4794,7 +4819,7 @@
         <v>201</v>
       </c>
       <c r="I101" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J101" t="s">
         <v>204</v>
@@ -4802,34 +4827,16 @@
       <c r="K101" t="s">
         <v>218</v>
       </c>
-      <c r="N101" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="O101" t="s">
-        <v>500</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>569</v>
-      </c>
     </row>
     <row r="102" spans="1:17">
       <c r="A102" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="D102" t="s">
-        <v>84</v>
-      </c>
-      <c r="E102" t="s">
-        <v>49</v>
+        <v>501</v>
       </c>
       <c r="F102" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
       <c r="G102" t="s">
         <v>148</v>
@@ -4838,7 +4845,7 @@
         <v>201</v>
       </c>
       <c r="I102" t="s">
-        <v>84</v>
+        <v>267</v>
       </c>
       <c r="J102" t="s">
         <v>204</v>
@@ -4846,14 +4853,14 @@
       <c r="K102" t="s">
         <v>218</v>
       </c>
-      <c r="L102" t="s">
-        <v>318</v>
-      </c>
-      <c r="M102" t="s">
-        <v>374</v>
-      </c>
-      <c r="P102" t="s">
-        <v>523</v>
+      <c r="N102" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="O102" t="s">
+        <v>500</v>
+      </c>
+      <c r="Q102" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="103" spans="1:17">
@@ -4863,8 +4870,41 @@
       <c r="B103" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="C103" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" t="s">
+        <v>84</v>
+      </c>
+      <c r="E103" t="s">
+        <v>49</v>
+      </c>
+      <c r="F103" t="s">
+        <v>149</v>
+      </c>
+      <c r="G103" t="s">
+        <v>148</v>
+      </c>
+      <c r="H103" t="s">
+        <v>201</v>
+      </c>
+      <c r="I103" t="s">
+        <v>84</v>
+      </c>
+      <c r="J103" t="s">
+        <v>204</v>
+      </c>
+      <c r="K103" t="s">
+        <v>218</v>
+      </c>
       <c r="L103" t="s">
-        <v>464</v>
+        <v>318</v>
+      </c>
+      <c r="M103" t="s">
+        <v>374</v>
+      </c>
+      <c r="P103" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="104" spans="1:17">
@@ -4872,52 +4912,10 @@
         <v>24</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="C104" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D104" t="s">
-        <v>72</v>
-      </c>
-      <c r="E104" t="s">
-        <v>49</v>
-      </c>
-      <c r="F104" t="s">
-        <v>150</v>
-      </c>
-      <c r="G104" t="s">
-        <v>148</v>
-      </c>
-      <c r="H104" t="s">
-        <v>201</v>
-      </c>
-      <c r="I104" t="s">
-        <v>268</v>
-      </c>
-      <c r="J104" t="s">
-        <v>204</v>
-      </c>
-      <c r="K104" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
       <c r="L104" t="s">
-        <v>311</v>
-      </c>
-      <c r="M104" t="s">
-        <v>371</v>
-      </c>
-      <c r="N104" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="O104" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="P104" t="s">
-        <v>522</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>548</v>
+        <v>464</v>
       </c>
     </row>
     <row r="105" spans="1:17">
@@ -4928,16 +4926,16 @@
         <v>535</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D105" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E105" t="s">
         <v>49</v>
       </c>
       <c r="F105" t="s">
-        <v>194</v>
+        <v>150</v>
       </c>
       <c r="G105" t="s">
         <v>148</v>
@@ -4946,7 +4944,7 @@
         <v>201</v>
       </c>
       <c r="I105" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J105" t="s">
         <v>204</v>
@@ -4955,16 +4953,22 @@
         <v>218</v>
       </c>
       <c r="L105" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="M105" t="s">
-        <v>372</v>
-      </c>
-      <c r="O105" t="s">
-        <v>494</v>
+        <v>371</v>
+      </c>
+      <c r="N105" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="O105" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="P105" t="s">
+        <v>522</v>
       </c>
       <c r="Q105" t="s">
-        <v>566</v>
+        <v>548</v>
       </c>
     </row>
     <row r="106" spans="1:17">
@@ -4974,8 +4978,17 @@
       <c r="B106" s="3" t="s">
         <v>535</v>
       </c>
+      <c r="C106" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D106" t="s">
+        <v>73</v>
+      </c>
+      <c r="E106" t="s">
+        <v>49</v>
+      </c>
       <c r="F106" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="G106" t="s">
         <v>148</v>
@@ -4984,7 +4997,7 @@
         <v>201</v>
       </c>
       <c r="I106" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J106" t="s">
         <v>204</v>
@@ -4993,16 +5006,16 @@
         <v>218</v>
       </c>
       <c r="L106" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M106" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O106" t="s">
-        <v>536</v>
+        <v>494</v>
       </c>
       <c r="Q106" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
     </row>
     <row r="107" spans="1:17">
@@ -5013,7 +5026,7 @@
         <v>535</v>
       </c>
       <c r="F107" t="s">
-        <v>347</v>
+        <v>187</v>
       </c>
       <c r="G107" t="s">
         <v>148</v>
@@ -5022,13 +5035,25 @@
         <v>201</v>
       </c>
       <c r="I107" t="s">
-        <v>490</v>
+        <v>270</v>
+      </c>
+      <c r="J107" t="s">
+        <v>204</v>
+      </c>
+      <c r="K107" t="s">
+        <v>218</v>
       </c>
       <c r="L107" t="s">
-        <v>460</v>
+        <v>321</v>
       </c>
       <c r="M107" t="s">
-        <v>383</v>
+        <v>373</v>
+      </c>
+      <c r="O107" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q107" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="108" spans="1:17">
@@ -5039,7 +5064,7 @@
         <v>535</v>
       </c>
       <c r="F108" t="s">
-        <v>190</v>
+        <v>347</v>
       </c>
       <c r="G108" t="s">
         <v>148</v>
@@ -5048,16 +5073,13 @@
         <v>201</v>
       </c>
       <c r="I108" t="s">
-        <v>271</v>
-      </c>
-      <c r="J108" t="s">
-        <v>204</v>
-      </c>
-      <c r="K108" t="s">
-        <v>218</v>
+        <v>490</v>
+      </c>
+      <c r="L108" t="s">
+        <v>460</v>
       </c>
       <c r="M108" t="s">
-        <v>410</v>
+        <v>383</v>
       </c>
     </row>
     <row r="109" spans="1:17">
@@ -5068,7 +5090,7 @@
         <v>535</v>
       </c>
       <c r="F109" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G109" t="s">
         <v>148</v>
@@ -5077,7 +5099,7 @@
         <v>201</v>
       </c>
       <c r="I109" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J109" t="s">
         <v>204</v>
@@ -5085,6 +5107,9 @@
       <c r="K109" t="s">
         <v>218</v>
       </c>
+      <c r="M109" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="110" spans="1:17">
       <c r="A110" s="3" t="s">
@@ -5094,7 +5119,7 @@
         <v>535</v>
       </c>
       <c r="F110" t="s">
-        <v>358</v>
+        <v>193</v>
       </c>
       <c r="G110" t="s">
         <v>148</v>
@@ -5103,7 +5128,13 @@
         <v>201</v>
       </c>
       <c r="I110" t="s">
-        <v>491</v>
+        <v>272</v>
+      </c>
+      <c r="J110" t="s">
+        <v>204</v>
+      </c>
+      <c r="K110" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:17">
@@ -5114,7 +5145,7 @@
         <v>535</v>
       </c>
       <c r="F111" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G111" t="s">
         <v>148</v>
@@ -5123,7 +5154,7 @@
         <v>201</v>
       </c>
       <c r="I111" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="112" spans="1:17">
@@ -5134,7 +5165,7 @@
         <v>535</v>
       </c>
       <c r="F112" t="s">
-        <v>576</v>
+        <v>361</v>
       </c>
       <c r="G112" t="s">
         <v>148</v>
@@ -5143,7 +5174,7 @@
         <v>201</v>
       </c>
       <c r="I112" t="s">
-        <v>73</v>
+        <v>492</v>
       </c>
     </row>
     <row r="113" spans="1:17">
@@ -5154,11 +5185,17 @@
         <v>535</v>
       </c>
       <c r="F113" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G113" t="s">
         <v>148</v>
       </c>
+      <c r="H113" t="s">
+        <v>201</v>
+      </c>
+      <c r="I113" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="114" spans="1:17">
       <c r="A114" s="3" t="s">
@@ -5167,49 +5204,19 @@
       <c r="B114" s="3" t="s">
         <v>535</v>
       </c>
+      <c r="F114" t="s">
+        <v>577</v>
+      </c>
+      <c r="G114" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="115" spans="1:17">
       <c r="A115" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D115" t="s">
-        <v>74</v>
-      </c>
-      <c r="E115" t="s">
-        <v>49</v>
-      </c>
-      <c r="F115" t="s">
-        <v>197</v>
-      </c>
-      <c r="G115" t="s">
-        <v>148</v>
-      </c>
-      <c r="H115" t="s">
-        <v>201</v>
-      </c>
-      <c r="I115" t="s">
-        <v>273</v>
-      </c>
-      <c r="J115" t="s">
-        <v>204</v>
-      </c>
-      <c r="K115" t="s">
-        <v>218</v>
-      </c>
-      <c r="M115" t="s">
-        <v>382</v>
-      </c>
-      <c r="N115" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="O115" s="10" t="s">
-        <v>448</v>
+        <v>535</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -5219,9 +5226,41 @@
       <c r="B116" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N116" s="10"/>
-      <c r="O116" t="s">
+      <c r="C116" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D116" t="s">
+        <v>74</v>
+      </c>
+      <c r="E116" t="s">
+        <v>49</v>
+      </c>
+      <c r="F116" t="s">
         <v>197</v>
+      </c>
+      <c r="G116" t="s">
+        <v>148</v>
+      </c>
+      <c r="H116" t="s">
+        <v>201</v>
+      </c>
+      <c r="I116" t="s">
+        <v>273</v>
+      </c>
+      <c r="J116" t="s">
+        <v>204</v>
+      </c>
+      <c r="K116" t="s">
+        <v>218</v>
+      </c>
+      <c r="M116" t="s">
+        <v>382</v>
+      </c>
+      <c r="N116" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="O116" s="10" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="117" spans="1:17">
@@ -5229,28 +5268,11 @@
         <v>24</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C117" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D117" t="s">
-        <v>92</v>
-      </c>
-      <c r="E117" t="s">
-        <v>49</v>
-      </c>
-      <c r="H117" t="s">
-        <v>201</v>
-      </c>
-      <c r="I117" t="s">
-        <v>274</v>
-      </c>
-      <c r="J117" t="s">
-        <v>204</v>
-      </c>
-      <c r="K117" t="s">
-        <v>218</v>
+        <v>29</v>
+      </c>
+      <c r="N117" s="10"/>
+      <c r="O117" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="118" spans="1:17">
@@ -5258,7 +5280,28 @@
         <v>24</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D118" t="s">
+        <v>92</v>
+      </c>
+      <c r="E118" t="s">
+        <v>49</v>
+      </c>
+      <c r="H118" t="s">
+        <v>201</v>
+      </c>
+      <c r="I118" t="s">
+        <v>274</v>
+      </c>
+      <c r="J118" t="s">
+        <v>204</v>
+      </c>
+      <c r="K118" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="1:17">
@@ -5266,52 +5309,7 @@
         <v>24</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D119" t="s">
-        <v>71</v>
-      </c>
-      <c r="E119" t="s">
-        <v>49</v>
-      </c>
-      <c r="F119" t="s">
-        <v>154</v>
-      </c>
-      <c r="G119" t="s">
-        <v>148</v>
-      </c>
-      <c r="H119" t="s">
-        <v>201</v>
-      </c>
-      <c r="I119" t="s">
-        <v>275</v>
-      </c>
-      <c r="J119" t="s">
-        <v>204</v>
-      </c>
-      <c r="K119" t="s">
-        <v>218</v>
-      </c>
-      <c r="L119" t="s">
-        <v>315</v>
-      </c>
-      <c r="M119" t="s">
-        <v>385</v>
-      </c>
-      <c r="N119" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="O119" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="P119" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q119" t="s">
-        <v>551</v>
+        <v>31</v>
       </c>
     </row>
     <row r="120" spans="1:17">
@@ -5321,8 +5319,17 @@
       <c r="B120" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="C120" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D120" t="s">
+        <v>71</v>
+      </c>
+      <c r="E120" t="s">
+        <v>49</v>
+      </c>
       <c r="F120" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G120" t="s">
         <v>148</v>
@@ -5331,7 +5338,7 @@
         <v>201</v>
       </c>
       <c r="I120" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J120" t="s">
         <v>204</v>
@@ -5340,10 +5347,22 @@
         <v>218</v>
       </c>
       <c r="L120" t="s">
-        <v>449</v>
-      </c>
-      <c r="O120" t="s">
-        <v>502</v>
+        <v>315</v>
+      </c>
+      <c r="M120" t="s">
+        <v>385</v>
+      </c>
+      <c r="N120" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="O120" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="P120" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q120" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="121" spans="1:17">
@@ -5354,7 +5373,7 @@
         <v>32</v>
       </c>
       <c r="F121" t="s">
-        <v>363</v>
+        <v>155</v>
       </c>
       <c r="G121" t="s">
         <v>148</v>
@@ -5362,8 +5381,20 @@
       <c r="H121" t="s">
         <v>201</v>
       </c>
+      <c r="I121" t="s">
+        <v>276</v>
+      </c>
+      <c r="J121" t="s">
+        <v>204</v>
+      </c>
+      <c r="K121" t="s">
+        <v>218</v>
+      </c>
+      <c r="L121" t="s">
+        <v>449</v>
+      </c>
       <c r="O121" t="s">
-        <v>538</v>
+        <v>502</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -5371,19 +5402,10 @@
         <v>24</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C122" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D122" t="s">
-        <v>70</v>
-      </c>
-      <c r="E122" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F122" t="s">
-        <v>153</v>
+        <v>363</v>
       </c>
       <c r="G122" t="s">
         <v>148</v>
@@ -5391,29 +5413,8 @@
       <c r="H122" t="s">
         <v>201</v>
       </c>
-      <c r="I122" t="s">
-        <v>277</v>
-      </c>
-      <c r="J122" t="s">
-        <v>204</v>
-      </c>
-      <c r="K122" t="s">
-        <v>218</v>
-      </c>
-      <c r="L122" t="s">
-        <v>334</v>
-      </c>
-      <c r="M122" t="s">
-        <v>381</v>
-      </c>
       <c r="O122" t="s">
-        <v>540</v>
-      </c>
-      <c r="P122" t="s">
-        <v>543</v>
-      </c>
-      <c r="Q122" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -5423,17 +5424,17 @@
       <c r="B123" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C123" s="6">
-        <v>253</v>
+      <c r="C123" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D123" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E123" t="s">
         <v>49</v>
       </c>
       <c r="F123" t="s">
-        <v>220</v>
+        <v>153</v>
       </c>
       <c r="G123" t="s">
         <v>148</v>
@@ -5442,7 +5443,7 @@
         <v>201</v>
       </c>
       <c r="I123" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J123" t="s">
         <v>204</v>
@@ -5450,6 +5451,21 @@
       <c r="K123" t="s">
         <v>218</v>
       </c>
+      <c r="L123" t="s">
+        <v>334</v>
+      </c>
+      <c r="M123" t="s">
+        <v>381</v>
+      </c>
+      <c r="O123" t="s">
+        <v>540</v>
+      </c>
+      <c r="P123" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q123" t="s">
+        <v>547</v>
+      </c>
     </row>
     <row r="124" spans="1:17">
       <c r="A124" s="3" t="s">
@@ -5458,8 +5474,17 @@
       <c r="B124" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="C124" s="6">
+        <v>253</v>
+      </c>
+      <c r="D124" t="s">
+        <v>90</v>
+      </c>
+      <c r="E124" t="s">
+        <v>49</v>
+      </c>
       <c r="F124" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="G124" t="s">
         <v>148</v>
@@ -5468,7 +5493,13 @@
         <v>201</v>
       </c>
       <c r="I124" t="s">
-        <v>481</v>
+        <v>278</v>
+      </c>
+      <c r="J124" t="s">
+        <v>204</v>
+      </c>
+      <c r="K124" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="125" spans="1:17">
@@ -5476,19 +5507,10 @@
         <v>24</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C125" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="D125" t="s">
-        <v>34</v>
-      </c>
-      <c r="E125" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F125" t="s">
-        <v>475</v>
+        <v>196</v>
       </c>
       <c r="G125" t="s">
         <v>148</v>
@@ -5497,25 +5519,7 @@
         <v>201</v>
       </c>
       <c r="I125" t="s">
-        <v>34</v>
-      </c>
-      <c r="J125" t="s">
-        <v>204</v>
-      </c>
-      <c r="K125" t="s">
-        <v>213</v>
-      </c>
-      <c r="L125" t="s">
-        <v>463</v>
-      </c>
-      <c r="M125" t="s">
-        <v>34</v>
-      </c>
-      <c r="O125" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="Q125" t="s">
-        <v>570</v>
+        <v>481</v>
       </c>
     </row>
     <row r="126" spans="1:17">
@@ -5525,8 +5529,47 @@
       <c r="B126" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="C126" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D126" t="s">
+        <v>34</v>
+      </c>
+      <c r="E126" t="s">
+        <v>49</v>
+      </c>
+      <c r="F126" t="s">
+        <v>475</v>
+      </c>
+      <c r="G126" t="s">
+        <v>148</v>
+      </c>
+      <c r="H126" t="s">
+        <v>201</v>
+      </c>
+      <c r="I126" t="s">
+        <v>34</v>
+      </c>
+      <c r="J126" t="s">
+        <v>204</v>
+      </c>
+      <c r="K126" t="s">
+        <v>213</v>
+      </c>
+      <c r="L126" t="s">
+        <v>463</v>
+      </c>
+      <c r="M126" t="s">
+        <v>34</v>
+      </c>
+      <c r="N126" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="O126" s="10" t="s">
-        <v>542</v>
+        <v>447</v>
+      </c>
+      <c r="Q126" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="127" spans="1:17">
@@ -5534,46 +5577,10 @@
         <v>24</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D127" t="s">
-        <v>89</v>
-      </c>
-      <c r="E127" t="s">
-        <v>49</v>
-      </c>
-      <c r="F127" t="s">
-        <v>195</v>
-      </c>
-      <c r="G127" t="s">
-        <v>148</v>
-      </c>
-      <c r="H127" t="s">
-        <v>201</v>
-      </c>
-      <c r="I127" t="s">
-        <v>280</v>
-      </c>
-      <c r="J127" t="s">
-        <v>204</v>
-      </c>
-      <c r="K127" t="s">
-        <v>213</v>
-      </c>
-      <c r="L127" t="s">
-        <v>462</v>
-      </c>
-      <c r="M127" t="s">
-        <v>380</v>
-      </c>
-      <c r="O127" t="s">
-        <v>507</v>
-      </c>
-      <c r="Q127" t="s">
-        <v>539</v>
+        <v>34</v>
+      </c>
+      <c r="O127" s="10" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="128" spans="1:17">
@@ -5583,8 +5590,17 @@
       <c r="B128" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C128" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D128" t="s">
+        <v>89</v>
+      </c>
+      <c r="E128" t="s">
+        <v>49</v>
+      </c>
       <c r="F128" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G128" t="s">
         <v>148</v>
@@ -5593,15 +5609,27 @@
         <v>201</v>
       </c>
       <c r="I128" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J128" t="s">
         <v>204</v>
       </c>
       <c r="K128" t="s">
-        <v>218</v>
+        <v>213</v>
+      </c>
+      <c r="L128" t="s">
+        <v>462</v>
+      </c>
+      <c r="M128" t="s">
+        <v>380</v>
+      </c>
+      <c r="N128" s="10" t="s">
+        <v>580</v>
       </c>
       <c r="O128" t="s">
+        <v>507</v>
+      </c>
+      <c r="Q128" t="s">
         <v>539</v>
       </c>
     </row>
@@ -5613,7 +5641,7 @@
         <v>35</v>
       </c>
       <c r="F129" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G129" t="s">
         <v>148</v>
@@ -5621,40 +5649,34 @@
       <c r="H129" t="s">
         <v>201</v>
       </c>
+      <c r="I129" t="s">
+        <v>281</v>
+      </c>
+      <c r="J129" t="s">
+        <v>204</v>
+      </c>
+      <c r="K129" t="s">
+        <v>218</v>
+      </c>
+      <c r="O129" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="130" spans="1:17">
       <c r="A130" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C130" s="6">
-        <v>311</v>
-      </c>
-      <c r="D130" t="s">
-        <v>75</v>
-      </c>
-      <c r="E130" t="s">
-        <v>51</v>
-      </c>
-      <c r="I130" t="s">
-        <v>282</v>
-      </c>
-      <c r="J130" t="s">
-        <v>204</v>
-      </c>
-      <c r="K130" t="s">
-        <v>218</v>
-      </c>
-      <c r="M130" t="s">
-        <v>376</v>
-      </c>
-      <c r="O130" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="P130" t="s">
-        <v>525</v>
+        <v>35</v>
+      </c>
+      <c r="F130" t="s">
+        <v>192</v>
+      </c>
+      <c r="G130" t="s">
+        <v>148</v>
+      </c>
+      <c r="H130" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="131" spans="1:17">
@@ -5665,16 +5687,31 @@
         <v>36</v>
       </c>
       <c r="C131" s="6">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D131" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="E131" t="s">
         <v>51</v>
       </c>
-      <c r="O131" t="s">
-        <v>565</v>
+      <c r="I131" t="s">
+        <v>282</v>
+      </c>
+      <c r="J131" t="s">
+        <v>204</v>
+      </c>
+      <c r="K131" t="s">
+        <v>218</v>
+      </c>
+      <c r="M131" t="s">
+        <v>376</v>
+      </c>
+      <c r="O131" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="P131" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="132" spans="1:17">
@@ -5682,19 +5719,19 @@
         <v>24</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>305</v>
+        <v>36</v>
+      </c>
+      <c r="C132" s="6">
+        <v>312</v>
       </c>
       <c r="D132" t="s">
-        <v>304</v>
+        <v>135</v>
       </c>
       <c r="E132" t="s">
-        <v>49</v>
-      </c>
-      <c r="M132" t="s">
-        <v>375</v>
+        <v>51</v>
+      </c>
+      <c r="O132" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="133" spans="1:17">
@@ -5702,10 +5739,19 @@
         <v>24</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>377</v>
+        <v>304</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="D133" t="s">
+        <v>304</v>
+      </c>
+      <c r="E133" t="s">
+        <v>49</v>
       </c>
       <c r="M133" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="134" spans="1:17">
@@ -5713,34 +5759,10 @@
         <v>24</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C134" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="D134" t="s">
-        <v>306</v>
-      </c>
-      <c r="E134" t="s">
-        <v>49</v>
-      </c>
-      <c r="F134" t="s">
-        <v>188</v>
-      </c>
-      <c r="G134" t="s">
-        <v>148</v>
-      </c>
-      <c r="H134" t="s">
-        <v>201</v>
-      </c>
-      <c r="I134" t="s">
-        <v>353</v>
-      </c>
-      <c r="J134" t="s">
-        <v>204</v>
-      </c>
-      <c r="K134" t="s">
-        <v>218</v>
+        <v>377</v>
+      </c>
+      <c r="M134" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="135" spans="1:17">
@@ -5748,10 +5770,19 @@
         <v>24</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>345</v>
+        <v>308</v>
+      </c>
+      <c r="C135" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D135" t="s">
+        <v>306</v>
+      </c>
+      <c r="E135" t="s">
+        <v>49</v>
       </c>
       <c r="F135" t="s">
-        <v>344</v>
+        <v>188</v>
       </c>
       <c r="G135" t="s">
         <v>148</v>
@@ -5759,8 +5790,14 @@
       <c r="H135" t="s">
         <v>201</v>
       </c>
-      <c r="L135" t="s">
-        <v>330</v>
+      <c r="I135" t="s">
+        <v>353</v>
+      </c>
+      <c r="J135" t="s">
+        <v>204</v>
+      </c>
+      <c r="K135" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="136" spans="1:17">
@@ -5768,10 +5805,10 @@
         <v>24</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>455</v>
+        <v>345</v>
       </c>
       <c r="F136" t="s">
-        <v>472</v>
+        <v>344</v>
       </c>
       <c r="G136" t="s">
         <v>148</v>
@@ -5779,17 +5816,8 @@
       <c r="H136" t="s">
         <v>201</v>
       </c>
-      <c r="I136" t="s">
-        <v>488</v>
-      </c>
-      <c r="J136" t="s">
-        <v>204</v>
-      </c>
-      <c r="K136" t="s">
-        <v>218</v>
-      </c>
       <c r="L136" t="s">
-        <v>456</v>
+        <v>330</v>
       </c>
     </row>
     <row r="137" spans="1:17">
@@ -5797,13 +5825,19 @@
         <v>24</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>406</v>
+        <v>455</v>
+      </c>
+      <c r="F137" t="s">
+        <v>472</v>
+      </c>
+      <c r="G137" t="s">
+        <v>148</v>
       </c>
       <c r="H137" t="s">
         <v>201</v>
       </c>
       <c r="I137" t="s">
-        <v>283</v>
+        <v>488</v>
       </c>
       <c r="J137" t="s">
         <v>204</v>
@@ -5811,14 +5845,8 @@
       <c r="K137" t="s">
         <v>218</v>
       </c>
-      <c r="M137" t="s">
-        <v>287</v>
-      </c>
-      <c r="N137" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="O137" s="10" t="s">
-        <v>435</v>
+      <c r="L137" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="138" spans="1:17">
@@ -5828,9 +5856,26 @@
       <c r="B138" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="N138" s="10"/>
+      <c r="H138" t="s">
+        <v>201</v>
+      </c>
+      <c r="I138" t="s">
+        <v>283</v>
+      </c>
+      <c r="J138" t="s">
+        <v>204</v>
+      </c>
+      <c r="K138" t="s">
+        <v>218</v>
+      </c>
+      <c r="M138" t="s">
+        <v>287</v>
+      </c>
+      <c r="N138" s="10" t="s">
+        <v>287</v>
+      </c>
       <c r="O138" s="10" t="s">
-        <v>537</v>
+        <v>435</v>
       </c>
     </row>
     <row r="139" spans="1:17">
@@ -5838,10 +5883,11 @@
         <v>24</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="M139" t="s">
-        <v>38</v>
+        <v>406</v>
+      </c>
+      <c r="N139" s="10"/>
+      <c r="O139" s="10" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="140" spans="1:17">
@@ -5849,16 +5895,10 @@
         <v>24</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="F140" t="s">
-        <v>470</v>
-      </c>
-      <c r="G140" t="s">
-        <v>148</v>
-      </c>
-      <c r="H140" t="s">
-        <v>201</v>
+        <v>407</v>
+      </c>
+      <c r="M140" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="141" spans="1:17">
@@ -5866,10 +5906,16 @@
         <v>24</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="O141" t="s">
-        <v>533</v>
+        <v>469</v>
+      </c>
+      <c r="F141" t="s">
+        <v>470</v>
+      </c>
+      <c r="G141" t="s">
+        <v>148</v>
+      </c>
+      <c r="H141" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:17">
@@ -5877,51 +5923,21 @@
         <v>24</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="O142" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17">
+      <c r="A143" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B143" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="Q142" t="s">
+      <c r="Q143" t="s">
         <v>550</v>
-      </c>
-    </row>
-    <row r="143" spans="1:17">
-      <c r="A143" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B143" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C143" s="6">
-        <v>511</v>
-      </c>
-      <c r="D143" t="s">
-        <v>81</v>
-      </c>
-      <c r="E143" t="s">
-        <v>50</v>
-      </c>
-      <c r="F143" t="s">
-        <v>181</v>
-      </c>
-      <c r="G143" t="s">
-        <v>186</v>
-      </c>
-      <c r="H143" t="s">
-        <v>201</v>
-      </c>
-      <c r="J143" t="s">
-        <v>206</v>
-      </c>
-      <c r="K143" t="s">
-        <v>217</v>
-      </c>
-      <c r="L143" t="s">
-        <v>313</v>
-      </c>
-      <c r="P143" t="s">
-        <v>526</v>
-      </c>
-      <c r="Q143" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="144" spans="1:17">
@@ -5931,8 +5947,17 @@
       <c r="B144" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C144" s="6">
+        <v>511</v>
+      </c>
+      <c r="D144" t="s">
+        <v>81</v>
+      </c>
+      <c r="E144" t="s">
+        <v>50</v>
+      </c>
       <c r="F144" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="G144" t="s">
         <v>186</v>
@@ -5940,9 +5965,6 @@
       <c r="H144" t="s">
         <v>201</v>
       </c>
-      <c r="I144" t="s">
-        <v>284</v>
-      </c>
       <c r="J144" t="s">
         <v>206</v>
       </c>
@@ -5950,7 +5972,16 @@
         <v>217</v>
       </c>
       <c r="L144" t="s">
-        <v>451</v>
+        <v>313</v>
+      </c>
+      <c r="N144" s="10" t="s">
+        <v>578</v>
+      </c>
+      <c r="P144" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="145" spans="1:17">
@@ -5960,17 +5991,8 @@
       <c r="B145" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C145" s="6">
-        <v>513</v>
-      </c>
-      <c r="D145" t="s">
-        <v>82</v>
-      </c>
-      <c r="E145" t="s">
-        <v>50</v>
-      </c>
       <c r="F145" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="G145" t="s">
         <v>186</v>
@@ -5979,7 +6001,7 @@
         <v>201</v>
       </c>
       <c r="I145" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J145" t="s">
         <v>206</v>
@@ -5988,7 +6010,7 @@
         <v>217</v>
       </c>
       <c r="L145" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="146" spans="1:17">
@@ -5998,8 +6020,17 @@
       <c r="B146" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="C146" s="6">
+        <v>513</v>
+      </c>
+      <c r="D146" t="s">
+        <v>82</v>
+      </c>
+      <c r="E146" t="s">
+        <v>50</v>
+      </c>
       <c r="F146" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G146" t="s">
         <v>186</v>
@@ -6008,7 +6039,7 @@
         <v>201</v>
       </c>
       <c r="I146" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J146" t="s">
         <v>206</v>
@@ -6017,7 +6048,7 @@
         <v>217</v>
       </c>
       <c r="L146" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="147" spans="1:17">
@@ -6028,7 +6059,7 @@
         <v>38</v>
       </c>
       <c r="F147" t="s">
-        <v>37</v>
+        <v>176</v>
       </c>
       <c r="G147" t="s">
         <v>186</v>
@@ -6037,16 +6068,16 @@
         <v>201</v>
       </c>
       <c r="I147" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J147" t="s">
         <v>206</v>
       </c>
       <c r="K147" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="L147" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -6057,7 +6088,7 @@
         <v>38</v>
       </c>
       <c r="F148" t="s">
-        <v>182</v>
+        <v>37</v>
       </c>
       <c r="G148" t="s">
         <v>186</v>
@@ -6066,19 +6097,19 @@
         <v>201</v>
       </c>
       <c r="I148" t="s">
-        <v>38</v>
+        <v>287</v>
       </c>
       <c r="J148" t="s">
         <v>206</v>
       </c>
       <c r="K148" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="L148" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="149" spans="1:17" ht="17" customHeight="1">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17">
       <c r="A149" s="4" t="s">
         <v>37</v>
       </c>
@@ -6086,7 +6117,7 @@
         <v>38</v>
       </c>
       <c r="F149" t="s">
-        <v>357</v>
+        <v>182</v>
       </c>
       <c r="G149" t="s">
         <v>186</v>
@@ -6095,13 +6126,16 @@
         <v>201</v>
       </c>
       <c r="I149" t="s">
-        <v>288</v>
+        <v>38</v>
       </c>
       <c r="J149" t="s">
         <v>206</v>
       </c>
       <c r="K149" t="s">
         <v>217</v>
+      </c>
+      <c r="L149" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="150" spans="1:17" ht="17" customHeight="1">
@@ -6112,7 +6146,7 @@
         <v>38</v>
       </c>
       <c r="F150" t="s">
-        <v>473</v>
+        <v>357</v>
       </c>
       <c r="G150" t="s">
         <v>186</v>
@@ -6121,7 +6155,7 @@
         <v>201</v>
       </c>
       <c r="I150" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J150" t="s">
         <v>206</v>
@@ -6138,7 +6172,7 @@
         <v>38</v>
       </c>
       <c r="F151" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G151" t="s">
         <v>186</v>
@@ -6147,7 +6181,7 @@
         <v>201</v>
       </c>
       <c r="I151" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J151" t="s">
         <v>206</v>
@@ -6163,11 +6197,17 @@
       <c r="B152" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F152" t="s">
+        <v>474</v>
+      </c>
+      <c r="G152" t="s">
+        <v>186</v>
+      </c>
       <c r="H152" t="s">
         <v>201</v>
       </c>
       <c r="I152" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J152" t="s">
         <v>206</v>
@@ -6183,17 +6223,11 @@
       <c r="B153" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F153" t="s">
-        <v>180</v>
-      </c>
-      <c r="G153" t="s">
-        <v>186</v>
-      </c>
       <c r="H153" t="s">
         <v>201</v>
       </c>
       <c r="I153" t="s">
-        <v>487</v>
+        <v>291</v>
       </c>
       <c r="J153" t="s">
         <v>206</v>
@@ -6210,7 +6244,7 @@
         <v>38</v>
       </c>
       <c r="F154" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="G154" t="s">
         <v>186</v>
@@ -6219,7 +6253,7 @@
         <v>201</v>
       </c>
       <c r="I154" t="s">
-        <v>212</v>
+        <v>487</v>
       </c>
       <c r="J154" t="s">
         <v>206</v>
@@ -6235,11 +6269,17 @@
       <c r="B155" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="F155" t="s">
+        <v>184</v>
+      </c>
+      <c r="G155" t="s">
+        <v>186</v>
+      </c>
       <c r="H155" t="s">
         <v>201</v>
       </c>
       <c r="I155" t="s">
-        <v>489</v>
+        <v>212</v>
       </c>
       <c r="J155" t="s">
         <v>206</v>
@@ -6259,7 +6299,7 @@
         <v>201</v>
       </c>
       <c r="I156" t="s">
-        <v>292</v>
+        <v>489</v>
       </c>
       <c r="J156" t="s">
         <v>206</v>
@@ -6268,39 +6308,24 @@
         <v>217</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="1:17" ht="17" customHeight="1">
       <c r="A157" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F157" t="s">
-        <v>175</v>
-      </c>
-      <c r="G157" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
       <c r="H157" t="s">
         <v>201</v>
       </c>
       <c r="I157" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J157" t="s">
         <v>206</v>
       </c>
       <c r="K157" t="s">
         <v>217</v>
-      </c>
-      <c r="L157" t="s">
-        <v>458</v>
-      </c>
-      <c r="P157" t="s">
-        <v>527</v>
-      </c>
-      <c r="Q157" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="158" spans="1:17">
@@ -6311,7 +6336,7 @@
         <v>39</v>
       </c>
       <c r="F158" t="s">
-        <v>362</v>
+        <v>175</v>
       </c>
       <c r="G158" t="s">
         <v>186</v>
@@ -6320,13 +6345,25 @@
         <v>201</v>
       </c>
       <c r="I158" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J158" t="s">
         <v>206</v>
       </c>
       <c r="K158" t="s">
         <v>217</v>
+      </c>
+      <c r="L158" t="s">
+        <v>458</v>
+      </c>
+      <c r="N158" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="P158" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q158" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="159" spans="1:17">
@@ -6336,11 +6373,17 @@
       <c r="B159" s="4" t="s">
         <v>39</v>
       </c>
+      <c r="F159" t="s">
+        <v>362</v>
+      </c>
+      <c r="G159" t="s">
+        <v>186</v>
+      </c>
       <c r="H159" t="s">
         <v>201</v>
       </c>
       <c r="I159" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J159" t="s">
         <v>206</v>
@@ -6354,34 +6397,19 @@
         <v>37</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F160" t="s">
-        <v>178</v>
-      </c>
-      <c r="G160" t="s">
-        <v>186</v>
+        <v>39</v>
       </c>
       <c r="H160" t="s">
         <v>201</v>
       </c>
       <c r="I160" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J160" t="s">
         <v>206</v>
       </c>
       <c r="K160" t="s">
         <v>217</v>
-      </c>
-      <c r="L160" t="s">
-        <v>459</v>
-      </c>
-      <c r="P160" t="s">
-        <v>528</v>
-      </c>
-      <c r="Q160" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="161" spans="1:17">
@@ -6392,19 +6420,34 @@
         <v>40</v>
       </c>
       <c r="F161" t="s">
-        <v>360</v>
+        <v>178</v>
+      </c>
+      <c r="G161" t="s">
+        <v>186</v>
       </c>
       <c r="H161" t="s">
         <v>201</v>
       </c>
       <c r="I161" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J161" t="s">
         <v>206</v>
       </c>
       <c r="K161" t="s">
         <v>217</v>
+      </c>
+      <c r="L161" t="s">
+        <v>459</v>
+      </c>
+      <c r="N161" s="10" t="s">
+        <v>581</v>
+      </c>
+      <c r="P161" t="s">
+        <v>528</v>
+      </c>
+      <c r="Q161" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="162" spans="1:17">
@@ -6412,34 +6455,22 @@
         <v>37</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>530</v>
+        <v>40</v>
       </c>
       <c r="F162" t="s">
-        <v>174</v>
-      </c>
-      <c r="G162" t="s">
-        <v>186</v>
+        <v>360</v>
       </c>
       <c r="H162" t="s">
         <v>201</v>
       </c>
       <c r="I162" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J162" t="s">
         <v>206</v>
       </c>
       <c r="K162" t="s">
         <v>217</v>
-      </c>
-      <c r="L162" t="s">
-        <v>452</v>
-      </c>
-      <c r="P162" t="s">
-        <v>529</v>
-      </c>
-      <c r="Q162" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="163" spans="1:17">
@@ -6450,7 +6481,7 @@
         <v>530</v>
       </c>
       <c r="F163" t="s">
-        <v>471</v>
+        <v>174</v>
       </c>
       <c r="G163" t="s">
         <v>186</v>
@@ -6459,13 +6490,25 @@
         <v>201</v>
       </c>
       <c r="I163" t="s">
-        <v>41</v>
+        <v>298</v>
       </c>
       <c r="J163" t="s">
         <v>206</v>
       </c>
       <c r="K163" t="s">
         <v>217</v>
+      </c>
+      <c r="L163" t="s">
+        <v>452</v>
+      </c>
+      <c r="N163" s="10" t="s">
+        <v>530</v>
+      </c>
+      <c r="P163" t="s">
+        <v>529</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="164" spans="1:17">
@@ -6475,11 +6518,17 @@
       <c r="B164" s="4" t="s">
         <v>530</v>
       </c>
+      <c r="F164" t="s">
+        <v>471</v>
+      </c>
+      <c r="G164" t="s">
+        <v>186</v>
+      </c>
       <c r="H164" t="s">
         <v>201</v>
       </c>
       <c r="I164" t="s">
-        <v>211</v>
+        <v>41</v>
       </c>
       <c r="J164" t="s">
         <v>206</v>
@@ -6499,7 +6548,7 @@
         <v>201</v>
       </c>
       <c r="I165" t="s">
-        <v>299</v>
+        <v>211</v>
       </c>
       <c r="J165" t="s">
         <v>206</v>
@@ -6513,10 +6562,19 @@
         <v>37</v>
       </c>
       <c r="B166" s="4" t="s">
-        <v>555</v>
-      </c>
-      <c r="Q166" t="s">
-        <v>557</v>
+        <v>530</v>
+      </c>
+      <c r="H166" t="s">
+        <v>201</v>
+      </c>
+      <c r="I166" t="s">
+        <v>299</v>
+      </c>
+      <c r="J166" t="s">
+        <v>206</v>
+      </c>
+      <c r="K166" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="167" spans="1:17">
@@ -6524,10 +6582,10 @@
         <v>37</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="Q167" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="168" spans="1:17">
@@ -6535,56 +6593,41 @@
         <v>37</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>291</v>
+        <v>556</v>
       </c>
       <c r="Q168" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17" ht="17" customHeight="1">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17">
       <c r="A169" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C169" s="6" t="s">
-        <v>468</v>
-      </c>
-      <c r="D169" t="s">
-        <v>467</v>
-      </c>
-      <c r="E169" t="s">
-        <v>50</v>
-      </c>
-      <c r="F169" t="s">
-        <v>185</v>
-      </c>
-      <c r="G169" t="s">
-        <v>186</v>
-      </c>
-      <c r="H169" t="s">
-        <v>201</v>
-      </c>
-      <c r="I169" t="s">
-        <v>300</v>
-      </c>
-      <c r="J169" t="s">
-        <v>206</v>
-      </c>
-      <c r="K169" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="170" spans="1:17">
+        <v>291</v>
+      </c>
+      <c r="Q169" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17" ht="17" customHeight="1">
       <c r="A170" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>42</v>
       </c>
+      <c r="C170" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="D170" t="s">
+        <v>467</v>
+      </c>
+      <c r="E170" t="s">
+        <v>50</v>
+      </c>
       <c r="F170" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G170" t="s">
         <v>186</v>
@@ -6592,28 +6635,31 @@
       <c r="H170" t="s">
         <v>201</v>
       </c>
+      <c r="I170" t="s">
+        <v>300</v>
+      </c>
+      <c r="J170" t="s">
+        <v>206</v>
+      </c>
+      <c r="K170" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="171" spans="1:17">
-      <c r="A171" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B171" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E171" t="s">
-        <v>52</v>
+      <c r="A171" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F171" t="s">
+        <v>183</v>
+      </c>
+      <c r="G171" t="s">
+        <v>186</v>
       </c>
       <c r="H171" t="s">
-        <v>200</v>
-      </c>
-      <c r="I171" t="s">
-        <v>301</v>
-      </c>
-      <c r="J171" t="s">
-        <v>209</v>
-      </c>
-      <c r="K171" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
     </row>
     <row r="172" spans="1:17">
@@ -6621,13 +6667,16 @@
         <v>43</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="E172" t="s">
+        <v>52</v>
       </c>
       <c r="H172" t="s">
         <v>200</v>
       </c>
       <c r="I172" t="s">
-        <v>208</v>
+        <v>301</v>
       </c>
       <c r="J172" t="s">
         <v>209</v>
@@ -6643,26 +6692,11 @@
       <c r="B173" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C173" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="D173" t="s">
-        <v>45</v>
-      </c>
-      <c r="E173" t="s">
-        <v>52</v>
-      </c>
-      <c r="F173" t="s">
-        <v>161</v>
-      </c>
-      <c r="G173" t="s">
-        <v>173</v>
-      </c>
       <c r="H173" t="s">
         <v>200</v>
       </c>
       <c r="I173" t="s">
-        <v>45</v>
+        <v>208</v>
       </c>
       <c r="J173" t="s">
         <v>209</v>
@@ -6676,22 +6710,28 @@
         <v>43</v>
       </c>
       <c r="B174" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D174" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
       <c r="E174" t="s">
         <v>52</v>
       </c>
+      <c r="F174" t="s">
+        <v>161</v>
+      </c>
+      <c r="G174" t="s">
+        <v>173</v>
+      </c>
       <c r="H174" t="s">
         <v>200</v>
       </c>
       <c r="I174" t="s">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="J174" t="s">
         <v>209</v>
@@ -6705,13 +6745,13 @@
         <v>43</v>
       </c>
       <c r="B175" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D175" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E175" t="s">
         <v>52</v>
@@ -6720,12 +6760,41 @@
         <v>200</v>
       </c>
       <c r="I175" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J175" t="s">
         <v>209</v>
       </c>
       <c r="K175" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="176" spans="1:17">
+      <c r="A176" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B176" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D176" t="s">
+        <v>47</v>
+      </c>
+      <c r="E176" t="s">
+        <v>52</v>
+      </c>
+      <c r="H176" t="s">
+        <v>200</v>
+      </c>
+      <c r="I176" t="s">
+        <v>303</v>
+      </c>
+      <c r="J176" t="s">
+        <v>209</v>
+      </c>
+      <c r="K176" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>